<commit_message>
selection set checkpoint 1
</commit_message>
<xml_diff>
--- a/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
+++ b/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\omer\myGitHub\Front-End-Compiler-Project\Mio Language Design\Syntax Analyze Phase\FirstFollowSelectionSet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects_collab\Front-End-Compiler-Project\Mio Language Design\Syntax Analyze Phase\FirstFollowSelectionSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D4BEA0-7510-4249-B527-841863745A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="487">
   <si>
     <t>&lt;Start&gt;</t>
   </si>
@@ -634,9 +633,6 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;J&gt; </t>
-  </si>
-  <si>
-    <t>mdm ? null</t>
   </si>
   <si>
     <t>power ? null</t>
@@ -1039,14 +1035,6 @@
     <t>dt ? Id</t>
   </si>
   <si>
-    <t>Begin?  def ?  Class ? Abstract ? const ?
-dt ? Id ?null</t>
-  </si>
-  <si>
-    <t>def ?  Class ? Abstract ? const  ?
-dt ? Id ? Null</t>
-  </si>
-  <si>
     <t>if ? Shift ? const ? dt ? id ? Parent ? Self ?  Test ?  Loop ? do ? stop ? Ret ? Cont ? raise</t>
   </si>
   <si>
@@ -1123,9 +1111,6 @@
     <t>&lt;IMPORTS&gt; ? &lt;ST_BODY&gt;</t>
   </si>
   <si>
-    <t>import ? Begin?  def ?  Class ? Abstract ? const ? dt ? Id ? null</t>
-  </si>
-  <si>
     <t>&lt;ST_BODY&gt;</t>
   </si>
   <si>
@@ -1454,12 +1439,121 @@
   </si>
   <si>
     <t>SELECTION SET</t>
+  </si>
+  <si>
+    <t>import?Begin?def ?Class?Abstract?const?dt?Id?null</t>
+  </si>
+  <si>
+    <t>Begin?def?Class?Abstract?const?
+dt?Id?null</t>
+  </si>
+  <si>
+    <t>import?Begin? def? Class? Abstract?const?dt?Id ?~</t>
+  </si>
+  <si>
+    <t>Begin?def?Class?Abstract?const?
+dt?Id?~</t>
+  </si>
+  <si>
+    <t>def?Class?Abstract?const ?
+dt?id? Null</t>
+  </si>
+  <si>
+    <t>def?Class?Abstract?const ?
+dt?id?~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if ? Shift ? const ? dt ? id ? Parent ? Self ?  Test ?  Loop ? do ? stop ? Ret ? Cont ? Raise ?state ? default ? } </t>
+  </si>
+  <si>
+    <t>[?id ?protected?private</t>
+  </si>
+  <si>
+    <t>protected?private?id</t>
+  </si>
+  <si>
+    <t>[ ? Id ?(</t>
+  </si>
+  <si>
+    <t>[ ? private ? Protected ? id ?(</t>
+  </si>
+  <si>
+    <t>protected ?id</t>
+  </si>
+  <si>
+    <t>&lt;?(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dot ? [ ? ( ? power ?  Mdm ?  Pm ? Rop ? 
+And ? Or ? ]  ? ) ? , ? }  ?  :  ? ; </t>
+  </si>
+  <si>
+    <t>[ ? dot ? = ? Cma ? inc_dec ? new? NaN ? power 
+?  Mdm ?  Pm ? Rop ? And ? Or ? 
+, ? ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inc_dec ? dot  ? [ ? ( ?power ?  Mdm ?  Pm ? Rop 
+? And ? Or ?  ]  ? ) ? , ? }  ?  :  ? ; </t>
+  </si>
+  <si>
+    <t>parent ? Self ?id</t>
+  </si>
+  <si>
+    <t>dot ? power ?  Mdm ?  Pm ? Rop ? And ? 
+Or ?  [ ? (?, ? ;</t>
+  </si>
+  <si>
+    <t>dot ? = ? Cma ? inc_dec ? new? NaN ? power 
+?  Mdm ?  Pm ? Rop ? And ? Or ? , ? ;</t>
+  </si>
+  <si>
+    <t>dot ? power ?  Mdm ?  Pm ? Rop ? And ? 
+Or ?, ? ;</t>
+  </si>
+  <si>
+    <t>power ?  Mdm ?  Pm ? Rop ? And ? Or ?, ? ;</t>
+  </si>
+  <si>
+    <t>dot ? [ ? ( ?'= ? ; ? state ? default ? } else ? Till ? def ? 
+ Static ? const ? dt ? id  ? }? Begin?  Class ? Abstract ?  ~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or ?]  ? ) ? , ? }  ? Or ? :  ? ; </t>
+  </si>
+  <si>
+    <t>and ?or ? ]  ? ) ? , ? }  ? :  ? ;</t>
+  </si>
+  <si>
+    <t>mdm ?pm ? rop ? and ? or ? ]  ? ) ? , ? }  
+? :  ? ;</t>
+  </si>
+  <si>
+    <t>power ? mdm ? pm ? rop ? and ? or ? ]  ? ) ? , ? }  ? :  ? ;</t>
+  </si>
+  <si>
+    <t> pm ? rop ? and ? or ? ]  ? ) ? , ? }  ? :  ? ;</t>
+  </si>
+  <si>
+    <t>mdm ? Null</t>
+  </si>
+  <si>
+    <t>else ? state ? default ? } else ? Till</t>
+  </si>
+  <si>
+    <t> dot ? [ ? ( ?)</t>
+  </si>
+  <si>
+    <t>except ? finally ?state ? default ? } else ? Till</t>
+  </si>
+  <si>
+    <t>raises ?{ ? ;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1517,7 +1611,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1548,6 +1642,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -1610,15 +1710,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1676,13 +1777,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
@@ -1695,9 +1790,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1708,8 +1800,36 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="6" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="6" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="6" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="6" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="40% - Accent1" xfId="6" builtinId="31"/>
     <cellStyle name="40% - Accent3" xfId="3" builtinId="39"/>
     <cellStyle name="Accent3" xfId="2" builtinId="37"/>
     <cellStyle name="Good" xfId="5" builtinId="26"/>
@@ -1992,23 +2112,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="3" max="3" width="47.42578125" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="38.85546875" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" customWidth="1"/>
+    <col min="8" max="8" width="57.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
@@ -2019,19 +2139,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
@@ -2046,13 +2166,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
-        <v>452</v>
+      <c r="E3" s="24" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2060,33 +2180,39 @@
         <v>4</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>355</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>455</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>272</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>331</v>
+        <v>271</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>456</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>452</v>
+        <v>448</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2094,16 +2220,19 @@
         <v>7</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>319</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>332</v>
+        <v>318</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>459</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>452</v>
+        <v>448</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -2130,17 +2259,20 @@
       <c r="C10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>439</v>
+      <c r="D10" s="37" t="s">
+        <v>331</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>435</v>
       </c>
       <c r="F10" t="s">
-        <v>440</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>441</v>
+        <v>436</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>437</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -2156,18 +2288,21 @@
         <v>10</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="E13" t="s">
-        <v>438</v>
-      </c>
-      <c r="F13" t="s">
-        <v>441</v>
+        <v>272</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>330</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>434</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>437</v>
       </c>
       <c r="G13" s="8"/>
+      <c r="H13" s="8" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -2176,14 +2311,17 @@
       <c r="C14" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>335</v>
+      <c r="D14" s="37" t="s">
+        <v>332</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>365</v>
+        <v>361</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -2198,446 +2336,542 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="35" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="35" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="35" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>322</v>
+      <c r="C22" s="35" t="s">
+        <v>321</v>
       </c>
       <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H22" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>320</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>321</v>
-      </c>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="13" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>296</v>
+      <c r="C26" s="35" t="s">
+        <v>295</v>
       </c>
       <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H26" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>276</v>
+      <c r="C27" s="35" t="s">
+        <v>275</v>
       </c>
       <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H27" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="35" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="17" t="s">
-        <v>369</v>
-      </c>
-      <c r="F28" s="25" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+      <c r="F28" s="43" t="s">
+        <v>367</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>274</v>
+      <c r="C29" s="35" t="s">
+        <v>273</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="18" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>275</v>
+      <c r="C30" s="35" t="s">
+        <v>274</v>
       </c>
       <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H30" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="13" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="35" t="s">
         <v>31</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="17" t="s">
-        <v>414</v>
-      </c>
-      <c r="F33" s="31" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>370</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="13" t="s">
         <v>32</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="35" t="s">
         <v>38</v>
       </c>
       <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="35" t="s">
         <v>39</v>
       </c>
       <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D40" s="35" t="s">
+        <v>334</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="35" t="s">
         <v>44</v>
       </c>
       <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D42" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D44" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C45" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="D45" s="35" t="s">
         <v>279</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="E45" s="17" t="s">
         <v>40</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G45" s="24" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="13" t="s">
         <v>45</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="35" t="s">
         <v>38</v>
       </c>
       <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C49" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="D49" s="35" t="s">
         <v>287</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="H49" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
-        <v>289</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D50" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C51" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="C51" s="15" t="s">
-        <v>291</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D51" s="35" t="s">
+        <v>327</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D52" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>283</v>
+      <c r="D53" s="35" t="s">
+        <v>282</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G53" s="24" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="35" t="s">
         <v>52</v>
       </c>
       <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H54" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="13" t="s">
         <v>53</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D57" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D58" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D58" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="H58" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>271</v>
+      <c r="C59" s="35" t="s">
+        <v>270</v>
       </c>
       <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H59" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="35" t="s">
         <v>63</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="24" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="35" t="s">
         <v>64</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="24" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H61" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="35" t="s">
         <v>65</v>
       </c>
       <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H62" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="35" t="s">
         <v>44</v>
       </c>
       <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H63" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -2656,8 +2890,11 @@
       <c r="C66" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>294</v>
+      <c r="D66" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
@@ -2667,13 +2904,16 @@
       <c r="C67" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>295</v>
+      <c r="D67" s="35" t="s">
+        <v>294</v>
       </c>
       <c r="E67" s="17" t="s">
-        <v>443</v>
-      </c>
-      <c r="F67" t="s">
+        <v>439</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="H67" s="2" t="s">
         <v>294</v>
       </c>
     </row>
@@ -2696,68 +2936,80 @@
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>338</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>375</v>
+        <v>335</v>
+      </c>
+      <c r="D71" s="35" t="s">
+        <v>371</v>
       </c>
       <c r="E71" s="17" t="s">
-        <v>376</v>
-      </c>
-      <c r="F71" s="26" t="s">
-        <v>377</v>
-      </c>
-      <c r="G71" s="30" t="s">
-        <v>413</v>
+        <v>372</v>
+      </c>
+      <c r="F71" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="G71" s="28" t="s">
+        <v>409</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>468</v>
       </c>
       <c r="I71" s="8"/>
     </row>
-    <row r="72" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="35" t="s">
         <v>29</v>
       </c>
       <c r="D72" s="2"/>
-      <c r="E72" s="26" t="s">
+      <c r="E72" s="25" t="s">
+        <v>412</v>
+      </c>
+      <c r="F72" s="30" t="s">
         <v>416</v>
       </c>
-      <c r="F72" s="33" t="s">
-        <v>420</v>
-      </c>
-      <c r="G72" s="32" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="73" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="G72" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C73" s="35" t="s">
         <v>285</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="17" t="s">
-        <v>415</v>
-      </c>
-      <c r="F73" s="34" t="s">
-        <v>421</v>
+        <v>411</v>
+      </c>
+      <c r="F73" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="35" t="s">
         <v>39</v>
       </c>
       <c r="D74" s="2"/>
+      <c r="H74" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="75" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
@@ -2766,18 +3018,24 @@
       <c r="C75" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D75" s="8" t="s">
-        <v>304</v>
+      <c r="D75" s="37" t="s">
+        <v>303</v>
+      </c>
+      <c r="H75" s="8" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="38" t="s">
         <v>44</v>
       </c>
       <c r="D76" s="2"/>
+      <c r="H76" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="77" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
@@ -2786,22 +3044,25 @@
       <c r="C77" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>305</v>
+      <c r="D77" s="36" t="s">
+        <v>304</v>
       </c>
       <c r="E77" s="17" t="s">
-        <v>387</v>
-      </c>
-      <c r="F77" t="s">
+        <v>383</v>
+      </c>
+      <c r="F77" s="24" t="s">
         <v>44</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>339</v>
+      <c r="C78" s="35" t="s">
+        <v>336</v>
       </c>
       <c r="D78" s="2"/>
     </row>
@@ -2810,1455 +3071,1751 @@
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B80" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>349</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
+      </c>
+      <c r="D81" s="39" t="s">
+        <v>347</v>
       </c>
       <c r="E81" s="17" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>427</v>
-      </c>
-      <c r="G81" s="30" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+      <c r="G81" s="28" t="s">
+        <v>408</v>
+      </c>
+      <c r="H81" s="34" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D82" s="4" t="s">
-        <v>352</v>
+      <c r="D82" s="39" t="s">
+        <v>349</v>
       </c>
       <c r="E82" s="17" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>351</v>
+      <c r="C83" s="35" t="s">
+        <v>348</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="17" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F83" s="15" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="13" t="s">
         <v>85</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" s="11" t="s">
         <v>87</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C87" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>306</v>
+      <c r="D87" s="35" t="s">
+        <v>305</v>
       </c>
       <c r="E87" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F87" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F87" s="24" t="s">
+        <v>437</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="D88" s="35" t="s">
+        <v>345</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C89" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D89" s="36" t="s">
+        <v>337</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C90" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>307</v>
+      <c r="D90" s="35" t="s">
+        <v>306</v>
       </c>
       <c r="E90" s="17" t="s">
+        <v>433</v>
+      </c>
+      <c r="F90" s="24" t="s">
         <v>437</v>
       </c>
-      <c r="F90" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H90" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C91" s="39" t="s">
         <v>106</v>
       </c>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C92" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D92" s="8" t="s">
-        <v>341</v>
+      <c r="D92" s="37" t="s">
+        <v>338</v>
       </c>
       <c r="E92" s="17" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F92" s="24" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H92" s="8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C93" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>299</v>
+      <c r="D93" s="35" t="s">
+        <v>298</v>
       </c>
       <c r="E93" s="24" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="94" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C94" s="16" t="s">
-        <v>327</v>
-      </c>
-      <c r="D94" s="20" t="s">
-        <v>342</v>
+        <v>326</v>
+      </c>
+      <c r="D94" s="40" t="s">
+        <v>339</v>
       </c>
       <c r="E94" t="s">
-        <v>381</v>
-      </c>
-      <c r="F94" t="s">
+        <v>377</v>
+      </c>
+      <c r="F94" s="24" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="95" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H94" s="20" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C95" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>326</v>
+      <c r="D95" s="36" t="s">
+        <v>325</v>
       </c>
       <c r="E95" s="17" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F95" s="17" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="G95" s="24" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="96" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H95" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C96" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>343</v>
+      <c r="D96" s="36" t="s">
+        <v>340</v>
       </c>
       <c r="E96" s="17" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F96" s="17" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="G96" s="24" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="97" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H96" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C97" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="D97" s="36" t="s">
         <v>324</v>
       </c>
-      <c r="D97" s="1" t="s">
-        <v>325</v>
-      </c>
       <c r="E97" s="17" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="G97" s="24" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="98" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H97" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C98" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>323</v>
+      <c r="D98" s="35" t="s">
+        <v>322</v>
       </c>
       <c r="E98" s="18" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="G98" s="24" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H98" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="35" t="s">
         <v>112</v>
       </c>
       <c r="D99" s="2"/>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H99" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="C100" s="39" t="s">
         <v>113</v>
       </c>
       <c r="D100" s="2"/>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H100" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" s="13" t="s">
         <v>114</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" s="11" t="s">
         <v>115</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
         <v>116</v>
       </c>
       <c r="C104" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D104" s="35" t="s">
+        <v>341</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C105" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D105" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D105" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="35" t="s">
         <v>122</v>
       </c>
       <c r="D106" s="2"/>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H106" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C107" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D107" s="4" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D107" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="H107" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" s="13" t="s">
         <v>124</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="C110" s="35" t="s">
         <v>127</v>
       </c>
       <c r="D110" s="2"/>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H110" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C111" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D111" s="35" t="s">
+        <v>311</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" s="13" t="s">
         <v>129</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C114" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="D114" s="35" t="s">
         <v>29</v>
       </c>
       <c r="E114" t="s">
-        <v>435</v>
-      </c>
-      <c r="F114" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="115" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+      <c r="F114" s="24" t="s">
+        <v>437</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="115" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
         <v>131</v>
       </c>
       <c r="C115" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="D115" s="35" t="s">
         <v>29</v>
       </c>
       <c r="E115" t="s">
-        <v>436</v>
-      </c>
-      <c r="F115" s="8" t="s">
-        <v>453</v>
+        <v>432</v>
+      </c>
+      <c r="F115" s="28" t="s">
+        <v>449</v>
       </c>
       <c r="G115" s="8"/>
-    </row>
-    <row r="116" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H115" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="35" t="s">
         <v>145</v>
       </c>
       <c r="D116" s="2"/>
       <c r="E116" t="s">
-        <v>434</v>
-      </c>
-      <c r="F116" s="8" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="117" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+      <c r="F116" s="28" t="s">
+        <v>450</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="117" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C117" s="4" t="s">
+      <c r="C117" s="39" t="s">
         <v>146</v>
       </c>
       <c r="D117" s="2"/>
       <c r="E117" t="s">
-        <v>433</v>
-      </c>
-      <c r="F117" s="8" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="118" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+      <c r="F117" s="28" t="s">
+        <v>450</v>
+      </c>
+      <c r="H117" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="118" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
         <v>134</v>
       </c>
       <c r="C118" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>318</v>
+      <c r="D118" s="36" t="s">
+        <v>317</v>
       </c>
       <c r="E118" t="s">
-        <v>432</v>
-      </c>
-      <c r="F118" s="8" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="F118" s="28" t="s">
+        <v>450</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C119" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C119" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="H119" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>136</v>
       </c>
       <c r="C120" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D120" s="8" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="121" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="D120" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="H120" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="121" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>137</v>
       </c>
       <c r="C121" s="17" t="s">
-        <v>422</v>
-      </c>
-      <c r="D121" t="s">
-        <v>375</v>
+        <v>418</v>
+      </c>
+      <c r="D121" s="38" t="s">
+        <v>371</v>
       </c>
       <c r="E121" s="17" t="s">
-        <v>428</v>
-      </c>
-      <c r="F121" s="35" t="s">
-        <v>445</v>
-      </c>
-      <c r="G121" s="36" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="122" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+      <c r="F121" s="32" t="s">
+        <v>441</v>
+      </c>
+      <c r="G121" s="33" t="s">
+        <v>451</v>
+      </c>
+      <c r="H121" s="8" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="122" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>138</v>
       </c>
-      <c r="C122" t="s">
-        <v>339</v>
+      <c r="C122" s="38" t="s">
+        <v>336</v>
       </c>
       <c r="E122" s="17" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="F122" s="17" t="s">
-        <v>431</v>
-      </c>
-      <c r="G122" s="20" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="123" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+      <c r="G122" s="33" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="123" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>139</v>
       </c>
       <c r="C123" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="D123" t="s">
-        <v>423</v>
+      <c r="D123" s="38" t="s">
+        <v>419</v>
       </c>
       <c r="E123" s="17" t="s">
-        <v>430</v>
-      </c>
-      <c r="F123" s="20" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+      <c r="F123" s="33" t="s">
+        <v>452</v>
+      </c>
+      <c r="H123" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>140</v>
       </c>
-      <c r="C124" s="5" t="s">
+      <c r="C124" s="41" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="125" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H124" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="125" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>141</v>
       </c>
       <c r="C125" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="D125" s="8" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D125" s="37" t="s">
+        <v>314</v>
+      </c>
+      <c r="G125" s="24"/>
+      <c r="H125" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>157</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="38" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="128" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H127" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="128" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>158</v>
       </c>
       <c r="C128" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="D128" s="8" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D128" s="37" t="s">
+        <v>314</v>
+      </c>
+      <c r="H128" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>159</v>
       </c>
       <c r="C129" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="D129" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D129" s="38" t="s">
+        <v>315</v>
+      </c>
+      <c r="H129" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>155</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" s="38" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="131" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H130" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="131" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>160</v>
       </c>
       <c r="C131" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="D131" s="8" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D131" s="37" t="s">
+        <v>314</v>
+      </c>
+      <c r="H131" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>156</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C132" s="38" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H132" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>142</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" s="38" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="136" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H135" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>143</v>
       </c>
       <c r="C136" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D136" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D136" s="36" t="s">
+        <v>313</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>144</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" s="38" t="s">
         <v>154</v>
       </c>
       <c r="G137" s="1"/>
-    </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H137" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B138" s="6"/>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B139" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="140" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>165</v>
       </c>
       <c r="C140" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="D140" s="38" t="s">
         <v>329</v>
       </c>
-      <c r="D140" t="s">
-        <v>330</v>
-      </c>
-      <c r="E140" s="26" t="s">
-        <v>444</v>
-      </c>
-      <c r="F140" s="8" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="141" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E140" s="25" t="s">
+        <v>440</v>
+      </c>
+      <c r="F140" s="28" t="s">
+        <v>453</v>
+      </c>
+      <c r="G140" s="24"/>
+      <c r="H140" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="141" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
+        <v>328</v>
+      </c>
+      <c r="C141" s="38" t="s">
         <v>329</v>
-      </c>
-      <c r="C141" t="s">
-        <v>330</v>
       </c>
       <c r="E141" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="F141" s="8" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F141" s="28" t="s">
+        <v>453</v>
+      </c>
+      <c r="H141" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>166</v>
       </c>
       <c r="C142" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="D142" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="143" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D142" s="38" t="s">
+        <v>295</v>
+      </c>
+      <c r="H142" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="143" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>167</v>
       </c>
       <c r="C143" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="D143" s="2" t="s">
-        <v>313</v>
+      <c r="D143" s="35" t="s">
+        <v>312</v>
       </c>
       <c r="E143" s="17" t="s">
-        <v>329</v>
-      </c>
-      <c r="F143" s="8" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+      <c r="F143" s="28" t="s">
+        <v>453</v>
+      </c>
+      <c r="H143" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>168</v>
       </c>
-      <c r="C144" s="5" t="s">
-        <v>311</v>
+      <c r="C144" s="41" t="s">
+        <v>310</v>
       </c>
       <c r="D144" s="5"/>
-    </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H144" s="5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>169</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="38" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H145" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B147" s="10" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>174</v>
       </c>
       <c r="C148" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="D148" s="19" t="s">
-        <v>298</v>
+        <v>292</v>
+      </c>
+      <c r="D148" s="38" t="s">
+        <v>297</v>
       </c>
       <c r="E148" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F148" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F148" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="H148" s="19" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>175</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C149" s="38" t="s">
         <v>180</v>
       </c>
       <c r="E149" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="F149" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F149" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="H149" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>176</v>
       </c>
-      <c r="C150" s="17" t="s">
+      <c r="C150" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="D150" t="s">
-        <v>277</v>
+      <c r="D150" s="38" t="s">
+        <v>276</v>
       </c>
       <c r="E150" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="F150" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F150" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="H150" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>177</v>
       </c>
       <c r="C151" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="D151" t="s">
-        <v>310</v>
+      <c r="D151" s="38" t="s">
+        <v>309</v>
       </c>
       <c r="E151" s="17" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="F151" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="G151" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G151" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="H151" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>178</v>
       </c>
-      <c r="C152" s="5" t="s">
+      <c r="C152" s="41" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H152" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>179</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C153" s="38" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H153" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B155" s="10" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="156" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>184</v>
       </c>
       <c r="C156" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="D156" s="1" t="s">
-        <v>303</v>
+      <c r="D156" s="36" t="s">
+        <v>302</v>
       </c>
       <c r="E156" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="F156" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+      <c r="F156" s="28" t="s">
+        <v>401</v>
+      </c>
+      <c r="H156" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>185</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C157" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E157" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="F157" s="30" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="158" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+      <c r="F157" s="28" t="s">
+        <v>401</v>
+      </c>
+      <c r="H157" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="158" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>186</v>
       </c>
       <c r="C158" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="D158" s="1" t="s">
-        <v>303</v>
+      <c r="D158" s="36" t="s">
+        <v>302</v>
       </c>
       <c r="E158" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="F158" s="8" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+      <c r="F158" s="28" t="s">
+        <v>402</v>
+      </c>
+      <c r="H158" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>187</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="38" t="s">
         <v>198</v>
       </c>
       <c r="E159" s="23" t="s">
-        <v>389</v>
-      </c>
-      <c r="F159" s="26" t="s">
-        <v>394</v>
+        <v>385</v>
+      </c>
+      <c r="F159" s="25" t="s">
+        <v>390</v>
       </c>
       <c r="G159" s="24" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="160" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+      <c r="H159" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="160" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>188</v>
       </c>
       <c r="C160" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="D160" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="E160" s="28" t="s">
-        <v>399</v>
-      </c>
-      <c r="F160" s="27" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D160" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="E160" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="F160" s="44" t="s">
+        <v>403</v>
+      </c>
+      <c r="H160" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>189</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="38" t="s">
         <v>199</v>
       </c>
       <c r="E161" s="23" t="s">
-        <v>390</v>
-      </c>
-      <c r="F161" s="26" t="s">
-        <v>395</v>
+        <v>386</v>
+      </c>
+      <c r="F161" s="25" t="s">
+        <v>391</v>
       </c>
       <c r="G161" s="24" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="162" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+      <c r="H161" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="162" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>190</v>
       </c>
       <c r="C162" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="D162" s="1" t="s">
-        <v>303</v>
+      <c r="D162" s="36" t="s">
+        <v>302</v>
       </c>
       <c r="E162" s="17" t="s">
-        <v>401</v>
-      </c>
-      <c r="F162" s="27" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="163" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+      <c r="F162" s="44" t="s">
+        <v>404</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="163" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>191</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C163" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="E163" s="26" t="s">
-        <v>391</v>
-      </c>
-      <c r="F163" s="26" t="s">
-        <v>396</v>
+      <c r="E163" s="25" t="s">
+        <v>387</v>
+      </c>
+      <c r="F163" s="25" t="s">
+        <v>392</v>
       </c>
       <c r="G163" s="24" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="164" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+      <c r="H163" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="164" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>192</v>
       </c>
       <c r="C164" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="D164" s="1" t="s">
-        <v>303</v>
+      <c r="D164" s="36" t="s">
+        <v>302</v>
       </c>
       <c r="E164" s="17" t="s">
-        <v>402</v>
-      </c>
-      <c r="F164" s="27" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="165" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+      <c r="F164" s="44" t="s">
+        <v>405</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="165" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>193</v>
       </c>
-      <c r="C165" t="s">
-        <v>202</v>
-      </c>
-      <c r="E165" s="26" t="s">
-        <v>392</v>
-      </c>
-      <c r="F165" s="26" t="s">
-        <v>397</v>
-      </c>
-      <c r="G165" s="30" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="166" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C165" s="38" t="s">
+        <v>482</v>
+      </c>
+      <c r="E165" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="F165" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="G165" s="28" t="s">
+        <v>446</v>
+      </c>
+      <c r="H165" s="8" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="166" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>194</v>
       </c>
       <c r="C166" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="D166" s="1" t="s">
-        <v>303</v>
+      <c r="D166" s="36" t="s">
+        <v>302</v>
       </c>
       <c r="E166" s="17" t="s">
-        <v>404</v>
-      </c>
-      <c r="F166" s="27" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="167" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+      <c r="F166" s="44" t="s">
+        <v>406</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="167" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>111</v>
       </c>
-      <c r="C167" t="s">
-        <v>203</v>
-      </c>
-      <c r="E167" s="26" t="s">
-        <v>393</v>
-      </c>
-      <c r="F167" s="26" t="s">
-        <v>398</v>
-      </c>
-      <c r="G167" s="30" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="168" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C167" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="E167" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="F167" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="G167" s="28" t="s">
+        <v>447</v>
+      </c>
+      <c r="H167" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="168" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>195</v>
       </c>
       <c r="C168" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="D168" s="1" t="s">
-        <v>303</v>
+      <c r="D168" s="36" t="s">
+        <v>302</v>
       </c>
       <c r="E168" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="F168" s="27" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="169" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+      <c r="F168" s="44" t="s">
+        <v>407</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="169" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>196</v>
       </c>
       <c r="C169" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="D169" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="E169" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="F169" s="28" t="s">
+        <v>407</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B171" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="D169" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="E169" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="F169" s="8" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B171" s="10" t="s">
+    </row>
+    <row r="172" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B172" s="9" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="172" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B172" s="9" t="s">
+      <c r="C172" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="D172" s="36" t="s">
+        <v>301</v>
+      </c>
+      <c r="E172" s="17" t="s">
+        <v>380</v>
+      </c>
+      <c r="F172" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="G172" s="28" t="s">
+        <v>408</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="173" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
         <v>206</v>
       </c>
-      <c r="C172" s="18" t="s">
+      <c r="C173" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="D172" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="E172" s="17" t="s">
-        <v>384</v>
-      </c>
-      <c r="F172" s="18" t="s">
-        <v>385</v>
-      </c>
-      <c r="G172" s="8" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B173" t="s">
+      <c r="H173" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="174" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
         <v>207</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C174" s="38" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B174" t="s">
-        <v>208</v>
-      </c>
-      <c r="C174" t="s">
+      <c r="H174" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B176" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="177" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B177" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B176" s="10" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="177" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B177" s="2" t="s">
+      <c r="C177" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C177" s="8" t="s">
+      <c r="H177" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B178" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C178" s="40" t="s">
+        <v>344</v>
+      </c>
+      <c r="H178" s="20" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B180" s="10" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B178" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C178" s="20" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B180" s="10" t="s">
+    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B181" s="12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B182" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B181" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
-        <v>215</v>
-      </c>
-      <c r="C182" t="s">
-        <v>217</v>
+      <c r="C182" s="38" t="s">
+        <v>216</v>
       </c>
       <c r="E182" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F182" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F182" s="24" t="s">
+        <v>437</v>
+      </c>
+      <c r="H182" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>216</v>
-      </c>
-      <c r="C183" t="s">
-        <v>218</v>
+        <v>215</v>
+      </c>
+      <c r="C183" s="38" t="s">
+        <v>217</v>
       </c>
       <c r="E183" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F183" s="24" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+      <c r="H183" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="185" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B185" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="186" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B186" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B186" t="s">
+      <c r="C186" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="H186" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="187" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B187" t="s">
         <v>221</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C187" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D187" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="H187" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="188" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B188" t="s">
+        <v>222</v>
+      </c>
+      <c r="C188" s="38" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B187" t="s">
-        <v>222</v>
-      </c>
-      <c r="C187" s="17" t="s">
+      <c r="H188" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="189" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
+        <v>354</v>
+      </c>
+      <c r="C189" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D189" s="37" t="s">
+        <v>363</v>
+      </c>
+      <c r="H189" s="8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="191" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B191" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="D187" t="s">
+    </row>
+    <row r="193" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B193" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="194" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
+        <v>229</v>
+      </c>
+      <c r="C194" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="H194" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="195" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>230</v>
+      </c>
+      <c r="C195" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="D195" s="38" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B188" t="s">
-        <v>223</v>
-      </c>
-      <c r="C188" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="189" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B189" t="s">
-        <v>358</v>
-      </c>
-      <c r="C189" s="17" t="s">
-        <v>366</v>
-      </c>
-      <c r="D189" s="8" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B191" s="10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B193" s="12" t="s">
+      <c r="H195" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="197" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B197" s="12" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B194" t="s">
-        <v>230</v>
-      </c>
-      <c r="C194" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B195" t="s">
-        <v>231</v>
-      </c>
-      <c r="C195" s="17" t="s">
+    <row r="198" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
         <v>233</v>
       </c>
-      <c r="D195" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B197" s="12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B198" t="s">
+      <c r="C198" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="H198" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="199" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
         <v>234</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C199" s="38" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
-        <v>235</v>
-      </c>
-      <c r="C199" t="s">
+      <c r="H199" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="201" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B201" s="12" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B201" s="12" t="s">
+    <row r="202" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B202" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B202" t="s">
+      <c r="C202" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="H202" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="203" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
         <v>239</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C203" s="38" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="203" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B203" t="s">
+      <c r="E203" s="24" t="s">
+        <v>443</v>
+      </c>
+      <c r="H203" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="204" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
         <v>240</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C204" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="D204" s="38" t="s">
+        <v>415</v>
+      </c>
+      <c r="E204" s="17" t="s">
+        <v>442</v>
+      </c>
+      <c r="F204" s="24" t="s">
+        <v>443</v>
+      </c>
+      <c r="H204" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="205" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
+        <v>241</v>
+      </c>
+      <c r="C205" s="38" t="s">
+        <v>414</v>
+      </c>
+      <c r="E205" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="F205" s="24" t="s">
+        <v>443</v>
+      </c>
+      <c r="H205" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="207" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B207" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="E203" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="204" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B204" t="s">
-        <v>241</v>
-      </c>
-      <c r="C204" s="17" t="s">
-        <v>417</v>
-      </c>
-      <c r="D204" t="s">
-        <v>419</v>
-      </c>
-      <c r="E204" s="17" t="s">
-        <v>446</v>
-      </c>
-      <c r="F204" s="24" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B205" t="s">
-        <v>242</v>
-      </c>
-      <c r="C205" t="s">
-        <v>418</v>
-      </c>
-      <c r="E205" s="17" t="s">
-        <v>241</v>
-      </c>
-      <c r="F205" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B207" s="10" t="s">
+    </row>
+    <row r="208" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B208" s="7"/>
+    </row>
+    <row r="209" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B209" s="12" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="208" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B208" s="7"/>
-    </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B209" s="12" t="s">
+    <row r="210" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
+        <v>247</v>
+      </c>
+      <c r="C210" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="H210" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="211" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
+        <v>248</v>
+      </c>
+      <c r="C211" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="H211" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="212" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
+        <v>249</v>
+      </c>
+      <c r="C212" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="H212" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="214" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B214" s="12" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B210" t="s">
-        <v>248</v>
-      </c>
-      <c r="C210" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B211" t="s">
-        <v>249</v>
-      </c>
-      <c r="C211" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B212" t="s">
-        <v>250</v>
-      </c>
-      <c r="C212" t="s">
+    <row r="215" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B215" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B214" s="12" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="215" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B215" t="s">
+      <c r="C215" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="C215" t="s">
+      <c r="H215" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="217" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B217" s="10" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B217" s="10" t="s">
+    <row r="218" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B218" t="s">
+      <c r="C218" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="C218" t="s">
+      <c r="H218" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="220" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B220" s="10" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B220" s="10" t="s">
+    <row r="221" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B221" t="s">
-        <v>260</v>
-      </c>
-      <c r="C221" t="s">
-        <v>265</v>
+      <c r="C221" s="38" t="s">
+        <v>264</v>
       </c>
       <c r="E221" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F221" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F221" s="24" t="s">
+        <v>437</v>
+      </c>
+      <c r="H221" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="222" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
+        <v>356</v>
+      </c>
+      <c r="C222" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="D222" s="38" t="s">
+        <v>358</v>
+      </c>
+      <c r="E222" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="F222" s="24" t="s">
+        <v>437</v>
+      </c>
+      <c r="H222" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="223" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
+        <v>260</v>
+      </c>
+      <c r="C223" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="H223" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="224" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
+        <v>261</v>
+      </c>
+      <c r="C224" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="H224" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="225" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B225" t="s">
+        <v>262</v>
+      </c>
+      <c r="C225" s="38" t="s">
+        <v>266</v>
+      </c>
+      <c r="E225" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="F225" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="C222" s="23" t="s">
-        <v>361</v>
-      </c>
-      <c r="D222" t="s">
-        <v>362</v>
-      </c>
-      <c r="E222" s="17" t="s">
-        <v>260</v>
-      </c>
-      <c r="F222" s="24" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B223" t="s">
-        <v>261</v>
-      </c>
-      <c r="C223" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B224" t="s">
-        <v>262</v>
-      </c>
-      <c r="C224" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B225" t="s">
+      <c r="H225" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="226" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B226" t="s">
         <v>263</v>
       </c>
-      <c r="C225" t="s">
-        <v>267</v>
-      </c>
-      <c r="E225" s="17" t="s">
-        <v>363</v>
-      </c>
-      <c r="F225" s="24" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B226" t="s">
-        <v>264</v>
-      </c>
-      <c r="C226" t="s">
-        <v>359</v>
+      <c r="C226" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="H226" t="s">
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-LL1Parser class made and much more
- START IMPOR PACKAGE CFG PARTIALLY TESTED
- CFG AND FIRST SET IS ADDED OF <START>
</commit_message>
<xml_diff>
--- a/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
+++ b/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omera\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\omer\myGitHub\Front-End-Compiler-Project\Mio Language Design\Syntax Analyze Phase\FirstFollowSelectionSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6529ED-5BBC-403F-83C9-6585570FFFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182E7041-0906-4DB7-957D-1152D38C861F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="494">
   <si>
     <t>&lt;Start&gt;</t>
   </si>
@@ -763,9 +763,6 @@
   </si>
   <si>
     <t>FIRST SET (substituting NN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;PACKAGE&gt; </t>
   </si>
   <si>
     <t>Class</t>
@@ -1564,6 +1561,12 @@
   <si>
     <t>mdm ? pm ? rop ? and ? or 
 ? ]  ? ) ? , ? }  ? :  ? ;</t>
+  </si>
+  <si>
+    <t>&lt;PACKAGE&gt;  | null</t>
+  </si>
+  <si>
+    <t>package | null</t>
   </si>
 </sst>
 </file>
@@ -2132,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C160" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="I170" sqref="I170"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,19 +2163,19 @@
         <v>244</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="F1" s="22" t="s">
-        <v>294</v>
-      </c>
       <c r="G1" s="22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
@@ -2187,13 +2190,19 @@
         <v>0</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>245</v>
+        <v>492</v>
       </c>
       <c r="D3" s="35" t="s">
+        <v>493</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
-        <v>355</v>
+      <c r="I3" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2201,22 +2210,22 @@
         <v>4</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -2224,22 +2233,22 @@
         <v>6</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2247,22 +2256,22 @@
         <v>7</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -2290,19 +2299,19 @@
         <v>9</v>
       </c>
       <c r="D10" s="43" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E10" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="F10" t="s">
         <v>348</v>
       </c>
-      <c r="F10" t="s">
-        <v>349</v>
-      </c>
       <c r="G10" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -2318,20 +2327,20 @@
         <v>10</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -2342,19 +2351,19 @@
         <v>28</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -2422,23 +2431,23 @@
         <v>19</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D22" s="2"/>
       <c r="H22" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -2458,11 +2467,11 @@
         <v>23</v>
       </c>
       <c r="C26" s="45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
@@ -2470,11 +2479,11 @@
         <v>24</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -2486,10 +2495,10 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>29</v>
@@ -2500,20 +2509,20 @@
         <v>26</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>29</v>
       </c>
       <c r="I29" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -2521,11 +2530,11 @@
         <v>27</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
@@ -2535,7 +2544,7 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -2549,16 +2558,16 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F33" s="29" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -2612,13 +2621,13 @@
         <v>35</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D40" s="45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
@@ -2635,16 +2644,16 @@
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="45" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
@@ -2657,13 +2666,13 @@
         <v>39</v>
       </c>
       <c r="C44" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="D44" s="35" t="s">
         <v>367</v>
       </c>
-      <c r="D44" s="35" t="s">
-        <v>368</v>
-      </c>
       <c r="H44" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
@@ -2671,22 +2680,22 @@
         <v>40</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D45" s="35" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E45" s="17" t="s">
         <v>39</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G45" s="24" t="s">
         <v>38</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I45" t="s">
         <v>38</v>
@@ -2721,41 +2730,41 @@
         <v>44</v>
       </c>
       <c r="C49" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="D49" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="D49" s="35" t="s">
-        <v>257</v>
-      </c>
       <c r="H49" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>45</v>
       </c>
       <c r="D50" s="35" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C51" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="C51" s="15" t="s">
-        <v>260</v>
-      </c>
       <c r="D51" s="35" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
@@ -2763,36 +2772,36 @@
         <v>45</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D52" s="35" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="53" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D53" s="35" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G53" s="24" t="s">
         <v>38</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I53" t="s">
         <v>38</v>
@@ -2803,11 +2812,11 @@
         <v>46</v>
       </c>
       <c r="C54" s="35" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D54" s="2"/>
       <c r="H54" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
@@ -2830,10 +2839,10 @@
         <v>55</v>
       </c>
       <c r="D57" s="35" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
@@ -2844,10 +2853,10 @@
         <v>56</v>
       </c>
       <c r="D58" s="44" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H58" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
@@ -2855,11 +2864,11 @@
         <v>50</v>
       </c>
       <c r="C59" s="35" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D59" s="2"/>
       <c r="H59" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
@@ -2871,13 +2880,13 @@
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I60" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
@@ -2892,7 +2901,7 @@
         <v>38</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I61" t="s">
         <v>38</v>
@@ -2942,10 +2951,10 @@
         <v>63</v>
       </c>
       <c r="D66" s="35" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
@@ -2956,16 +2965,16 @@
         <v>64</v>
       </c>
       <c r="D67" s="35" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E67" s="17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F67" t="s">
+        <v>262</v>
+      </c>
+      <c r="H67" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
@@ -2975,14 +2984,14 @@
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -2992,25 +3001,25 @@
         <v>65</v>
       </c>
       <c r="C71" s="16" t="s">
+        <v>373</v>
+      </c>
+      <c r="D71" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="E71" s="17" t="s">
         <v>374</v>
       </c>
-      <c r="D71" s="35" t="s">
-        <v>311</v>
-      </c>
-      <c r="E71" s="17" t="s">
-        <v>375</v>
-      </c>
       <c r="F71" s="25" t="s">
+        <v>427</v>
+      </c>
+      <c r="G71" s="28" t="s">
         <v>428</v>
       </c>
-      <c r="G71" s="28" t="s">
-        <v>429</v>
-      </c>
       <c r="H71" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="72" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -3022,13 +3031,13 @@
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F72" s="30" t="s">
+        <v>429</v>
+      </c>
+      <c r="G72" t="s">
         <v>430</v>
-      </c>
-      <c r="G72" t="s">
-        <v>431</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>29</v>
@@ -3036,23 +3045,23 @@
     </row>
     <row r="73" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C73" s="35" t="s">
         <v>254</v>
-      </c>
-      <c r="C73" s="35" t="s">
-        <v>255</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F73" s="31" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
@@ -3075,10 +3084,10 @@
         <v>71</v>
       </c>
       <c r="D75" s="37" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H75" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
@@ -3101,24 +3110,24 @@
         <v>72</v>
       </c>
       <c r="D77" s="36" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E77" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F77" t="s">
         <v>41</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C78" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D78" s="2"/>
     </row>
@@ -3129,7 +3138,7 @@
     </row>
     <row r="80" spans="2:9" ht="135" x14ac:dyDescent="0.25">
       <c r="B80" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
@@ -3139,25 +3148,25 @@
         <v>73</v>
       </c>
       <c r="C81" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="D81" s="39" t="s">
         <v>289</v>
       </c>
-      <c r="D81" s="39" t="s">
-        <v>290</v>
-      </c>
       <c r="E81" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G81" s="28" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H81" s="34" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I81" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
@@ -3165,37 +3174,37 @@
         <v>74</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D82" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E82" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C83" s="35" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="F83" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="F83" s="15" t="s">
-        <v>335</v>
-      </c>
       <c r="H83" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
@@ -3225,16 +3234,16 @@
         <v>90</v>
       </c>
       <c r="D87" s="35" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E87" s="17" t="s">
         <v>10</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
@@ -3245,10 +3254,10 @@
         <v>91</v>
       </c>
       <c r="D88" s="35" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="89" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -3256,13 +3265,13 @@
         <v>79</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D89" s="36" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="90" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -3270,19 +3279,19 @@
         <v>80</v>
       </c>
       <c r="C90" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="D90" s="35" t="s">
         <v>383</v>
       </c>
-      <c r="D90" s="35" t="s">
-        <v>384</v>
-      </c>
       <c r="E90" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
@@ -3302,16 +3311,16 @@
         <v>93</v>
       </c>
       <c r="D92" s="37" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E92" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F92" t="s">
         <v>97</v>
       </c>
       <c r="H92" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
@@ -3322,13 +3331,13 @@
         <v>94</v>
       </c>
       <c r="D93" s="35" t="s">
+        <v>405</v>
+      </c>
+      <c r="E93" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="H93" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="E93" s="24" t="s">
-        <v>310</v>
-      </c>
-      <c r="H93" s="2" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="94" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3336,19 +3345,19 @@
         <v>84</v>
       </c>
       <c r="C94" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D94" s="40" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E94" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F94" t="s">
         <v>97</v>
       </c>
       <c r="H94" s="20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="95" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -3359,19 +3368,19 @@
         <v>95</v>
       </c>
       <c r="D95" s="36" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E95" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="F95" s="17" t="s">
         <v>314</v>
-      </c>
-      <c r="F95" s="17" t="s">
-        <v>315</v>
       </c>
       <c r="G95" s="24" t="s">
         <v>97</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I95" t="s">
         <v>97</v>
@@ -3382,22 +3391,22 @@
         <v>86</v>
       </c>
       <c r="C96" s="16" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D96" s="36" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E96" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F96" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G96" s="24" t="s">
         <v>97</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I96" t="s">
         <v>97</v>
@@ -3408,22 +3417,22 @@
         <v>87</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D97" s="36" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E97" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G97" s="24" t="s">
         <v>97</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I97" t="s">
         <v>97</v>
@@ -3431,25 +3440,25 @@
     </row>
     <row r="98" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C98" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D98" s="35" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E98" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F98" s="17" t="s">
         <v>316</v>
-      </c>
-      <c r="F98" s="17" t="s">
-        <v>317</v>
       </c>
       <c r="G98" s="24" t="s">
         <v>97</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I98" t="s">
         <v>97</v>
@@ -3503,32 +3512,32 @@
         <v>101</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D104" s="35" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C105" s="15" t="s">
         <v>103</v>
       </c>
       <c r="D105" s="35" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C106" s="35" t="s">
         <v>104</v>
@@ -3546,10 +3555,10 @@
         <v>105</v>
       </c>
       <c r="D107" s="39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H107" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
@@ -3584,10 +3593,10 @@
         <v>110</v>
       </c>
       <c r="D111" s="35" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
@@ -3613,10 +3622,10 @@
         <v>29</v>
       </c>
       <c r="E114" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F114" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>29</v>
@@ -3633,10 +3642,10 @@
         <v>29</v>
       </c>
       <c r="E115" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F115" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G115" s="8"/>
       <c r="H115" s="2" t="s">
@@ -3652,10 +3661,10 @@
       </c>
       <c r="D116" s="2"/>
       <c r="E116" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>127</v>
@@ -3670,10 +3679,10 @@
       </c>
       <c r="D117" s="2"/>
       <c r="E117" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H117" s="4" t="s">
         <v>128</v>
@@ -3687,16 +3696,16 @@
         <v>129</v>
       </c>
       <c r="D118" s="36" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E118" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F118" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
@@ -3704,10 +3713,10 @@
         <v>117</v>
       </c>
       <c r="C119" s="38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H119" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
@@ -3718,36 +3727,36 @@
         <v>129</v>
       </c>
       <c r="D120" s="37" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H120" s="8" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="121" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>119</v>
       </c>
       <c r="C121" s="17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D121" s="38" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E121" s="17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F121" s="32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G121" s="33" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H121" s="8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I121" s="20" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="122" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -3755,16 +3764,16 @@
         <v>120</v>
       </c>
       <c r="C122" s="38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E122" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F122" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G122" s="20" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="123" spans="2:9" ht="75" x14ac:dyDescent="0.25">
@@ -3775,16 +3784,16 @@
         <v>130</v>
       </c>
       <c r="D123" s="38" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E123" s="17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F123" s="20" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H123" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
@@ -3806,10 +3815,10 @@
         <v>132</v>
       </c>
       <c r="D125" s="37" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H125" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
@@ -3831,10 +3840,10 @@
         <v>144</v>
       </c>
       <c r="D128" s="37" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H128" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="129" spans="2:8" x14ac:dyDescent="0.25">
@@ -3845,10 +3854,10 @@
         <v>133</v>
       </c>
       <c r="D129" s="38" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H129" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="130" spans="2:8" x14ac:dyDescent="0.25">
@@ -3870,10 +3879,10 @@
         <v>144</v>
       </c>
       <c r="D131" s="37" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H131" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.25">
@@ -3906,10 +3915,10 @@
         <v>135</v>
       </c>
       <c r="D136" s="36" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="137" spans="2:8" x14ac:dyDescent="0.25">
@@ -3937,36 +3946,36 @@
         <v>147</v>
       </c>
       <c r="C140" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D140" s="38" t="s">
+        <v>390</v>
+      </c>
+      <c r="E140" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="F140" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="E140" s="25" t="s">
-        <v>352</v>
-      </c>
-      <c r="F140" s="8" t="s">
-        <v>392</v>
-      </c>
       <c r="H140" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="141" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C141" s="38" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E141" s="17" t="s">
         <v>147</v>
       </c>
       <c r="F141" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H141" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="142" spans="2:8" x14ac:dyDescent="0.25">
@@ -3977,10 +3986,10 @@
         <v>152</v>
       </c>
       <c r="D142" s="44" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H142" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="143" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -3991,16 +4000,16 @@
         <v>153</v>
       </c>
       <c r="D143" s="35" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E143" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F143" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="H143" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="H143" s="2" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="144" spans="2:8" x14ac:dyDescent="0.25">
@@ -4008,11 +4017,11 @@
         <v>150</v>
       </c>
       <c r="C144" s="41" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D144" s="5"/>
       <c r="H144" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.25">
@@ -4036,19 +4045,19 @@
         <v>156</v>
       </c>
       <c r="C148" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D148" s="38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E148" s="17" t="s">
         <v>62</v>
       </c>
       <c r="F148" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H148" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="149" spans="2:9" x14ac:dyDescent="0.25">
@@ -4062,7 +4071,7 @@
         <v>156</v>
       </c>
       <c r="F149" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H149" t="s">
         <v>162</v>
@@ -4076,16 +4085,16 @@
         <v>23</v>
       </c>
       <c r="D150" s="38" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E150" s="17" t="s">
         <v>157</v>
       </c>
       <c r="F150" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H150" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="151" spans="2:9" x14ac:dyDescent="0.25">
@@ -4096,19 +4105,19 @@
         <v>163</v>
       </c>
       <c r="D151" s="44" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E151" s="17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F151" s="17" t="s">
         <v>157</v>
       </c>
       <c r="G151" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H151" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.25">
@@ -4146,16 +4155,16 @@
         <v>168</v>
       </c>
       <c r="D156" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E156" s="17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F156" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="157" spans="2:9" x14ac:dyDescent="0.25">
@@ -4166,16 +4175,16 @@
         <v>179</v>
       </c>
       <c r="E157" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F157" s="28" t="s">
+        <v>477</v>
+      </c>
+      <c r="H157" t="s">
         <v>478</v>
       </c>
-      <c r="H157" t="s">
-        <v>479</v>
-      </c>
       <c r="I157" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="158" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4186,16 +4195,16 @@
         <v>170</v>
       </c>
       <c r="D158" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E158" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F158" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="159" spans="2:9" x14ac:dyDescent="0.25">
@@ -4203,22 +4212,22 @@
         <v>169</v>
       </c>
       <c r="C159" s="44" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E159" s="23" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F159" s="25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G159" s="24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H159" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I159" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="160" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4229,16 +4238,16 @@
         <v>172</v>
       </c>
       <c r="D160" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E160" s="26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F160" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="161" spans="2:9" x14ac:dyDescent="0.25">
@@ -4246,22 +4255,22 @@
         <v>171</v>
       </c>
       <c r="C161" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E161" s="23" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F161" s="25" t="s">
+        <v>440</v>
+      </c>
+      <c r="G161" s="24" t="s">
         <v>441</v>
       </c>
-      <c r="G161" s="24" t="s">
-        <v>442</v>
-      </c>
       <c r="H161" t="s">
+        <v>480</v>
+      </c>
+      <c r="I161" t="s">
         <v>481</v>
-      </c>
-      <c r="I161" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="162" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4272,16 +4281,16 @@
         <v>174</v>
       </c>
       <c r="D162" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E162" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F162" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H162" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="163" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -4292,19 +4301,19 @@
         <v>180</v>
       </c>
       <c r="E163" s="25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F163" s="25" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G163" s="24" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H163" t="s">
+        <v>482</v>
+      </c>
+      <c r="I163" t="s">
         <v>483</v>
-      </c>
-      <c r="I163" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="164" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4315,16 +4324,16 @@
         <v>181</v>
       </c>
       <c r="D164" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E164" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F164" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="165" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -4332,22 +4341,22 @@
         <v>175</v>
       </c>
       <c r="C165" s="38" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E165" s="25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F165" s="25" t="s">
+        <v>447</v>
+      </c>
+      <c r="G165" s="28" t="s">
         <v>448</v>
       </c>
-      <c r="G165" s="28" t="s">
-        <v>449</v>
-      </c>
       <c r="H165" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="I165" s="8" t="s">
         <v>485</v>
-      </c>
-      <c r="I165" s="8" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="166" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4358,16 +4367,16 @@
         <v>177</v>
       </c>
       <c r="D166" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E166" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F166" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H166" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="167" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -4378,19 +4387,19 @@
         <v>182</v>
       </c>
       <c r="E167" s="25" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F167" s="25" t="s">
+        <v>450</v>
+      </c>
+      <c r="G167" s="28" t="s">
         <v>451</v>
       </c>
-      <c r="G167" s="28" t="s">
-        <v>452</v>
-      </c>
       <c r="H167" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I167" s="8" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="168" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4401,16 +4410,16 @@
         <v>178</v>
       </c>
       <c r="D168" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E168" s="17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F168" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H168" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="169" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4421,16 +4430,16 @@
         <v>183</v>
       </c>
       <c r="D169" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E169" s="27" t="s">
         <v>177</v>
       </c>
       <c r="F169" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="171" spans="2:9" x14ac:dyDescent="0.25">
@@ -4446,19 +4455,19 @@
         <v>188</v>
       </c>
       <c r="D172" s="36" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E172" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F172" s="18" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G172" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H172" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="173" spans="2:9" x14ac:dyDescent="0.25">
@@ -4485,7 +4494,7 @@
     </row>
     <row r="176" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B176" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="177" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -4501,13 +4510,13 @@
     </row>
     <row r="178" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B178" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C178" s="40" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H178" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="180" spans="2:9" x14ac:dyDescent="0.25">
@@ -4531,13 +4540,13 @@
         <v>10</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H182" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="183" spans="2:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>195</v>
       </c>
@@ -4548,13 +4557,13 @@
         <v>194</v>
       </c>
       <c r="F183" s="28" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H183" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I183" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="185" spans="2:9" x14ac:dyDescent="0.25">
@@ -4581,10 +4590,10 @@
         <v>205</v>
       </c>
       <c r="D187" s="38" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H187" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="188" spans="2:9" x14ac:dyDescent="0.25">
@@ -4600,16 +4609,16 @@
     </row>
     <row r="189" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C189" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D189" s="37" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H189" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="191" spans="2:9" x14ac:dyDescent="0.25">
@@ -4641,10 +4650,10 @@
         <v>212</v>
       </c>
       <c r="D195" s="38" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H195" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.25">
@@ -4698,7 +4707,7 @@
         <v>222</v>
       </c>
       <c r="E203" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H203" t="s">
         <v>222</v>
@@ -4709,39 +4718,39 @@
         <v>220</v>
       </c>
       <c r="C204" s="18" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D204" s="38" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E204" s="17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F204" s="24" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H204" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I204" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C205" s="38" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E205" s="17" t="s">
         <v>220</v>
       </c>
       <c r="F205" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H205" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="207" spans="2:9" x14ac:dyDescent="0.25">
@@ -4773,10 +4782,10 @@
         <v>227</v>
       </c>
       <c r="C211" s="44" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H211" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="212" spans="2:9" x14ac:dyDescent="0.25">
@@ -4800,10 +4809,10 @@
         <v>231</v>
       </c>
       <c r="C215" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H215" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="217" spans="2:9" x14ac:dyDescent="0.25">
@@ -4838,33 +4847,33 @@
         <v>10</v>
       </c>
       <c r="F221" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H221" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="222" spans="2:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
+        <v>298</v>
+      </c>
+      <c r="C222" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="C222" s="23" t="s">
+      <c r="D222" s="38" t="s">
         <v>300</v>
-      </c>
-      <c r="D222" s="38" t="s">
-        <v>301</v>
       </c>
       <c r="E222" s="17" t="s">
         <v>236</v>
       </c>
       <c r="F222" s="28" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H222" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I222" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="223" spans="2:9" x14ac:dyDescent="0.25">
@@ -4897,16 +4906,16 @@
         <v>243</v>
       </c>
       <c r="E225" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="F225" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="F225" s="24" t="s">
-        <v>303</v>
-      </c>
       <c r="H225" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I225" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="226" spans="2:9" x14ac:dyDescent="0.25">
@@ -4914,10 +4923,10 @@
         <v>240</v>
       </c>
       <c r="C226" s="38" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H226" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing update revert if problem
</commit_message>
<xml_diff>
--- a/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
+++ b/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\omer\myGitHub\Front-End-Compiler-Project\Mio Language Design\Syntax Analyze Phase\FirstFollowSelectionSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780D7A95-C5D3-4CB3-8CAE-5E1409C6AE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B67BDEB-1F63-4624-8250-FE9A7382FD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="503">
   <si>
     <t>&lt;Start&gt;</t>
   </si>
@@ -319,12 +319,6 @@
     <t>&lt;TWO_ASSIGN&gt;</t>
   </si>
   <si>
-    <t>dot ? &lt;TWO_ASSIGN&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dot ? ; </t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;INC_DEC&gt;? &lt;ASSIGN_OP&gt; </t>
   </si>
   <si>
@@ -536,9 +530,6 @@
   </si>
   <si>
     <t>Operands</t>
-  </si>
-  <si>
-    <t>&lt;OPERAND&gt;</t>
   </si>
   <si>
     <t>&lt;UNARY&gt;</t>
@@ -819,12 +810,6 @@
 ? charConst ? boolConst ? strConst </t>
   </si>
   <si>
-    <t xml:space="preserve"> dot ? inc_dec ? = ? cma ? [ ? (</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dot ? inc_dec ? = ? cma </t>
-  </si>
-  <si>
     <t xml:space="preserve">inc_dec ? = ? cma </t>
   </si>
   <si>
@@ -832,9 +817,6 @@
   </si>
   <si>
     <t>[ ? id ? dot ? inc_dec ? = ? cma ? [ ? (</t>
-  </si>
-  <si>
-    <t>&lt;INC_DEC_DOT&gt;? &lt;SUBSCRIPT&gt; ? &lt;FN_BRACKETS&gt; ? Null</t>
   </si>
   <si>
     <t>inc_dec ? dot  ? [ ? ( ? Null</t>
@@ -952,13 +934,7 @@
     <t>&lt;SUBSCRIPT&gt;</t>
   </si>
   <si>
-    <t> dot</t>
-  </si>
-  <si>
     <t> dot ? [ ? ( ? Null</t>
-  </si>
-  <si>
-    <t>&lt;POS2&gt; ? &lt;INC_DEC&gt;</t>
   </si>
   <si>
     <t>&lt;POS2&gt;</t>
@@ -1023,33 +999,14 @@
     <t>End only with id, array subscript.</t>
   </si>
   <si>
-    <t>&lt;DOT_id&gt; ? &lt;SUBSCRIPT&gt;  ? 
-&lt;FN_BRACKETS&gt; ? Null</t>
-  </si>
-  <si>
-    <t>&lt;DOT_id&gt; ? F&lt;id_TO_EXPR&gt; ? &lt;OPERAND&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;DOT_id&gt;     </t>
-  </si>
-  <si>
     <t>End with id and array subscript with posibility of pos 
 increment decrement in the end, and function call ends with null.</t>
   </si>
   <si>
-    <t>&lt;DOT_id2&gt; ? &lt;OPERANDS&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;DOT_id2&gt;    </t>
-  </si>
-  <si>
     <t>[  ? id</t>
   </si>
   <si>
     <t xml:space="preserve">dot ? &lt;id_TO_EXPR&gt;  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;DOT_id3&gt; ? &lt;SUBSCRIPT&gt; ? &lt;FN_BRACKETS&gt; </t>
   </si>
   <si>
     <t>F&lt;EXPR1&gt; ? &lt;id_TO_EXPR&gt; ? &lt;F&gt;</t>
@@ -1070,9 +1027,6 @@
 &lt;id_TO_EXPR&gt; ? &lt;J&gt; </t>
   </si>
   <si>
-    <t>&lt;INIT&gt; ? F&lt;id_TO_EXPR&gt; ? &lt;IS_FLAG&gt;</t>
-  </si>
-  <si>
     <t>pm ? Parent ? Self ? id ? ( ? typeCast ? not? intConst ? 
 floatConst ? charConst ? boolConst ? strConst ?  new ? NaN</t>
   </si>
@@ -1132,10 +1086,6 @@
   </si>
   <si>
     <t>[ ? protected ? private ? id</t>
-  </si>
-  <si>
-    <t>power ?  mdm ?  pm ? Rop ? 
-And ? Or ? &lt;OPER_TO_EXPR&gt; ? &lt;OPERAND&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">power ?  mdm ?  pm ? Rop ? 
@@ -1155,9 +1105,6 @@
 Or ? Null</t>
   </si>
   <si>
-    <t>, ? ; ? power ?  mdm ?  pm ? Rop ? And ? Or ? &lt;OPER_TO_EXPR&gt; ? &lt;IS_FLAG&gt;</t>
-  </si>
-  <si>
     <t>And ? null</t>
   </si>
   <si>
@@ -1205,10 +1152,6 @@
   </si>
   <si>
     <t xml:space="preserve">power ? mdm? pm? Rop ? And ? or ? ]  ? ) ? , ? }  ?  :  ? ; </t>
-  </si>
-  <si>
-    <t>&lt;DOT_id5&gt; ? &lt;SUBSCRIPT&gt;? &lt;FN_BRACKETS&gt; 
- ? Null</t>
   </si>
   <si>
     <t>SELECTION SET NULL</t>
@@ -1529,9 +1472,6 @@
 floatConst ? charConst ? boolConst ? strConst ?  new ? NaN ? )</t>
   </si>
   <si>
-    <t>&lt;INC_DEC&gt; ?  &lt;DOT_ID2&gt;</t>
-  </si>
-  <si>
     <t>&lt;IS_ACMETH&gt;? &lt;INC_DEC&gt; ? ( ? &lt;UNARY&gt;
 ? &lt;CONST&gt; ? &lt;FLAG&gt;</t>
   </si>
@@ -1572,6 +1512,95 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;DOT_ID3&gt;   </t>
+  </si>
+  <si>
+    <t>if ? shift ? const ? dt ?str? id ? Parent ?
+ Self ?  test ?  loop ? do ? stop ? ret ? Cont ? raise?state ? default ? } ?else ?till?;</t>
+  </si>
+  <si>
+    <t>&lt;DOT_ID_SUBSCRIPT&gt; ? 
+&lt;FN_BRACKETS&gt; ? Null</t>
+  </si>
+  <si>
+    <t>&lt;DOT_ID_SUBSCRIPT&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dot ? &lt;SUBSCRIPT&gt;  </t>
+  </si>
+  <si>
+    <t>&lt;DOT_ID_SUBSCRIPT2&gt;</t>
+  </si>
+  <si>
+    <t>&lt;INC_DEC&gt; ?  &lt;DOT_ID_SUBSCRIPT2&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dot ? [ </t>
+  </si>
+  <si>
+    <t>&lt;INC_DEC_DOT&gt; ? &lt;FN_BRACKETS&gt;</t>
+  </si>
+  <si>
+    <t>dot ? &lt;SUBSCRIPT&gt;  ? NULL</t>
+  </si>
+  <si>
+    <t>dot ? [ ?null</t>
+  </si>
+  <si>
+    <t>inc_dec ? dot ? [?null</t>
+  </si>
+  <si>
+    <t>&lt;DOT_ID3&gt; ? &lt;FN_BRACKETS&gt; ?  
+&lt;TWO_ASSIGN&gt;</t>
+  </si>
+  <si>
+    <t>dot ? &lt;SUBSCRIPT&gt;</t>
+  </si>
+  <si>
+    <t>&lt;DOT_ID3&gt;?;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dot ? [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  dot ? [ ? ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dot ? [ ? ; ? ( ? Inc_dec ? = ? cma</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dot ? [ ? ; ? ( ? Inc_dec ? = ? Cma</t>
+  </si>
+  <si>
+    <t>dot ? [ ? ;</t>
+  </si>
+  <si>
+    <t> dot ? &lt;SUBSCRIPT&gt; ? Null</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;FN_BRACKETS&gt; ? &lt;DOT_ID5&gt;
+</t>
+  </si>
+  <si>
+    <t>&lt;POS2&gt; ? &lt;INC_DEC_DOT&gt;</t>
+  </si>
+  <si>
+    <t>&lt;DOT_ID_SUBSCRIPT2&gt; ? &lt;OPERANDS&gt;</t>
+  </si>
+  <si>
+    <t>F&lt;ID_TO_EXPR&gt; ? &lt;IS_FLAG&gt;</t>
+  </si>
+  <si>
+    <t>power ?  mdm ?  pm ? Rop ? And ? Or ? &lt;OPER_TO_EXPR&gt; ? &lt;IS_FLAG&gt;</t>
+  </si>
+  <si>
+    <t>&lt;OPERANDS&gt;</t>
+  </si>
+  <si>
+    <t>&lt;DOT_ID_SUBSCRIPT&gt; ? F&lt;ID_TO_EXPR&gt; ? &lt;OPERANDS&gt;</t>
+  </si>
+  <si>
+    <t>power ?  mdm ?  pm ? Rop ? 
+And ? Or ? &lt;OPER_TO_EXPR&gt; ? &lt;OPERANDS&gt;</t>
   </si>
 </sst>
 </file>
@@ -1889,7 +1918,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2107,6 +2136,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="40% - Accent1" xfId="6" builtinId="31"/>
@@ -2398,8 +2430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:A83"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2423,22 +2455,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E1" s="63" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
@@ -2458,13 +2490,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="F3" s="37"/>
       <c r="G3" s="37"/>
@@ -2472,7 +2504,7 @@
         <v>18</v>
       </c>
       <c r="I3" s="46" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2480,23 +2512,23 @@
         <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>467</v>
+        <v>449</v>
       </c>
       <c r="E4" s="64" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G4" s="37"/>
       <c r="H4" s="47" t="s">
-        <v>466</v>
+        <v>448</v>
       </c>
       <c r="I4" s="46" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -2504,23 +2536,23 @@
         <v>6</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="E5" s="64" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G5" s="37"/>
       <c r="H5" s="47" t="s">
-        <v>436</v>
+        <v>418</v>
       </c>
       <c r="I5" s="46" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2528,23 +2560,23 @@
         <v>7</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="E6" s="64" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G6" s="37"/>
       <c r="H6" s="47" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="I6" s="46" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -2584,22 +2616,22 @@
         <v>8</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="E10" s="65" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H10" s="48" t="s">
-        <v>475</v>
+        <v>457</v>
       </c>
       <c r="I10" s="46"/>
     </row>
@@ -2626,20 +2658,20 @@
         <v>9</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>470</v>
+        <v>452</v>
       </c>
       <c r="E13" s="64" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="G13" s="38"/>
       <c r="H13" s="48" t="s">
-        <v>470</v>
+        <v>452</v>
       </c>
       <c r="I13" s="46"/>
     </row>
@@ -2648,23 +2680,23 @@
         <v>10</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c r="E14" s="64" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="G14" s="37"/>
       <c r="H14" s="48" t="s">
-        <v>473</v>
+        <v>455</v>
       </c>
       <c r="I14" s="46" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -2694,14 +2726,14 @@
         <v>11</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="32"/>
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
       <c r="H17" s="49" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="I17" s="46"/>
     </row>
@@ -2764,30 +2796,30 @@
         <v>17</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="32"/>
       <c r="F22" s="37"/>
       <c r="G22" s="37"/>
       <c r="H22" s="49" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="I22" s="46"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="32"/>
       <c r="F23" s="37"/>
       <c r="G23" s="37"/>
       <c r="H23" s="49" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="I23" s="46"/>
     </row>
@@ -2818,14 +2850,14 @@
         <v>21</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="32"/>
       <c r="F26" s="37"/>
       <c r="G26" s="37"/>
       <c r="H26" s="49" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="I26" s="46"/>
     </row>
@@ -2834,14 +2866,14 @@
         <v>22</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="32"/>
       <c r="F27" s="37"/>
       <c r="G27" s="37"/>
       <c r="H27" s="49" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I27" s="46"/>
     </row>
@@ -2854,10 +2886,10 @@
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="64" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="G28" s="37"/>
       <c r="H28" s="49" t="s">
@@ -2870,21 +2902,21 @@
         <v>24</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="65" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="F29" s="39" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="G29" s="37"/>
       <c r="H29" s="49" t="s">
         <v>26</v>
       </c>
       <c r="I29" s="46" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -2892,14 +2924,14 @@
         <v>25</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="32"/>
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
       <c r="H30" s="49" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="I30" s="46"/>
     </row>
@@ -2915,7 +2947,7 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2934,17 +2966,17 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="64" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="F33" s="58" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="G33" s="37"/>
       <c r="H33" s="49" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="I33" s="46" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -3026,16 +3058,16 @@
         <v>32</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="E40" s="32"/>
       <c r="F40" s="37"/>
       <c r="G40" s="37"/>
       <c r="H40" s="49" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="I40" s="46"/>
     </row>
@@ -3057,19 +3089,19 @@
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="E42" s="32"/>
       <c r="F42" s="37"/>
       <c r="G42" s="37"/>
       <c r="H42" s="49" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="I42" s="46"/>
     </row>
@@ -3088,16 +3120,16 @@
         <v>36</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="E44" s="32"/>
       <c r="F44" s="37"/>
       <c r="G44" s="37"/>
       <c r="H44" s="49" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="I44" s="46"/>
     </row>
@@ -3106,22 +3138,22 @@
         <v>37</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E45" s="64" t="s">
         <v>36</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G45" s="39" t="s">
         <v>35</v>
       </c>
       <c r="H45" s="49" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="I45" s="46" t="s">
         <v>35</v>
@@ -3170,52 +3202,52 @@
         <v>41</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E49" s="32"/>
       <c r="F49" s="37"/>
       <c r="G49" s="37"/>
       <c r="H49" s="49" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I49" s="46"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>42</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="E50" s="32"/>
       <c r="F50" s="37"/>
       <c r="G50" s="37"/>
       <c r="H50" s="49" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="I50" s="46"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="E51" s="32"/>
       <c r="F51" s="37"/>
       <c r="G51" s="37"/>
       <c r="H51" s="49" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="I51" s="46"/>
     </row>
@@ -3224,40 +3256,40 @@
         <v>42</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="E52" s="32"/>
       <c r="F52" s="37"/>
       <c r="G52" s="37"/>
       <c r="H52" s="49" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="I52" s="46"/>
     </row>
     <row r="53" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="E53" s="64" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G53" s="39" t="s">
         <v>35</v>
       </c>
       <c r="H53" s="49" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="I53" s="46" t="s">
         <v>35</v>
@@ -3268,14 +3300,14 @@
         <v>43</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="32"/>
       <c r="F54" s="37"/>
       <c r="G54" s="37"/>
       <c r="H54" s="49" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="I54" s="46"/>
     </row>
@@ -3309,13 +3341,13 @@
         <v>52</v>
       </c>
       <c r="D57" s="19" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E57" s="32"/>
       <c r="F57" s="37"/>
       <c r="G57" s="37"/>
       <c r="H57" s="49" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="I57" s="46"/>
     </row>
@@ -3324,16 +3356,16 @@
         <v>46</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="E58" s="32"/>
       <c r="F58" s="37"/>
       <c r="G58" s="37"/>
       <c r="H58" s="45" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="I58" s="46"/>
     </row>
@@ -3342,14 +3374,14 @@
         <v>47</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="32"/>
       <c r="F59" s="37"/>
       <c r="G59" s="37"/>
       <c r="H59" s="49" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I59" s="46"/>
     </row>
@@ -3362,15 +3394,15 @@
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="33" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="F60" s="37"/>
       <c r="G60" s="37"/>
       <c r="H60" s="49" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="I60" s="46" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
@@ -3387,7 +3419,7 @@
       <c r="F61" s="37"/>
       <c r="G61" s="37"/>
       <c r="H61" s="49" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="I61" s="46" t="s">
         <v>35</v>
@@ -3455,13 +3487,13 @@
         <v>59</v>
       </c>
       <c r="D66" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E66" s="32"/>
       <c r="F66" s="37"/>
       <c r="G66" s="37"/>
       <c r="H66" s="49" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="I66" s="46"/>
     </row>
@@ -3473,17 +3505,17 @@
         <v>60</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E67" s="64" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="F67" s="37" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G67" s="37"/>
       <c r="H67" s="49" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="I67" s="46"/>
     </row>
@@ -3499,7 +3531,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B69" s="9" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -3511,7 +3543,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B70" s="9" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3527,25 +3559,25 @@
         <v>61</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>329</v>
+        <v>476</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E71" s="64" t="s">
-        <v>330</v>
+        <v>501</v>
       </c>
       <c r="F71" s="59" t="s">
-        <v>363</v>
+        <v>502</v>
       </c>
       <c r="G71" s="40" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="H71" s="47" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
       <c r="I71" s="50" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3558,13 +3590,13 @@
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="66" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
       <c r="F72" s="60" t="s">
-        <v>490</v>
+        <v>471</v>
       </c>
       <c r="G72" s="38" t="s">
-        <v>491</v>
+        <v>472</v>
       </c>
       <c r="H72" s="49" t="s">
         <v>26</v>
@@ -3574,29 +3606,30 @@
     <row r="73" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="30"/>
       <c r="B73" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="D73" s="19" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E73" s="64" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="F73" s="18" t="s">
-        <v>491</v>
+        <v>472</v>
       </c>
       <c r="G73" s="37"/>
       <c r="H73" s="47" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
       <c r="I73" s="50" t="s">
-        <v>491</v>
+        <v>472</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="30"/>
       <c r="B74" s="1" t="s">
         <v>63</v>
       </c>
@@ -3613,6 +3646,7 @@
       <c r="I74" s="46"/>
     </row>
     <row r="75" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="30"/>
       <c r="B75" s="1" t="s">
         <v>64</v>
       </c>
@@ -3620,17 +3654,18 @@
         <v>67</v>
       </c>
       <c r="D75" s="21" t="s">
-        <v>482</v>
+        <v>464</v>
       </c>
       <c r="E75" s="32"/>
       <c r="F75" s="37"/>
       <c r="G75" s="37"/>
       <c r="H75" s="48" t="s">
-        <v>482</v>
+        <v>464</v>
       </c>
       <c r="I75" s="46"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="30"/>
       <c r="B76" s="1" t="s">
         <v>65</v>
       </c>
@@ -3647,6 +3682,7 @@
       <c r="I76" s="46"/>
     </row>
     <row r="77" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A77" s="30"/>
       <c r="B77" s="1" t="s">
         <v>66</v>
       </c>
@@ -3654,33 +3690,36 @@
         <v>68</v>
       </c>
       <c r="D77" s="20" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="E77" s="64" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="F77" s="37" t="s">
         <v>38</v>
       </c>
       <c r="G77" s="37"/>
       <c r="H77" s="47" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="I77" s="46"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="30"/>
       <c r="B78" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="C78" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="D78" s="1"/>
+        <v>477</v>
+      </c>
+      <c r="C78" s="99" t="s">
+        <v>478</v>
+      </c>
+      <c r="D78" s="19" t="s">
+        <v>481</v>
+      </c>
       <c r="E78" s="32"/>
       <c r="F78" s="37"/>
       <c r="G78" s="37"/>
       <c r="H78" s="45" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="I78" s="46"/>
     </row>
@@ -3696,7 +3735,7 @@
     </row>
     <row r="80" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="B80" s="10" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -3707,73 +3746,76 @@
       <c r="I80" s="46"/>
     </row>
     <row r="81" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="30"/>
       <c r="B81" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>267</v>
+        <v>482</v>
       </c>
       <c r="D81" s="23" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="E81" s="64" t="s">
-        <v>333</v>
+        <v>497</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="G81" s="40" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="H81" s="51" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
       <c r="I81" s="50" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C82" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="D82" s="23" t="s">
+        <v>485</v>
+      </c>
+      <c r="E82" s="64" t="s">
+        <v>301</v>
+      </c>
+      <c r="F82" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="G82" s="40" t="s">
+        <v>349</v>
+      </c>
+      <c r="H82" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="I82" s="46"/>
+    </row>
+    <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B83" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C83" s="99" t="s">
         <v>483</v>
       </c>
-      <c r="D82" s="23" t="s">
-        <v>270</v>
-      </c>
-      <c r="E82" s="64" t="s">
-        <v>309</v>
-      </c>
-      <c r="F82" s="17" t="s">
-        <v>309</v>
-      </c>
-      <c r="G82" s="37"/>
-      <c r="H82" s="52" t="s">
-        <v>270</v>
-      </c>
-      <c r="I82" s="46"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="30"/>
-      <c r="B83" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="C83" s="19" t="s">
-        <v>269</v>
-      </c>
-      <c r="D83" s="1"/>
+      <c r="D83" s="19" t="s">
+        <v>484</v>
+      </c>
       <c r="E83" s="64" t="s">
-        <v>308</v>
+        <v>496</v>
       </c>
       <c r="F83" s="61" t="s">
-        <v>309</v>
-      </c>
-      <c r="G83" s="37"/>
+        <v>301</v>
+      </c>
+      <c r="G83" s="40" t="s">
+        <v>349</v>
+      </c>
       <c r="H83" s="49" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="I83" s="46"/>
     </row>
@@ -3816,16 +3858,16 @@
         <v>73</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="E87" s="32"/>
       <c r="F87" s="38"/>
       <c r="G87" s="37"/>
       <c r="H87" s="49" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="I87" s="46"/>
     </row>
@@ -3837,13 +3879,13 @@
         <v>86</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E88" s="32"/>
       <c r="F88" s="37"/>
       <c r="G88" s="37"/>
       <c r="H88" s="49" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="I88" s="46"/>
     </row>
@@ -3862,16 +3904,16 @@
         <v>75</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
       <c r="D90" s="20" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
       <c r="E90" s="34"/>
       <c r="F90" s="37"/>
       <c r="G90" s="37"/>
       <c r="H90" s="47" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
       <c r="I90" s="46"/>
     </row>
@@ -3880,16 +3922,16 @@
         <v>76</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="D91" s="19" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="E91" s="32"/>
       <c r="F91" s="38"/>
       <c r="G91" s="37"/>
       <c r="H91" s="49" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="I91" s="46"/>
     </row>
@@ -3915,17 +3957,17 @@
         <v>88</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="E93" s="65" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="F93" s="37" t="s">
         <v>91</v>
       </c>
       <c r="G93" s="37"/>
       <c r="H93" s="48" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="I93" s="46"/>
     </row>
@@ -3937,18 +3979,18 @@
         <v>89</v>
       </c>
       <c r="D94" s="19" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="E94" s="33" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="F94" s="37"/>
       <c r="G94" s="37"/>
       <c r="H94" s="49" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="I94" s="46" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3956,20 +3998,20 @@
         <v>80</v>
       </c>
       <c r="C95" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="D95" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="D95" s="24" t="s">
-        <v>261</v>
-      </c>
       <c r="E95" s="32" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="F95" s="37" t="s">
         <v>91</v>
       </c>
       <c r="G95" s="37"/>
       <c r="H95" s="53" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="I95" s="46"/>
     </row>
@@ -3979,22 +4021,22 @@
         <v>81</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="D96" s="20" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="E96" s="64" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="F96" s="17" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="G96" s="39" t="s">
         <v>91</v>
       </c>
       <c r="H96" s="47" t="s">
-        <v>489</v>
+        <v>470</v>
       </c>
       <c r="I96" s="46" t="s">
         <v>91</v>
@@ -4006,22 +4048,22 @@
         <v>82</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
       <c r="D97" s="20" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="E97" s="64" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="G97" s="39" t="s">
         <v>91</v>
       </c>
       <c r="H97" s="47" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="I97" s="46" t="s">
         <v>91</v>
@@ -4032,22 +4074,22 @@
         <v>83</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="E98" s="64" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="G98" s="39" t="s">
         <v>91</v>
       </c>
       <c r="H98" s="47" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="I98" s="46" t="s">
         <v>91</v>
@@ -4055,25 +4097,25 @@
     </row>
     <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="C99" s="11" t="s">
         <v>90</v>
       </c>
       <c r="D99" s="20" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
       <c r="E99" s="65" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="G99" s="39" t="s">
         <v>91</v>
       </c>
       <c r="H99" s="49" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="I99" s="46" t="s">
         <v>91</v>
@@ -4145,55 +4187,57 @@
       <c r="H104" s="45"/>
       <c r="I104" s="46"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C105" s="11" t="s">
-        <v>337</v>
+      <c r="C105" s="12" t="s">
+        <v>486</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>262</v>
+        <v>491</v>
       </c>
       <c r="E105" s="32"/>
       <c r="F105" s="37"/>
       <c r="G105" s="37"/>
       <c r="H105" s="49" t="s">
-        <v>262</v>
+        <v>492</v>
       </c>
       <c r="I105" s="46"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
-        <v>493</v>
+        <v>474</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>97</v>
+        <v>487</v>
       </c>
       <c r="D106" s="19" t="s">
-        <v>263</v>
+        <v>489</v>
       </c>
       <c r="E106" s="32"/>
       <c r="F106" s="37"/>
       <c r="G106" s="37"/>
       <c r="H106" s="49" t="s">
-        <v>263</v>
+        <v>489</v>
       </c>
       <c r="I106" s="46"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
-        <v>492</v>
+        <v>473</v>
       </c>
       <c r="C107" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D107" s="1"/>
+        <v>488</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>493</v>
+      </c>
       <c r="E107" s="32"/>
       <c r="F107" s="37"/>
       <c r="G107" s="37"/>
       <c r="H107" s="49" t="s">
-        <v>98</v>
+        <v>490</v>
       </c>
       <c r="I107" s="46"/>
     </row>
@@ -4202,16 +4246,16 @@
         <v>96</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D108" s="23" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E108" s="32"/>
       <c r="F108" s="37"/>
       <c r="G108" s="37"/>
       <c r="H108" s="52" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I108" s="46"/>
     </row>
@@ -4227,7 +4271,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B110" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -4239,58 +4283,58 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B111" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C111" s="19" t="s">
         <v>101</v>
-      </c>
-      <c r="C111" s="19" t="s">
-        <v>103</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="32" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
       <c r="F111" s="38" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="G111" s="37"/>
       <c r="H111" s="49" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I111" s="46"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C112" s="71" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
       <c r="E112" s="32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F112" s="38"/>
       <c r="G112" s="37"/>
       <c r="H112" s="49" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
       <c r="I112" s="46"/>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D113" s="19" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="E113" s="32" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F113" s="38"/>
       <c r="G113" s="37"/>
       <c r="H113" s="49" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="I113" s="46"/>
     </row>
@@ -4306,7 +4350,7 @@
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -4318,7 +4362,7 @@
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="72" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C116" s="73" t="s">
         <v>23</v>
@@ -4336,7 +4380,7 @@
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="72" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C117" s="73" t="s">
         <v>23</v>
@@ -4354,112 +4398,112 @@
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" s="72" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C118" s="72" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D118" s="72"/>
       <c r="E118" s="77"/>
       <c r="F118" s="75"/>
       <c r="G118" s="81"/>
       <c r="H118" s="91" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I118" s="76"/>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="72" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C119" s="78" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D119" s="72"/>
       <c r="E119" s="74"/>
       <c r="F119" s="75"/>
       <c r="G119" s="81"/>
       <c r="H119" s="92" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I119" s="76"/>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="72" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C120" s="73" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D120" s="79" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E120" s="74"/>
       <c r="F120" s="75"/>
       <c r="G120" s="81"/>
       <c r="H120" s="93" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="I120" s="76"/>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="72" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C121" s="80" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D121" s="80"/>
       <c r="E121" s="74"/>
       <c r="F121" s="81"/>
       <c r="G121" s="81"/>
       <c r="H121" s="94" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I121" s="76"/>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" s="80" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C122" s="82" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D122" s="83" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E122" s="74"/>
       <c r="F122" s="81"/>
       <c r="G122" s="81"/>
       <c r="H122" s="95" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="I122" s="76"/>
     </row>
     <row r="123" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B123" s="80" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C123" s="84" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="D123" s="80" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="E123" s="74"/>
       <c r="F123" s="88"/>
       <c r="G123" s="88"/>
       <c r="H123" s="95" t="s">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="I123" s="86"/>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" s="80" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C124" s="80" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D124" s="80"/>
       <c r="E124" s="74"/>
@@ -4470,61 +4514,61 @@
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B125" s="80" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="C125" s="82" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="D125" s="80" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="E125" s="74"/>
       <c r="F125" s="81"/>
       <c r="G125" s="89"/>
       <c r="H125" s="94" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="I125" s="76"/>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" s="80" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C126" s="82" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
       <c r="D126" s="80" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="E126" s="74"/>
       <c r="F126" s="88"/>
       <c r="G126" s="81"/>
       <c r="H126" s="94" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="I126" s="76"/>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" s="80" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C127" s="87" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="D127" s="88" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="E127" s="74"/>
       <c r="F127" s="89"/>
       <c r="G127" s="81"/>
       <c r="H127" s="96" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="I127" s="76"/>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B128" s="80" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
       <c r="C128" s="85" t="s">
         <v>91</v>
@@ -4540,23 +4584,23 @@
     </row>
     <row r="129" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C129" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D129" s="21" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="E129" s="32" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
       <c r="F129" s="37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G129" s="38"/>
       <c r="H129" s="48" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="I129" s="46"/>
     </row>
@@ -4569,123 +4613,123 @@
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C131" s="90" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="E131" s="32" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
       <c r="F131" s="97" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="G131" s="37"/>
       <c r="H131" s="45" t="s">
         <v>26</v>
       </c>
       <c r="I131" s="46" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
     </row>
     <row r="132" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D132" s="21" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="E132" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F132" s="37"/>
       <c r="G132" s="37"/>
       <c r="H132" s="48" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="I132" s="46"/>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D133" s="22" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E133" s="32"/>
       <c r="F133" s="37"/>
       <c r="G133" s="37"/>
       <c r="H133" s="45" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="I133" s="46"/>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C134" s="90" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="E134" s="32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F134" s="97" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="G134" s="37"/>
       <c r="H134" s="45" t="s">
         <v>26</v>
       </c>
       <c r="I134" s="46" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
     </row>
     <row r="135" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C135" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D135" s="21" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="E135" s="32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F135" s="37"/>
       <c r="G135" s="37"/>
       <c r="H135" s="48" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="I135" s="46"/>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C136" s="90" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="E136" s="32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F136" s="97" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="G136" s="37"/>
       <c r="H136" s="45" t="s">
         <v>26</v>
       </c>
       <c r="I136" s="46" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.25">
@@ -4704,49 +4748,49 @@
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C139" s="22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E139" s="32"/>
       <c r="F139" s="37"/>
       <c r="G139" s="37"/>
       <c r="H139" s="45" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I139" s="46"/>
     </row>
     <row r="140" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C140" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D140" s="20" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="E140" s="32"/>
       <c r="F140" s="37"/>
       <c r="G140" s="37"/>
       <c r="H140" s="47" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="I140" s="46"/>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C141" s="22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E141" s="32"/>
       <c r="F141" s="37"/>
       <c r="G141" s="41"/>
       <c r="H141" s="45" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I141" s="46"/>
     </row>
@@ -4760,7 +4804,7 @@
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B143" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E143" s="32"/>
       <c r="F143" s="37"/>
@@ -4770,88 +4814,88 @@
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C144" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D144" s="22" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="E144" s="32"/>
       <c r="F144" s="38"/>
       <c r="G144" s="37"/>
       <c r="H144" s="45" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="I144" s="46"/>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C145" s="13" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
       <c r="D145" s="19" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
       <c r="E145" s="32"/>
       <c r="F145" s="38"/>
       <c r="G145" s="37"/>
       <c r="H145" s="49" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
       <c r="I145" s="46"/>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="C146" s="13" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D146" s="19" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E146" s="32"/>
       <c r="F146" s="38"/>
       <c r="G146" s="37"/>
       <c r="H146" s="49" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="I146" s="46"/>
     </row>
     <row r="147" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C147" s="70" t="s">
-        <v>478</v>
+        <v>460</v>
       </c>
       <c r="D147" s="25" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="E147" s="32"/>
       <c r="F147" s="37"/>
       <c r="G147" s="37"/>
       <c r="H147" s="54" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="I147" s="46"/>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C148" s="22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E148" s="32"/>
       <c r="F148" s="37"/>
       <c r="G148" s="37"/>
       <c r="H148" s="45" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I148" s="46"/>
     </row>
@@ -4864,7 +4908,7 @@
     </row>
     <row r="150" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B150" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E150" s="32"/>
       <c r="F150" s="37"/>
@@ -4874,85 +4918,85 @@
     </row>
     <row r="151" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C151" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="D151" s="22" t="s">
         <v>244</v>
-      </c>
-      <c r="D151" s="22" t="s">
-        <v>247</v>
       </c>
       <c r="E151" s="32"/>
       <c r="F151" s="37"/>
       <c r="G151" s="37"/>
       <c r="H151" s="55" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="I151" s="46"/>
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C152" s="26" t="s">
-        <v>460</v>
+        <v>442</v>
       </c>
       <c r="D152" s="22" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="E152" s="32"/>
       <c r="F152" s="37"/>
       <c r="G152" s="37"/>
       <c r="H152" s="45" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I152" s="46"/>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>461</v>
+        <v>443</v>
       </c>
       <c r="C153" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D153" s="22" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="E153" s="32"/>
       <c r="F153" s="37"/>
       <c r="G153" s="37"/>
       <c r="H153" s="45" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I153" s="46"/>
     </row>
     <row r="154" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C154" s="13" t="s">
-        <v>463</v>
+        <v>445</v>
       </c>
       <c r="D154" s="28" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="E154" s="32"/>
       <c r="F154" s="37"/>
       <c r="G154" s="37"/>
       <c r="H154" s="45" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="I154" s="46"/>
     </row>
     <row r="155" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>464</v>
+        <v>446</v>
       </c>
       <c r="C155" s="13" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
       <c r="D155" s="28" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="E155" s="32"/>
       <c r="F155" s="37"/>
@@ -4962,31 +5006,31 @@
     </row>
     <row r="156" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C156" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E156" s="32"/>
       <c r="F156" s="37"/>
       <c r="G156" s="37"/>
       <c r="H156" s="54" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I156" s="46"/>
     </row>
     <row r="157" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
+        <v>145</v>
+      </c>
+      <c r="C157" s="22" t="s">
         <v>147</v>
-      </c>
-      <c r="C157" s="22" t="s">
-        <v>149</v>
       </c>
       <c r="E157" s="32"/>
       <c r="F157" s="37"/>
       <c r="G157" s="37"/>
       <c r="H157" s="45" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I157" s="46"/>
     </row>
@@ -4999,7 +5043,7 @@
     </row>
     <row r="159" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B159" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E159" s="32"/>
       <c r="F159" s="37"/>
@@ -5009,246 +5053,246 @@
     </row>
     <row r="160" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
+        <v>149</v>
+      </c>
+      <c r="C160" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="C160" s="13" t="s">
-        <v>153</v>
-      </c>
       <c r="D160" s="20" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="E160" s="64" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="F160" s="37" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="G160" s="37"/>
       <c r="H160" s="47" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="I160" s="46"/>
     </row>
     <row r="161" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C161" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E161" s="64" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
       <c r="F161" s="40" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="G161" s="37"/>
       <c r="H161" s="45" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="I161" s="46" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
     </row>
     <row r="162" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
+        <v>151</v>
+      </c>
+      <c r="C162" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="C162" s="13" t="s">
-        <v>155</v>
-      </c>
       <c r="D162" s="20" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="E162" s="64" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="F162" s="37" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="G162" s="37"/>
       <c r="H162" s="47" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="I162" s="46"/>
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C163" s="28" t="s">
-        <v>369</v>
+        <v>352</v>
       </c>
       <c r="E163" s="67" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="F163" s="59" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="G163" s="39" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="H163" s="45" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="I163" s="46" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="164" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
+        <v>153</v>
+      </c>
+      <c r="C164" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="C164" s="13" t="s">
-        <v>157</v>
-      </c>
       <c r="D164" s="20" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="E164" s="68" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="F164" s="37" t="s">
-        <v>370</v>
+        <v>353</v>
       </c>
       <c r="G164" s="37"/>
       <c r="H164" s="47" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="I164" s="46"/>
     </row>
     <row r="165" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C165" s="22" t="s">
-        <v>373</v>
+        <v>356</v>
       </c>
       <c r="E165" s="67" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="F165" s="59" t="s">
-        <v>371</v>
+        <v>354</v>
       </c>
       <c r="G165" s="39" t="s">
-        <v>372</v>
+        <v>355</v>
       </c>
       <c r="H165" s="45" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="I165" s="46" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
     </row>
     <row r="166" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
+        <v>155</v>
+      </c>
+      <c r="C166" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C166" s="13" t="s">
-        <v>159</v>
-      </c>
       <c r="D166" s="20" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="E166" s="64" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="F166" s="37" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
       <c r="G166" s="37"/>
       <c r="H166" s="47" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="I166" s="46"/>
     </row>
     <row r="167" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C167" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E167" s="66" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F167" s="59" t="s">
-        <v>376</v>
+        <v>359</v>
       </c>
       <c r="G167" s="39" t="s">
-        <v>374</v>
+        <v>357</v>
       </c>
       <c r="H167" s="45" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="I167" s="46" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
     </row>
     <row r="168" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C168" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D168" s="20" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="E168" s="64" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="F168" s="37" t="s">
-        <v>377</v>
+        <v>360</v>
       </c>
       <c r="G168" s="37"/>
       <c r="H168" s="47" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="I168" s="46"/>
     </row>
     <row r="169" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C169" s="22" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="E169" s="66" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="F169" s="59" t="s">
-        <v>378</v>
+        <v>361</v>
       </c>
       <c r="G169" s="40" t="s">
-        <v>379</v>
+        <v>362</v>
       </c>
       <c r="H169" s="48" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="I169" s="50" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
     </row>
     <row r="170" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C170" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D170" s="20" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="E170" s="64" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="F170" s="37" t="s">
-        <v>380</v>
+        <v>363</v>
       </c>
       <c r="G170" s="37"/>
       <c r="H170" s="47" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="I170" s="46"/>
     </row>
@@ -5257,65 +5301,65 @@
         <v>90</v>
       </c>
       <c r="C171" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E171" s="66" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="F171" s="59" t="s">
-        <v>381</v>
+        <v>364</v>
       </c>
       <c r="G171" s="40" t="s">
-        <v>382</v>
+        <v>365</v>
       </c>
       <c r="H171" s="45" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="I171" s="50" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
     </row>
     <row r="172" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C172" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D172" s="20" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="E172" s="64" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="F172" s="37" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="G172" s="37"/>
       <c r="H172" s="47" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="I172" s="46"/>
     </row>
     <row r="173" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="E173" s="69" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F173" s="37" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="G173" s="37"/>
       <c r="H173" s="47" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="I173" s="46"/>
     </row>
@@ -5328,7 +5372,7 @@
     </row>
     <row r="175" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B175" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E175" s="32"/>
       <c r="F175" s="37"/>
@@ -5338,55 +5382,55 @@
     </row>
     <row r="176" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B176" s="5" t="s">
-        <v>170</v>
+        <v>500</v>
       </c>
       <c r="C176" s="14" t="s">
-        <v>484</v>
+        <v>465</v>
       </c>
       <c r="D176" s="20" t="s">
-        <v>485</v>
+        <v>466</v>
       </c>
       <c r="E176" s="64" t="s">
-        <v>343</v>
+        <v>498</v>
       </c>
       <c r="F176" s="62" t="s">
-        <v>368</v>
-      </c>
-      <c r="G176" s="37" t="s">
-        <v>365</v>
+        <v>499</v>
+      </c>
+      <c r="G176" s="38" t="s">
+        <v>349</v>
       </c>
       <c r="H176" s="47" t="s">
-        <v>485</v>
+        <v>466</v>
       </c>
       <c r="I176" s="46"/>
     </row>
     <row r="177" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C177" s="22" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E177" s="32"/>
       <c r="F177" s="37"/>
       <c r="G177" s="37"/>
       <c r="H177" s="45" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I177" s="46"/>
     </row>
     <row r="178" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C178" s="22" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E178" s="32"/>
       <c r="F178" s="37"/>
       <c r="G178" s="37"/>
       <c r="H178" s="45" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I178" s="46"/>
     </row>
@@ -5399,7 +5443,7 @@
     </row>
     <row r="180" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B180" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E180" s="32"/>
       <c r="F180" s="37"/>
@@ -5409,31 +5453,31 @@
     </row>
     <row r="181" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B181" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C181" s="21" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E181" s="32"/>
       <c r="F181" s="37"/>
       <c r="G181" s="37"/>
       <c r="H181" s="48" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I181" s="46"/>
     </row>
     <row r="182" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B182" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C182" s="24" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E182" s="32"/>
       <c r="F182" s="37"/>
       <c r="G182" s="37"/>
       <c r="H182" s="53" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I182" s="46"/>
     </row>
@@ -5446,7 +5490,7 @@
     </row>
     <row r="184" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B184" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E184" s="32"/>
       <c r="F184" s="37"/>
@@ -5456,7 +5500,7 @@
     </row>
     <row r="185" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B185" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E185" s="32"/>
       <c r="F185" s="37"/>
@@ -5466,42 +5510,42 @@
     </row>
     <row r="186" spans="2:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C186" s="22" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E186" s="64" t="s">
         <v>9</v>
       </c>
       <c r="F186" s="38" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="G186" s="37"/>
       <c r="H186" s="45" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I186" s="46"/>
     </row>
     <row r="187" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C187" s="22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E187" s="64" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F187" s="40" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="G187" s="37"/>
       <c r="H187" s="45" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="I187" s="50" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
     </row>
     <row r="188" spans="2:9" x14ac:dyDescent="0.25">
@@ -5513,7 +5557,7 @@
     </row>
     <row r="189" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B189" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E189" s="32"/>
       <c r="F189" s="37"/>
@@ -5523,80 +5567,80 @@
     </row>
     <row r="190" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
+        <v>181</v>
+      </c>
+      <c r="C190" s="22" t="s">
         <v>184</v>
-      </c>
-      <c r="C190" s="22" t="s">
-        <v>187</v>
       </c>
       <c r="E190" s="32"/>
       <c r="F190" s="37"/>
       <c r="G190" s="37"/>
       <c r="H190" s="45" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I190" s="46"/>
     </row>
     <row r="191" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C191" s="13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D191" s="22" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E191" s="32"/>
       <c r="F191" s="37"/>
       <c r="G191" s="37"/>
       <c r="H191" s="45" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="I191" s="46"/>
     </row>
     <row r="192" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C192" s="22" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E192" s="32"/>
       <c r="F192" s="37"/>
       <c r="G192" s="37"/>
       <c r="H192" s="45" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I192" s="46"/>
     </row>
-    <row r="193" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C193" s="13" t="s">
-        <v>476</v>
+        <v>458</v>
       </c>
       <c r="D193" s="21" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
       <c r="E193" s="32"/>
       <c r="F193" s="37"/>
       <c r="G193" s="37"/>
       <c r="H193" s="48" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="I193" s="46"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E194" s="32"/>
       <c r="F194" s="37"/>
       <c r="G194" s="37"/>
       <c r="H194" s="45"/>
       <c r="I194" s="46"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B195" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E195" s="32"/>
       <c r="F195" s="37"/>
@@ -5604,16 +5648,16 @@
       <c r="H195" s="45"/>
       <c r="I195" s="46"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E196" s="32"/>
       <c r="F196" s="37"/>
       <c r="G196" s="37"/>
       <c r="H196" s="45"/>
       <c r="I196" s="46"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B197" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E197" s="32"/>
       <c r="F197" s="37"/>
@@ -5621,49 +5665,49 @@
       <c r="H197" s="45"/>
       <c r="I197" s="46"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C198" s="22" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E198" s="32"/>
       <c r="F198" s="37"/>
       <c r="G198" s="37"/>
       <c r="H198" s="45" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I198" s="46"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C199" s="13" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D199" s="22" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E199" s="32"/>
       <c r="F199" s="37"/>
       <c r="G199" s="37"/>
       <c r="H199" s="45" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="I199" s="46"/>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E200" s="32"/>
       <c r="F200" s="37"/>
       <c r="G200" s="37"/>
       <c r="H200" s="45"/>
       <c r="I200" s="46"/>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B201" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E201" s="32"/>
       <c r="F201" s="37"/>
@@ -5671,46 +5715,46 @@
       <c r="H201" s="45"/>
       <c r="I201" s="46"/>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C202" s="22" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E202" s="32"/>
       <c r="F202" s="37"/>
       <c r="G202" s="37"/>
       <c r="H202" s="45" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I202" s="46"/>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C203" s="22" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E203" s="32"/>
       <c r="F203" s="37"/>
       <c r="G203" s="37"/>
       <c r="H203" s="45" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I203" s="46"/>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E204" s="32"/>
       <c r="F204" s="37"/>
       <c r="G204" s="37"/>
       <c r="H204" s="45"/>
       <c r="I204" s="46"/>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B205" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E205" s="32"/>
       <c r="F205" s="37"/>
@@ -5718,93 +5762,96 @@
       <c r="H205" s="45"/>
       <c r="I205" s="46"/>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
+        <v>199</v>
+      </c>
+      <c r="C206" s="22" t="s">
         <v>202</v>
-      </c>
-      <c r="C206" s="22" t="s">
-        <v>205</v>
       </c>
       <c r="E206" s="32"/>
       <c r="F206" s="37"/>
       <c r="G206" s="37"/>
       <c r="H206" s="45" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I206" s="46"/>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
+        <v>200</v>
+      </c>
+      <c r="C207" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="C207" s="22" t="s">
-        <v>206</v>
-      </c>
       <c r="E207" s="32" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="F207" s="37"/>
       <c r="G207" s="37"/>
       <c r="H207" s="45" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I207" s="46"/>
     </row>
-    <row r="208" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A208" s="30"/>
+    <row r="208" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C208" s="14" t="s">
-        <v>384</v>
+        <v>495</v>
       </c>
       <c r="D208" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="E208" s="64" t="s">
+        <v>423</v>
+      </c>
+      <c r="F208" s="39" t="s">
         <v>307</v>
-      </c>
-      <c r="E208" s="64" t="s">
-        <v>441</v>
-      </c>
-      <c r="F208" s="39" t="s">
-        <v>315</v>
       </c>
       <c r="G208" s="37"/>
       <c r="H208" s="45" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="I208" s="46" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A209" s="30"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="209" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>440</v>
-      </c>
-      <c r="C209" s="22" t="s">
-        <v>306</v>
+        <v>422</v>
+      </c>
+      <c r="C209" s="26" t="s">
+        <v>494</v>
+      </c>
+      <c r="D209" s="22" t="s">
+        <v>300</v>
       </c>
       <c r="E209" s="64" t="s">
-        <v>204</v>
-      </c>
-      <c r="F209" s="37" t="s">
-        <v>315</v>
+        <v>201</v>
+      </c>
+      <c r="F209" s="39" t="s">
+        <v>307</v>
       </c>
       <c r="G209" s="37"/>
       <c r="H209" s="45" t="s">
-        <v>306</v>
-      </c>
-      <c r="I209" s="46"/>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+      <c r="I209" s="46" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="210" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E210" s="32"/>
       <c r="F210" s="37"/>
       <c r="G210" s="37"/>
       <c r="H210" s="45"/>
       <c r="I210" s="46"/>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B211" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E211" s="32"/>
       <c r="F211" s="37"/>
@@ -5812,7 +5859,7 @@
       <c r="H211" s="45"/>
       <c r="I211" s="46"/>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B212" s="4"/>
       <c r="E212" s="32"/>
       <c r="F212" s="37"/>
@@ -5820,9 +5867,9 @@
       <c r="H212" s="45"/>
       <c r="I212" s="46"/>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B213" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E213" s="32"/>
       <c r="F213" s="37"/>
@@ -5830,61 +5877,61 @@
       <c r="H213" s="45"/>
       <c r="I213" s="46"/>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
+        <v>207</v>
+      </c>
+      <c r="C214" s="22" t="s">
         <v>210</v>
-      </c>
-      <c r="C214" s="22" t="s">
-        <v>213</v>
       </c>
       <c r="E214" s="32"/>
       <c r="F214" s="37"/>
       <c r="G214" s="37"/>
       <c r="H214" s="45" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I214" s="46"/>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C215" s="28" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="E215" s="32"/>
       <c r="F215" s="37"/>
       <c r="G215" s="37"/>
       <c r="H215" s="45" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="I215" s="46"/>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C216" s="22" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E216" s="32"/>
       <c r="F216" s="37"/>
       <c r="G216" s="37"/>
       <c r="H216" s="45" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I216" s="46"/>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E217" s="32"/>
       <c r="F217" s="37"/>
       <c r="G217" s="37"/>
       <c r="H217" s="45"/>
       <c r="I217" s="46"/>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B218" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E218" s="32"/>
       <c r="F218" s="37"/>
@@ -5892,31 +5939,31 @@
       <c r="H218" s="45"/>
       <c r="I218" s="46"/>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C219" s="28" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="E219" s="32"/>
       <c r="F219" s="37"/>
       <c r="G219" s="37"/>
       <c r="H219" s="45" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="I219" s="46"/>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E220" s="32"/>
       <c r="F220" s="37"/>
       <c r="G220" s="37"/>
       <c r="H220" s="45"/>
       <c r="I220" s="46"/>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B221" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E221" s="32"/>
       <c r="F221" s="37"/>
@@ -5924,31 +5971,31 @@
       <c r="H221" s="45"/>
       <c r="I221" s="46"/>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C222" s="22" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E222" s="32"/>
       <c r="F222" s="38"/>
       <c r="G222" s="37"/>
       <c r="H222" s="45" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I222" s="46"/>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E223" s="32"/>
       <c r="F223" s="37"/>
       <c r="G223" s="37"/>
       <c r="H223" s="45"/>
       <c r="I223" s="46"/>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B224" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E224" s="32"/>
       <c r="F224" s="37"/>
@@ -5958,50 +6005,50 @@
     </row>
     <row r="225" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C225" s="22" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E225" s="64" t="s">
         <v>9</v>
       </c>
       <c r="F225" s="38" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="G225" s="37"/>
       <c r="H225" s="45" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I225" s="46"/>
     </row>
     <row r="226" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C226" s="16" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D226" s="22" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="E226" s="64" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F226" s="40" t="s">
-        <v>479</v>
+        <v>461</v>
       </c>
       <c r="G226" s="37"/>
       <c r="H226" s="45" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="I226" s="50" t="s">
-        <v>480</v>
+        <v>462</v>
       </c>
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C227" s="22" t="s">
         <v>35</v>
@@ -6016,52 +6063,52 @@
     </row>
     <row r="228" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C228" s="22" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E228" s="32"/>
       <c r="F228" s="37"/>
       <c r="G228" s="37"/>
       <c r="H228" s="45" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I228" s="46"/>
     </row>
     <row r="229" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C229" s="22" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E229" s="64" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F229" s="39" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="G229" s="37"/>
       <c r="H229" s="45" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="I229" s="46" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="230" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B230" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C230" s="22" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E230" s="35"/>
       <c r="F230" s="42"/>
       <c r="G230" s="42"/>
       <c r="H230" s="56" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="I230" s="57"/>
     </row>

</xml_diff>

<commit_message>
IMPLEMENTTION OF NEW OBJ WITH ARRAY RIGHT SIDE DEC
</commit_message>
<xml_diff>
--- a/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
+++ b/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\omer\myGitHub\Front-End-Compiler-Project\Mio Language Design\Syntax Analyze Phase\FirstFollowSelectionSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CBEF67-187C-41AE-8EAD-4EB93F2C2708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A9AC6A-49DE-439B-9AAC-81153E4C0CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="508">
   <si>
     <t>&lt;Start&gt;</t>
   </si>
@@ -399,9 +399,6 @@
     <t xml:space="preserve">, ? } </t>
   </si>
   <si>
-    <t>&lt;MUL_ARR_DEC2&gt;</t>
-  </si>
-  <si>
     <t>&lt;EMP_ARR_DEC2&gt;</t>
   </si>
   <si>
@@ -412,9 +409,6 @@
   </si>
   <si>
     <t>&lt;EMP_ARR_DEC&gt;</t>
-  </si>
-  <si>
-    <t>&lt;LEN_OF_ARR2&gt;</t>
   </si>
   <si>
     <t>&lt;EXPR&gt;? ]</t>
@@ -985,10 +979,6 @@
   <si>
     <t>pm ? Parent ? Self ? id ? ( ? typeCast ? not? intConst ? 
 floatConst ? charConst ? boolConst ? strConst ? ]</t>
-  </si>
-  <si>
-    <t>pm ? Parent ? Self ? id ? ( ? typeCast ? not? intConst ? 
-floatConst ? charConst ? boolConst ? strConst ? {  ? }</t>
   </si>
   <si>
     <t>Parent ? Self</t>
@@ -1607,6 +1597,13 @@
   </si>
   <si>
     <t>= ? &lt;LIST_C&gt;</t>
+  </si>
+  <si>
+    <t>, ? ) ? ;</t>
+  </si>
+  <si>
+    <t>pm ? Parent ? Self ? id ?inc_dec( ? typeCast ? not? intConst ? 
+floatConst ? charConst ? boolConst ? strConst ? {  ? }</t>
   </si>
 </sst>
 </file>
@@ -2417,10 +2414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I231"/>
+  <dimension ref="B1:I229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F156" sqref="F156"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F139" sqref="F139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,22 +2441,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H1" s="42" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
@@ -2479,13 +2476,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
@@ -2493,7 +2490,7 @@
         <v>18</v>
       </c>
       <c r="I3" s="45" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2501,23 +2498,23 @@
         <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E4" s="63" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="46" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="I4" s="45" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -2525,23 +2522,23 @@
         <v>6</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E5" s="63" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G5" s="36"/>
       <c r="H5" s="46" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2549,23 +2546,23 @@
         <v>7</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E6" s="63" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G6" s="36"/>
       <c r="H6" s="46" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="I6" s="45" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -2605,22 +2602,22 @@
         <v>8</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E10" s="64" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H10" s="47" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="I10" s="45"/>
     </row>
@@ -2647,20 +2644,20 @@
         <v>9</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="47" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="I13" s="45"/>
     </row>
@@ -2669,23 +2666,23 @@
         <v>10</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E14" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G14" s="36"/>
       <c r="H14" s="47" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="I14" s="45" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -2715,14 +2712,14 @@
         <v>11</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="31"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
       <c r="H17" s="48" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I17" s="45"/>
     </row>
@@ -2785,30 +2782,30 @@
         <v>17</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="31"/>
       <c r="F22" s="36"/>
       <c r="G22" s="36"/>
       <c r="H22" s="48" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I22" s="45"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="31"/>
       <c r="F23" s="36"/>
       <c r="G23" s="36"/>
       <c r="H23" s="48" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I23" s="45"/>
     </row>
@@ -2839,14 +2836,14 @@
         <v>21</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="31"/>
       <c r="F26" s="36"/>
       <c r="G26" s="36"/>
       <c r="H26" s="48" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="I26" s="45"/>
     </row>
@@ -2855,14 +2852,14 @@
         <v>22</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="31"/>
       <c r="F27" s="36"/>
       <c r="G27" s="36"/>
       <c r="H27" s="48" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I27" s="45"/>
     </row>
@@ -2875,10 +2872,10 @@
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="63" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F28" s="36" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G28" s="36"/>
       <c r="H28" s="48" t="s">
@@ -2891,21 +2888,21 @@
         <v>24</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="64" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G29" s="36"/>
       <c r="H29" s="48" t="s">
         <v>26</v>
       </c>
       <c r="I29" s="45" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -2913,14 +2910,14 @@
         <v>25</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="31"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
       <c r="H30" s="48" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="I30" s="45"/>
     </row>
@@ -2936,7 +2933,7 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2955,17 +2952,17 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="63" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F33" s="57" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G33" s="36"/>
       <c r="H33" s="48" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="I33" s="45" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -3047,16 +3044,16 @@
         <v>32</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E40" s="31"/>
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
       <c r="H40" s="48" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="I40" s="45"/>
     </row>
@@ -3078,19 +3075,19 @@
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E42" s="31"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
       <c r="H42" s="48" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I42" s="45"/>
     </row>
@@ -3109,16 +3106,16 @@
         <v>36</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E44" s="31"/>
       <c r="F44" s="36"/>
       <c r="G44" s="36"/>
       <c r="H44" s="48" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I44" s="45"/>
     </row>
@@ -3127,22 +3124,22 @@
         <v>37</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E45" s="63" t="s">
         <v>36</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G45" s="38" t="s">
         <v>35</v>
       </c>
       <c r="H45" s="48" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="I45" s="45" t="s">
         <v>35</v>
@@ -3191,52 +3188,52 @@
         <v>41</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E49" s="31"/>
       <c r="F49" s="36"/>
       <c r="G49" s="36"/>
       <c r="H49" s="48" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I49" s="45"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>42</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E50" s="31"/>
       <c r="F50" s="36"/>
       <c r="G50" s="36"/>
       <c r="H50" s="48" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I50" s="45"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E51" s="31"/>
       <c r="F51" s="36"/>
       <c r="G51" s="36"/>
       <c r="H51" s="48" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I51" s="45"/>
     </row>
@@ -3245,40 +3242,40 @@
         <v>42</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E52" s="31"/>
       <c r="F52" s="36"/>
       <c r="G52" s="36"/>
       <c r="H52" s="48" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I52" s="45"/>
     </row>
     <row r="53" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E53" s="63" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G53" s="38" t="s">
         <v>35</v>
       </c>
       <c r="H53" s="48" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="I53" s="45" t="s">
         <v>35</v>
@@ -3289,14 +3286,14 @@
         <v>43</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="31"/>
       <c r="F54" s="36"/>
       <c r="G54" s="36"/>
       <c r="H54" s="48" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="I54" s="45"/>
     </row>
@@ -3330,13 +3327,13 @@
         <v>52</v>
       </c>
       <c r="D57" s="19" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E57" s="31"/>
       <c r="F57" s="36"/>
       <c r="G57" s="36"/>
       <c r="H57" s="48" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I57" s="45"/>
     </row>
@@ -3345,16 +3342,16 @@
         <v>46</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E58" s="31"/>
       <c r="F58" s="36"/>
       <c r="G58" s="36"/>
       <c r="H58" s="44" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="I58" s="45"/>
     </row>
@@ -3363,14 +3360,14 @@
         <v>47</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="31"/>
       <c r="F59" s="36"/>
       <c r="G59" s="36"/>
       <c r="H59" s="48" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I59" s="45"/>
     </row>
@@ -3383,15 +3380,15 @@
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="32" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F60" s="36"/>
       <c r="G60" s="36"/>
       <c r="H60" s="48" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="I60" s="45" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
@@ -3408,7 +3405,7 @@
       <c r="F61" s="36"/>
       <c r="G61" s="36"/>
       <c r="H61" s="48" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="I61" s="45" t="s">
         <v>35</v>
@@ -3476,13 +3473,13 @@
         <v>59</v>
       </c>
       <c r="D66" s="19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E66" s="31"/>
       <c r="F66" s="36"/>
       <c r="G66" s="36"/>
       <c r="H66" s="48" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I66" s="45"/>
     </row>
@@ -3494,17 +3491,17 @@
         <v>60</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E67" s="63" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F67" s="36" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G67" s="36"/>
       <c r="H67" s="48" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I67" s="45"/>
     </row>
@@ -3513,7 +3510,7 @@
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="63" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="F68" s="36"/>
       <c r="G68" s="36"/>
@@ -3522,7 +3519,7 @@
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -3534,7 +3531,7 @@
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3549,22 +3546,22 @@
         <v>61</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F71" s="58" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="G71" s="39" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="H71" s="46" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="I71" s="49" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="72" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3576,13 +3573,13 @@
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="65" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F72" s="59" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="G72" s="37" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="H72" s="48" t="s">
         <v>26</v>
@@ -3591,26 +3588,26 @@
     </row>
     <row r="73" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D73" s="19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E73" s="63" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F73" s="18" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="G73" s="36"/>
       <c r="H73" s="46" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="I73" s="49" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
@@ -3637,13 +3634,13 @@
         <v>67</v>
       </c>
       <c r="D75" s="21" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E75" s="31"/>
       <c r="F75" s="36"/>
       <c r="G75" s="36"/>
       <c r="H75" s="47" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="I75" s="45"/>
     </row>
@@ -3671,37 +3668,37 @@
         <v>68</v>
       </c>
       <c r="D77" s="20" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E77" s="63" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F77" s="36" t="s">
         <v>38</v>
       </c>
       <c r="G77" s="36"/>
       <c r="H77" s="46" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I77" s="45"/>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C78" s="97" t="s">
+        <v>444</v>
+      </c>
+      <c r="D78" s="19" t="s">
         <v>447</v>
       </c>
-      <c r="D78" s="19" t="s">
-        <v>450</v>
-      </c>
       <c r="E78" s="13" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="F78" s="36"/>
       <c r="G78" s="36"/>
       <c r="H78" s="44" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="I78" s="45"/>
     </row>
@@ -3717,7 +3714,7 @@
     </row>
     <row r="80" spans="2:9" ht="135" x14ac:dyDescent="0.25">
       <c r="B80" s="10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -3732,25 +3729,25 @@
         <v>69</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D81" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E81" s="63" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G81" s="39" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="H81" s="50" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="I81" s="49" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="82" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3758,51 +3755,51 @@
         <v>70</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D82" s="23" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E82" s="63" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G82" s="39" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="H82" s="51" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="I82" s="49" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="83" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C83" s="97" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D83" s="19" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="E83" s="63" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="F83" s="60" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G83" s="39" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="H83" s="48" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="I83" s="49" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
@@ -3844,16 +3841,16 @@
         <v>73</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="E87" s="31"/>
       <c r="F87" s="37"/>
       <c r="G87" s="36"/>
       <c r="H87" s="48" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="I87" s="45"/>
     </row>
@@ -3865,13 +3862,13 @@
         <v>85</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E88" s="31"/>
       <c r="F88" s="36"/>
       <c r="G88" s="36"/>
       <c r="H88" s="48" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="I88" s="45"/>
     </row>
@@ -3890,16 +3887,16 @@
         <v>75</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D90" s="20" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E90" s="33"/>
       <c r="F90" s="36"/>
       <c r="G90" s="36"/>
       <c r="H90" s="46" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="I90" s="45"/>
     </row>
@@ -3908,16 +3905,16 @@
         <v>76</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D91" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E91" s="31"/>
       <c r="F91" s="37"/>
       <c r="G91" s="36"/>
       <c r="H91" s="48" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I91" s="45"/>
     </row>
@@ -3926,16 +3923,16 @@
         <v>77</v>
       </c>
       <c r="C92" s="99" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D92" s="19" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E92" s="31"/>
       <c r="F92" s="36"/>
       <c r="G92" s="36"/>
       <c r="H92" s="44" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I92" s="45"/>
     </row>
@@ -3944,19 +3941,19 @@
         <v>78</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E93" s="64" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F93" s="36" t="s">
         <v>88</v>
       </c>
       <c r="H93" s="47" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="I93" s="45"/>
     </row>
@@ -3968,18 +3965,18 @@
         <v>86</v>
       </c>
       <c r="D94" s="19" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E94" s="32" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F94" s="36"/>
       <c r="G94" s="36"/>
       <c r="H94" s="48" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I94" s="45" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="95" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3987,19 +3984,19 @@
         <v>80</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D95" s="24" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="E95" s="31" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F95" s="36" t="s">
         <v>88</v>
       </c>
       <c r="H95" s="52" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I95" s="45"/>
     </row>
@@ -4008,22 +4005,22 @@
         <v>81</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D96" s="20" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E96" s="63" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="F96" s="17" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G96" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H96" s="98" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="I96" s="45" t="s">
         <v>88</v>
@@ -4034,22 +4031,22 @@
         <v>82</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D97" s="20" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E97" s="63" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G97" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H97" s="98" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="I97" s="45" t="s">
         <v>88</v>
@@ -4057,25 +4054,25 @@
     </row>
     <row r="98" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C98" s="11" t="s">
         <v>87</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E98" s="64" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G98" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H98" s="98" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="I98" s="45" t="s">
         <v>88</v>
@@ -4152,88 +4149,88 @@
         <v>92</v>
       </c>
       <c r="C104" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="D104" s="19" t="s">
         <v>485</v>
-      </c>
-      <c r="D104" s="19" t="s">
-        <v>488</v>
       </c>
       <c r="E104" s="31"/>
       <c r="F104" s="36"/>
       <c r="G104" s="36"/>
       <c r="H104" s="48" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="I104" s="45"/>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E105" s="31"/>
       <c r="F105" s="36"/>
       <c r="G105" s="36"/>
       <c r="H105" s="48" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I105" s="45"/>
     </row>
     <row r="106" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D106" s="19" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="E106" s="31"/>
       <c r="F106" s="36"/>
       <c r="G106" s="36"/>
       <c r="H106" s="48" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="I106" s="45"/>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D107" s="19" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="E107" s="31"/>
       <c r="F107" s="36"/>
       <c r="G107" s="36"/>
       <c r="H107" s="48" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="I107" s="45"/>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C108" s="97" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="E108" s="31"/>
       <c r="F108" s="36"/>
       <c r="G108" s="36"/>
       <c r="H108" s="48" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="I108" s="45"/>
     </row>
@@ -4245,13 +4242,13 @@
         <v>94</v>
       </c>
       <c r="D109" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E109" s="31"/>
       <c r="F109" s="36"/>
       <c r="G109" s="36"/>
       <c r="H109" s="51" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I109" s="45"/>
     </row>
@@ -4286,10 +4283,10 @@
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="31" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F112" s="37" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="G112" s="36"/>
       <c r="H112" s="48" t="s">
@@ -4302,7 +4299,7 @@
         <v>97</v>
       </c>
       <c r="C113" s="70" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="E113" s="31" t="s">
         <v>96</v>
@@ -4310,19 +4307,19 @@
       <c r="F113" s="37"/>
       <c r="G113" s="36"/>
       <c r="H113" s="48" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="I113" s="45"/>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C114" s="11" t="s">
         <v>99</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E114" s="31" t="s">
         <v>97</v>
@@ -4330,7 +4327,7 @@
       <c r="F114" s="37"/>
       <c r="G114" s="36"/>
       <c r="H114" s="48" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I114" s="45"/>
     </row>
@@ -4432,13 +4429,13 @@
         <v>118</v>
       </c>
       <c r="D121" s="78" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E121" s="73"/>
       <c r="F121" s="74"/>
       <c r="G121" s="80"/>
       <c r="H121" s="92" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I121" s="75"/>
     </row>
@@ -4447,14 +4444,14 @@
         <v>106</v>
       </c>
       <c r="C122" s="79" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D122" s="79"/>
       <c r="E122" s="73"/>
       <c r="F122" s="80"/>
       <c r="G122" s="80"/>
       <c r="H122" s="93" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I122" s="75"/>
     </row>
@@ -4466,13 +4463,13 @@
         <v>118</v>
       </c>
       <c r="D123" s="82" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E123" s="73"/>
       <c r="F123" s="80"/>
       <c r="G123" s="80"/>
       <c r="H123" s="94" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I123" s="75"/>
     </row>
@@ -4481,16 +4478,16 @@
         <v>108</v>
       </c>
       <c r="C124" s="83" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D124" s="79" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E124" s="73"/>
       <c r="F124" s="87"/>
       <c r="G124" s="87"/>
       <c r="H124" s="94" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="I124" s="85"/>
     </row>
@@ -4499,7 +4496,7 @@
         <v>109</v>
       </c>
       <c r="C125" s="79" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D125" s="79"/>
       <c r="E125" s="73"/>
@@ -4510,19 +4507,19 @@
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" s="79" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C126" s="81" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D126" s="79" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E126" s="73"/>
       <c r="F126" s="80"/>
       <c r="G126" s="88"/>
       <c r="H126" s="93" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="I126" s="75"/>
     </row>
@@ -4531,16 +4528,16 @@
         <v>110</v>
       </c>
       <c r="C127" s="81" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D127" s="79" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E127" s="73"/>
       <c r="F127" s="87"/>
       <c r="G127" s="80"/>
       <c r="H127" s="93" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="I127" s="75"/>
     </row>
@@ -4549,22 +4546,22 @@
         <v>111</v>
       </c>
       <c r="C128" s="86" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D128" s="87" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E128" s="73"/>
       <c r="F128" s="88"/>
       <c r="G128" s="80"/>
       <c r="H128" s="95" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I128" s="75"/>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" s="79" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C129" s="84" t="s">
         <v>88</v>
@@ -4586,17 +4583,17 @@
         <v>119</v>
       </c>
       <c r="D130" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E130" s="31" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="F130" s="36" t="s">
         <v>97</v>
       </c>
       <c r="G130" s="37"/>
       <c r="H130" s="47" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I130" s="45"/>
     </row>
@@ -4609,60 +4606,60 @@
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C132" s="89" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E132" s="31" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F132" s="96" t="s">
-        <v>417</v>
+        <v>506</v>
       </c>
       <c r="G132" s="36"/>
       <c r="H132" s="44" t="s">
         <v>26</v>
       </c>
       <c r="I132" s="45" t="s">
-        <v>417</v>
+        <v>506</v>
       </c>
     </row>
     <row r="133" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D133" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E133" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F133" s="36"/>
       <c r="G133" s="36"/>
       <c r="H133" s="47" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I133" s="45"/>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C134" s="13" t="s">
         <v>120</v>
       </c>
       <c r="D134" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E134" s="31"/>
       <c r="F134" s="36"/>
       <c r="G134" s="36"/>
       <c r="H134" s="44" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I134" s="45"/>
     </row>
@@ -4671,280 +4668,275 @@
         <v>124</v>
       </c>
       <c r="C135" s="89" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E135" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F135" s="96" t="s">
-        <v>417</v>
+        <v>506</v>
       </c>
       <c r="G135" s="36"/>
       <c r="H135" s="44" t="s">
         <v>26</v>
       </c>
       <c r="I135" s="45" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="136" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
-        <v>129</v>
-      </c>
-      <c r="C136" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="D136" s="21" t="s">
-        <v>316</v>
-      </c>
-      <c r="E136" s="31" t="s">
-        <v>124</v>
-      </c>
+        <v>506</v>
+      </c>
+    </row>
+    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E136" s="31"/>
       <c r="F136" s="36"/>
       <c r="G136" s="36"/>
-      <c r="H136" s="47" t="s">
-        <v>316</v>
-      </c>
+      <c r="H136" s="44"/>
       <c r="I136" s="45"/>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B137" t="s">
-        <v>125</v>
-      </c>
-      <c r="C137" s="89" t="s">
-        <v>413</v>
-      </c>
-      <c r="E137" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="F137" s="96" t="s">
-        <v>417</v>
-      </c>
+      <c r="E137" s="31"/>
+      <c r="F137" s="36"/>
       <c r="G137" s="36"/>
-      <c r="H137" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="I137" s="45" t="s">
-        <v>417</v>
-      </c>
+      <c r="H137" s="44"/>
+      <c r="I137" s="45"/>
     </row>
     <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>113</v>
+      </c>
+      <c r="C138" s="22" t="s">
+        <v>121</v>
+      </c>
       <c r="E138" s="31"/>
       <c r="F138" s="36"/>
       <c r="G138" s="36"/>
-      <c r="H138" s="44"/>
+      <c r="H138" s="44" t="s">
+        <v>121</v>
+      </c>
       <c r="I138" s="45"/>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>114</v>
+      </c>
+      <c r="C139" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D139" s="20" t="s">
+        <v>507</v>
+      </c>
       <c r="E139" s="31"/>
       <c r="F139" s="36"/>
       <c r="G139" s="36"/>
-      <c r="H139" s="44"/>
+      <c r="H139" s="46" t="s">
+        <v>507</v>
+      </c>
       <c r="I139" s="45"/>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C140" s="22" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E140" s="31"/>
       <c r="F140" s="36"/>
-      <c r="G140" s="36"/>
+      <c r="G140" s="40"/>
       <c r="H140" s="44" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I140" s="45"/>
     </row>
-    <row r="141" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B141" t="s">
-        <v>114</v>
-      </c>
-      <c r="C141" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D141" s="20" t="s">
-        <v>317</v>
-      </c>
+    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B141" s="3"/>
       <c r="E141" s="31"/>
       <c r="F141" s="36"/>
       <c r="G141" s="36"/>
-      <c r="H141" s="46" t="s">
-        <v>317</v>
-      </c>
+      <c r="H141" s="44"/>
       <c r="I141" s="45"/>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B142" t="s">
-        <v>115</v>
-      </c>
-      <c r="C142" s="22" t="s">
-        <v>123</v>
+      <c r="B142" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="E142" s="31"/>
       <c r="F142" s="36"/>
-      <c r="G142" s="40"/>
-      <c r="H142" s="44" t="s">
-        <v>123</v>
-      </c>
+      <c r="G142" s="36"/>
+      <c r="H142" s="44"/>
       <c r="I142" s="45"/>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B143" s="3"/>
+      <c r="B143" t="s">
+        <v>130</v>
+      </c>
+      <c r="C143" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D143" s="22" t="s">
+        <v>319</v>
+      </c>
       <c r="E143" s="31"/>
-      <c r="F143" s="36"/>
+      <c r="F143" s="37"/>
       <c r="G143" s="36"/>
-      <c r="H143" s="44"/>
+      <c r="H143" s="44" t="s">
+        <v>319</v>
+      </c>
       <c r="I143" s="45"/>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B144" s="6" t="s">
+      <c r="B144" t="s">
         <v>131</v>
       </c>
+      <c r="C144" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="D144" s="19" t="s">
+        <v>395</v>
+      </c>
       <c r="E144" s="31"/>
-      <c r="F144" s="36"/>
+      <c r="F144" s="37"/>
       <c r="G144" s="36"/>
-      <c r="H144" s="44"/>
+      <c r="H144" s="48" t="s">
+        <v>395</v>
+      </c>
       <c r="I144" s="45"/>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>132</v>
+        <v>388</v>
       </c>
       <c r="C145" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D145" s="22" t="s">
-        <v>322</v>
+        <v>272</v>
+      </c>
+      <c r="D145" s="19" t="s">
+        <v>272</v>
       </c>
       <c r="E145" s="31"/>
       <c r="F145" s="37"/>
       <c r="G145" s="36"/>
-      <c r="H145" s="44" t="s">
-        <v>322</v>
+      <c r="H145" s="48" t="s">
+        <v>272</v>
       </c>
       <c r="I145" s="45"/>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>133</v>
-      </c>
-      <c r="C146" s="13" t="s">
-        <v>390</v>
-      </c>
-      <c r="D146" s="19" t="s">
-        <v>398</v>
+        <v>132</v>
+      </c>
+      <c r="C146" s="69" t="s">
+        <v>433</v>
+      </c>
+      <c r="D146" s="25" t="s">
+        <v>432</v>
       </c>
       <c r="E146" s="31"/>
-      <c r="F146" s="37"/>
+      <c r="F146" s="36"/>
       <c r="G146" s="36"/>
-      <c r="H146" s="48" t="s">
-        <v>398</v>
+      <c r="H146" s="53" t="s">
+        <v>432</v>
       </c>
       <c r="I146" s="45"/>
     </row>
     <row r="147" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>391</v>
-      </c>
-      <c r="C147" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="D147" s="19" t="s">
-        <v>274</v>
+        <v>133</v>
+      </c>
+      <c r="C147" s="22" t="s">
+        <v>134</v>
       </c>
       <c r="E147" s="31"/>
-      <c r="F147" s="37"/>
+      <c r="F147" s="36"/>
       <c r="G147" s="36"/>
-      <c r="H147" s="48" t="s">
-        <v>274</v>
+      <c r="H147" s="44" t="s">
+        <v>134</v>
       </c>
       <c r="I147" s="45"/>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B148" t="s">
-        <v>134</v>
-      </c>
-      <c r="C148" s="69" t="s">
-        <v>436</v>
-      </c>
-      <c r="D148" s="25" t="s">
-        <v>435</v>
-      </c>
       <c r="E148" s="31"/>
       <c r="F148" s="36"/>
       <c r="G148" s="36"/>
-      <c r="H148" s="53" t="s">
-        <v>435</v>
-      </c>
+      <c r="H148" s="44"/>
       <c r="I148" s="45"/>
     </row>
     <row r="149" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B149" t="s">
+      <c r="B149" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="C149" s="22" t="s">
-        <v>136</v>
       </c>
       <c r="E149" s="31"/>
       <c r="F149" s="36"/>
       <c r="G149" s="36"/>
-      <c r="H149" s="44" t="s">
+      <c r="H149" s="44"/>
+      <c r="I149" s="45"/>
+    </row>
+    <row r="150" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
         <v>136</v>
       </c>
-      <c r="I149" s="45"/>
-    </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C150" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D150" s="22" t="s">
+        <v>239</v>
+      </c>
       <c r="E150" s="31"/>
       <c r="F150" s="36"/>
       <c r="G150" s="36"/>
-      <c r="H150" s="44"/>
+      <c r="H150" s="54" t="s">
+        <v>239</v>
+      </c>
       <c r="I150" s="45"/>
     </row>
     <row r="151" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B151" s="6" t="s">
+      <c r="B151" t="s">
         <v>137</v>
+      </c>
+      <c r="C151" s="26" t="s">
+        <v>415</v>
+      </c>
+      <c r="D151" s="22" t="s">
+        <v>417</v>
       </c>
       <c r="E151" s="31"/>
       <c r="F151" s="36"/>
       <c r="G151" s="36"/>
-      <c r="H151" s="44"/>
+      <c r="H151" s="44" t="s">
+        <v>141</v>
+      </c>
       <c r="I151" s="45"/>
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>138</v>
-      </c>
-      <c r="C152" s="13" t="s">
-        <v>238</v>
+        <v>416</v>
+      </c>
+      <c r="C152" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="D152" s="22" t="s">
-        <v>241</v>
+        <v>319</v>
       </c>
       <c r="E152" s="31"/>
       <c r="F152" s="36"/>
       <c r="G152" s="36"/>
-      <c r="H152" s="54" t="s">
-        <v>241</v>
+      <c r="H152" s="44" t="s">
+        <v>225</v>
       </c>
       <c r="I152" s="45"/>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>139</v>
-      </c>
-      <c r="C153" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C153" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="D153" s="22" t="s">
-        <v>420</v>
+      <c r="D153" s="28" t="s">
+        <v>327</v>
       </c>
       <c r="E153" s="31"/>
       <c r="F153" s="36"/>
       <c r="G153" s="36"/>
       <c r="H153" s="44" t="s">
-        <v>143</v>
+        <v>327</v>
       </c>
       <c r="I153" s="45"/>
     </row>
@@ -4952,103 +4944,110 @@
       <c r="B154" t="s">
         <v>419</v>
       </c>
-      <c r="C154" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D154" s="22" t="s">
-        <v>322</v>
+      <c r="C154" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="D154" s="28" t="s">
+        <v>389</v>
       </c>
       <c r="E154" s="31"/>
       <c r="F154" s="36"/>
       <c r="G154" s="36"/>
-      <c r="H154" s="44" t="s">
-        <v>227</v>
-      </c>
+      <c r="H154" s="44"/>
       <c r="I154" s="45"/>
     </row>
     <row r="155" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>140</v>
-      </c>
-      <c r="C155" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="D155" s="28" t="s">
-        <v>330</v>
+        <v>139</v>
+      </c>
+      <c r="C155" s="69" t="s">
+        <v>505</v>
+      </c>
+      <c r="D155" s="25" t="s">
+        <v>432</v>
       </c>
       <c r="E155" s="31"/>
       <c r="F155" s="36"/>
       <c r="G155" s="36"/>
-      <c r="H155" s="44" t="s">
-        <v>330</v>
+      <c r="H155" s="53" t="s">
+        <v>432</v>
       </c>
       <c r="I155" s="45"/>
     </row>
     <row r="156" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>422</v>
-      </c>
-      <c r="C156" s="13" t="s">
-        <v>423</v>
-      </c>
-      <c r="D156" s="28" t="s">
-        <v>392</v>
+        <v>140</v>
+      </c>
+      <c r="C156" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="E156" s="31"/>
       <c r="F156" s="36"/>
       <c r="G156" s="36"/>
-      <c r="H156" s="44"/>
+      <c r="H156" s="44" t="s">
+        <v>142</v>
+      </c>
       <c r="I156" s="45"/>
     </row>
     <row r="157" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B157" t="s">
-        <v>141</v>
-      </c>
-      <c r="C157" s="69" t="s">
-        <v>508</v>
-      </c>
-      <c r="D157" s="25" t="s">
-        <v>435</v>
-      </c>
       <c r="E157" s="31"/>
       <c r="F157" s="36"/>
       <c r="G157" s="36"/>
-      <c r="H157" s="53" t="s">
-        <v>435</v>
-      </c>
+      <c r="H157" s="44"/>
       <c r="I157" s="45"/>
     </row>
     <row r="158" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B158" t="s">
-        <v>142</v>
-      </c>
-      <c r="C158" s="22" t="s">
-        <v>144</v>
+      <c r="B158" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="E158" s="31"/>
       <c r="F158" s="36"/>
       <c r="G158" s="36"/>
-      <c r="H158" s="44" t="s">
+      <c r="H158" s="44"/>
+      <c r="I158" s="45"/>
+    </row>
+    <row r="159" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
         <v>144</v>
       </c>
-      <c r="I158" s="45"/>
-    </row>
-    <row r="159" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E159" s="31"/>
-      <c r="F159" s="36"/>
+      <c r="C159" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D159" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="E159" s="63" t="s">
+        <v>276</v>
+      </c>
+      <c r="F159" s="36" t="s">
+        <v>355</v>
+      </c>
       <c r="G159" s="36"/>
-      <c r="H159" s="44"/>
+      <c r="H159" s="46" t="s">
+        <v>477</v>
+      </c>
       <c r="I159" s="45"/>
     </row>
     <row r="160" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B160" s="6" t="s">
+      <c r="B160" t="s">
         <v>145</v>
       </c>
-      <c r="E160" s="31"/>
-      <c r="F160" s="36"/>
+      <c r="C160" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="E160" s="63" t="s">
+        <v>403</v>
+      </c>
+      <c r="F160" s="39" t="s">
+        <v>355</v>
+      </c>
       <c r="G160" s="36"/>
-      <c r="H160" s="44"/>
-      <c r="I160" s="45"/>
+      <c r="H160" s="44" t="s">
+        <v>356</v>
+      </c>
+      <c r="I160" s="45" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="161" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
@@ -5058,17 +5057,17 @@
         <v>148</v>
       </c>
       <c r="D161" s="20" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E161" s="63" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F161" s="36" t="s">
-        <v>358</v>
+        <v>285</v>
       </c>
       <c r="G161" s="36"/>
       <c r="H161" s="46" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I161" s="45"/>
     </row>
@@ -5076,21 +5075,23 @@
       <c r="B162" t="s">
         <v>147</v>
       </c>
-      <c r="C162" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="E162" s="63" t="s">
-        <v>406</v>
-      </c>
-      <c r="F162" s="39" t="s">
-        <v>358</v>
-      </c>
-      <c r="G162" s="36"/>
+      <c r="C162" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="E162" s="66" t="s">
+        <v>495</v>
+      </c>
+      <c r="F162" s="58" t="s">
+        <v>278</v>
+      </c>
+      <c r="G162" s="38" t="s">
+        <v>285</v>
+      </c>
       <c r="H162" s="44" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="I162" s="45" t="s">
-        <v>358</v>
+        <v>285</v>
       </c>
     </row>
     <row r="163" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -5101,17 +5102,17 @@
         <v>150</v>
       </c>
       <c r="D163" s="20" t="s">
-        <v>480</v>
-      </c>
-      <c r="E163" s="63" t="s">
-        <v>282</v>
+        <v>477</v>
+      </c>
+      <c r="E163" s="67" t="s">
+        <v>279</v>
       </c>
       <c r="F163" s="36" t="s">
-        <v>287</v>
+        <v>331</v>
       </c>
       <c r="G163" s="36"/>
       <c r="H163" s="46" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I163" s="45"/>
     </row>
@@ -5119,23 +5120,23 @@
       <c r="B164" t="s">
         <v>149</v>
       </c>
-      <c r="C164" s="28" t="s">
+      <c r="C164" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="E164" s="66" t="s">
+        <v>496</v>
+      </c>
+      <c r="F164" s="58" t="s">
+        <v>332</v>
+      </c>
+      <c r="G164" s="38" t="s">
         <v>333</v>
       </c>
-      <c r="E164" s="66" t="s">
-        <v>498</v>
-      </c>
-      <c r="F164" s="58" t="s">
-        <v>280</v>
-      </c>
-      <c r="G164" s="38" t="s">
-        <v>287</v>
-      </c>
       <c r="H164" s="44" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I164" s="45" t="s">
-        <v>287</v>
+        <v>359</v>
       </c>
     </row>
     <row r="165" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -5146,41 +5147,41 @@
         <v>152</v>
       </c>
       <c r="D165" s="20" t="s">
-        <v>480</v>
-      </c>
-      <c r="E165" s="67" t="s">
+        <v>477</v>
+      </c>
+      <c r="E165" s="63" t="s">
         <v>281</v>
       </c>
       <c r="F165" s="36" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="G165" s="36"/>
       <c r="H165" s="46" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I165" s="45"/>
     </row>
-    <row r="166" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>151</v>
       </c>
       <c r="C166" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E166" s="65" t="s">
+        <v>497</v>
+      </c>
+      <c r="F166" s="58" t="s">
         <v>337</v>
       </c>
-      <c r="E166" s="66" t="s">
-        <v>499</v>
-      </c>
-      <c r="F166" s="58" t="s">
+      <c r="G166" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="G166" s="38" t="s">
-        <v>336</v>
-      </c>
       <c r="H166" s="44" t="s">
+        <v>360</v>
+      </c>
+      <c r="I166" s="45" t="s">
         <v>361</v>
-      </c>
-      <c r="I166" s="45" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="167" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -5188,44 +5189,44 @@
         <v>152</v>
       </c>
       <c r="C167" s="13" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D167" s="20" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E167" s="63" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F167" s="36" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G167" s="36"/>
       <c r="H167" s="46" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I167" s="45"/>
     </row>
-    <row r="168" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>153</v>
       </c>
       <c r="C168" s="22" t="s">
-        <v>160</v>
+        <v>298</v>
       </c>
       <c r="E168" s="65" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="F168" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="G168" s="39" t="s">
         <v>340</v>
       </c>
-      <c r="G168" s="38" t="s">
-        <v>338</v>
-      </c>
-      <c r="H168" s="44" t="s">
+      <c r="H168" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="I168" s="49" t="s">
         <v>363</v>
-      </c>
-      <c r="I168" s="45" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="169" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -5233,10 +5234,10 @@
         <v>154</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D169" s="20" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E169" s="63" t="s">
         <v>284</v>
@@ -5246,19 +5247,19 @@
       </c>
       <c r="G169" s="36"/>
       <c r="H169" s="46" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I169" s="45"/>
     </row>
-    <row r="170" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>155</v>
+        <v>87</v>
       </c>
       <c r="C170" s="22" t="s">
-        <v>300</v>
+        <v>160</v>
       </c>
       <c r="E170" s="65" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F170" s="58" t="s">
         <v>342</v>
@@ -5266,302 +5267,290 @@
       <c r="G170" s="39" t="s">
         <v>343</v>
       </c>
-      <c r="H170" s="47" t="s">
-        <v>365</v>
+      <c r="H170" s="44" t="s">
+        <v>364</v>
       </c>
       <c r="I170" s="49" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="171" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
+        <v>155</v>
+      </c>
+      <c r="C171" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="C171" s="13" t="s">
-        <v>157</v>
-      </c>
       <c r="D171" s="20" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E171" s="63" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F171" s="36" t="s">
         <v>344</v>
       </c>
       <c r="G171" s="36"/>
       <c r="H171" s="46" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I171" s="45"/>
     </row>
-    <row r="172" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>87</v>
-      </c>
-      <c r="C172" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C172" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D172" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="E172" s="68" t="s">
+        <v>155</v>
+      </c>
+      <c r="F172" s="36" t="s">
+        <v>344</v>
+      </c>
+      <c r="G172" s="36"/>
+      <c r="H172" s="46" t="s">
+        <v>477</v>
+      </c>
+      <c r="I172" s="45"/>
+    </row>
+    <row r="173" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E173" s="31"/>
+      <c r="F173" s="36"/>
+      <c r="G173" s="36"/>
+      <c r="H173" s="44"/>
+      <c r="I173" s="45"/>
+    </row>
+    <row r="174" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B174" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="E172" s="65" t="s">
-        <v>502</v>
-      </c>
-      <c r="F172" s="58" t="s">
-        <v>345</v>
-      </c>
-      <c r="G172" s="39" t="s">
-        <v>346</v>
-      </c>
-      <c r="H172" s="44" t="s">
-        <v>367</v>
-      </c>
-      <c r="I172" s="49" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="173" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B173" t="s">
-        <v>157</v>
-      </c>
-      <c r="C173" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="D173" s="20" t="s">
-        <v>480</v>
-      </c>
-      <c r="E173" s="63" t="s">
-        <v>285</v>
-      </c>
-      <c r="F173" s="36" t="s">
-        <v>347</v>
-      </c>
-      <c r="G173" s="36"/>
-      <c r="H173" s="46" t="s">
-        <v>480</v>
-      </c>
-      <c r="I173" s="45"/>
-    </row>
-    <row r="174" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B174" t="s">
-        <v>158</v>
-      </c>
-      <c r="C174" s="13" t="s">
+      <c r="E174" s="31"/>
+      <c r="F174" s="36"/>
+      <c r="G174" s="36"/>
+      <c r="H174" s="44"/>
+      <c r="I174" s="45"/>
+    </row>
+    <row r="175" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B175" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="C175" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="D175" s="20" t="s">
+        <v>476</v>
+      </c>
+      <c r="E175" s="63" t="s">
+        <v>460</v>
+      </c>
+      <c r="F175" s="61" t="s">
+        <v>461</v>
+      </c>
+      <c r="G175" s="37" t="s">
+        <v>329</v>
+      </c>
+      <c r="H175" s="46" t="s">
+        <v>477</v>
+      </c>
+      <c r="I175" s="45"/>
+    </row>
+    <row r="176" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
         <v>163</v>
       </c>
-      <c r="D174" s="20" t="s">
-        <v>480</v>
-      </c>
-      <c r="E174" s="68" t="s">
-        <v>157</v>
-      </c>
-      <c r="F174" s="36" t="s">
-        <v>347</v>
-      </c>
-      <c r="G174" s="36"/>
-      <c r="H174" s="46" t="s">
-        <v>480</v>
-      </c>
-      <c r="I174" s="45"/>
-    </row>
-    <row r="175" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E175" s="31"/>
-      <c r="F175" s="36"/>
-      <c r="G175" s="36"/>
-      <c r="H175" s="44"/>
-      <c r="I175" s="45"/>
-    </row>
-    <row r="176" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B176" s="6" t="s">
-        <v>164</v>
+      <c r="C176" s="22" t="s">
+        <v>165</v>
       </c>
       <c r="E176" s="31"/>
       <c r="F176" s="36"/>
       <c r="G176" s="36"/>
-      <c r="H176" s="44"/>
+      <c r="H176" s="44" t="s">
+        <v>165</v>
+      </c>
       <c r="I176" s="45"/>
     </row>
-    <row r="177" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B177" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="C177" s="14" t="s">
-        <v>441</v>
-      </c>
-      <c r="D177" s="20" t="s">
-        <v>479</v>
-      </c>
-      <c r="E177" s="63" t="s">
-        <v>463</v>
-      </c>
-      <c r="F177" s="61" t="s">
-        <v>464</v>
-      </c>
-      <c r="G177" s="37" t="s">
-        <v>332</v>
-      </c>
-      <c r="H177" s="46" t="s">
-        <v>480</v>
+    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
+        <v>164</v>
+      </c>
+      <c r="C177" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="E177" s="31"/>
+      <c r="F177" s="36"/>
+      <c r="G177" s="36"/>
+      <c r="H177" s="44" t="s">
+        <v>166</v>
       </c>
       <c r="I177" s="45"/>
     </row>
     <row r="178" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B178" t="s">
-        <v>165</v>
-      </c>
-      <c r="C178" s="22" t="s">
-        <v>167</v>
-      </c>
       <c r="E178" s="31"/>
       <c r="F178" s="36"/>
       <c r="G178" s="36"/>
-      <c r="H178" s="44" t="s">
-        <v>167</v>
-      </c>
+      <c r="H178" s="44"/>
       <c r="I178" s="45"/>
     </row>
     <row r="179" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
-        <v>166</v>
-      </c>
-      <c r="C179" s="22" t="s">
-        <v>168</v>
+      <c r="B179" s="6" t="s">
+        <v>241</v>
       </c>
       <c r="E179" s="31"/>
       <c r="F179" s="36"/>
       <c r="G179" s="36"/>
-      <c r="H179" s="44" t="s">
+      <c r="H179" s="44"/>
+      <c r="I179" s="45"/>
+    </row>
+    <row r="180" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B180" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C180" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="I179" s="45"/>
-    </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E180" s="31"/>
       <c r="F180" s="36"/>
       <c r="G180" s="36"/>
-      <c r="H180" s="44"/>
+      <c r="H180" s="47" t="s">
+        <v>168</v>
+      </c>
       <c r="I180" s="45"/>
     </row>
     <row r="181" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B181" s="6" t="s">
-        <v>243</v>
+      <c r="B181" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C181" s="24" t="s">
+        <v>254</v>
       </c>
       <c r="E181" s="31"/>
       <c r="F181" s="36"/>
       <c r="G181" s="36"/>
-      <c r="H181" s="44"/>
+      <c r="H181" s="52" t="s">
+        <v>254</v>
+      </c>
       <c r="I181" s="45"/>
     </row>
-    <row r="182" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B182" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C182" s="21" t="s">
-        <v>170</v>
-      </c>
+    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E182" s="31"/>
       <c r="F182" s="36"/>
       <c r="G182" s="36"/>
-      <c r="H182" s="47" t="s">
-        <v>170</v>
-      </c>
+      <c r="H182" s="44"/>
       <c r="I182" s="45"/>
     </row>
     <row r="183" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B183" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C183" s="24" t="s">
-        <v>256</v>
+      <c r="B183" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="E183" s="31"/>
       <c r="F183" s="36"/>
       <c r="G183" s="36"/>
-      <c r="H183" s="52" t="s">
-        <v>256</v>
-      </c>
+      <c r="H183" s="44"/>
       <c r="I183" s="45"/>
     </row>
     <row r="184" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B184" s="8" t="s">
+        <v>174</v>
+      </c>
       <c r="E184" s="31"/>
       <c r="F184" s="36"/>
       <c r="G184" s="36"/>
       <c r="H184" s="44"/>
       <c r="I184" s="45"/>
     </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B185" s="6" t="s">
+    <row r="185" spans="2:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B185" t="s">
+        <v>170</v>
+      </c>
+      <c r="C185" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="E185" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F185" s="37" t="s">
+        <v>429</v>
+      </c>
+      <c r="G185" s="36"/>
+      <c r="H185" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="I185" s="45"/>
+    </row>
+    <row r="186" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="B186" t="s">
         <v>171</v>
       </c>
-      <c r="E185" s="31"/>
-      <c r="F185" s="36"/>
-      <c r="G185" s="36"/>
-      <c r="H185" s="44"/>
-      <c r="I185" s="45"/>
-    </row>
-    <row r="186" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B186" s="8" t="s">
+      <c r="C186" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="E186" s="63" t="s">
+        <v>170</v>
+      </c>
+      <c r="F186" s="39" t="s">
+        <v>429</v>
+      </c>
+      <c r="G186" s="36"/>
+      <c r="H186" s="44" t="s">
+        <v>365</v>
+      </c>
+      <c r="I186" s="49" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="187" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E187" s="31"/>
+      <c r="F187" s="36"/>
+      <c r="G187" s="36"/>
+      <c r="H187" s="44"/>
+      <c r="I187" s="45"/>
+    </row>
+    <row r="188" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B188" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E188" s="31"/>
+      <c r="F188" s="36"/>
+      <c r="G188" s="36"/>
+      <c r="H188" s="44"/>
+      <c r="I188" s="45"/>
+    </row>
+    <row r="189" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
         <v>176</v>
       </c>
-      <c r="E186" s="31"/>
-      <c r="F186" s="36"/>
-      <c r="G186" s="36"/>
-      <c r="H186" s="44"/>
-      <c r="I186" s="45"/>
-    </row>
-    <row r="187" spans="2:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B187" t="s">
-        <v>172</v>
-      </c>
-      <c r="C187" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="E187" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="F187" s="37" t="s">
-        <v>432</v>
-      </c>
-      <c r="G187" s="36"/>
-      <c r="H187" s="44" t="s">
-        <v>174</v>
-      </c>
-      <c r="I187" s="45"/>
-    </row>
-    <row r="188" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B188" t="s">
-        <v>173</v>
-      </c>
-      <c r="C188" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="E188" s="63" t="s">
-        <v>172</v>
-      </c>
-      <c r="F188" s="39" t="s">
-        <v>432</v>
-      </c>
-      <c r="G188" s="36"/>
-      <c r="H188" s="44" t="s">
-        <v>368</v>
-      </c>
-      <c r="I188" s="49" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="189" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C189" s="22" t="s">
+        <v>179</v>
+      </c>
       <c r="E189" s="31"/>
       <c r="F189" s="36"/>
       <c r="G189" s="36"/>
-      <c r="H189" s="44"/>
+      <c r="H189" s="44" t="s">
+        <v>179</v>
+      </c>
       <c r="I189" s="45"/>
     </row>
     <row r="190" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B190" s="8" t="s">
+      <c r="B190" t="s">
         <v>177</v>
+      </c>
+      <c r="C190" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="D190" s="22" t="s">
+        <v>242</v>
       </c>
       <c r="E190" s="31"/>
       <c r="F190" s="36"/>
       <c r="G190" s="36"/>
-      <c r="H190" s="44"/>
+      <c r="H190" s="44" t="s">
+        <v>242</v>
+      </c>
       <c r="I190" s="45"/>
     </row>
     <row r="191" spans="2:9" x14ac:dyDescent="0.25">
@@ -5569,65 +5558,49 @@
         <v>178</v>
       </c>
       <c r="C191" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E191" s="31"/>
       <c r="F191" s="36"/>
       <c r="G191" s="36"/>
       <c r="H191" s="44" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I191" s="45"/>
     </row>
-    <row r="192" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>179</v>
+        <v>260</v>
       </c>
       <c r="C192" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="D192" s="22" t="s">
-        <v>244</v>
+        <v>431</v>
+      </c>
+      <c r="D192" s="21" t="s">
+        <v>407</v>
       </c>
       <c r="E192" s="31"/>
       <c r="F192" s="36"/>
       <c r="G192" s="36"/>
-      <c r="H192" s="44" t="s">
-        <v>244</v>
+      <c r="H192" s="47" t="s">
+        <v>318</v>
       </c>
       <c r="I192" s="45"/>
     </row>
     <row r="193" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
-        <v>180</v>
-      </c>
-      <c r="C193" s="22" t="s">
-        <v>182</v>
-      </c>
       <c r="E193" s="31"/>
       <c r="F193" s="36"/>
       <c r="G193" s="36"/>
-      <c r="H193" s="44" t="s">
+      <c r="H193" s="44"/>
+      <c r="I193" s="45"/>
+    </row>
+    <row r="194" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B194" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="I193" s="45"/>
-    </row>
-    <row r="194" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B194" t="s">
-        <v>262</v>
-      </c>
-      <c r="C194" s="13" t="s">
-        <v>434</v>
-      </c>
-      <c r="D194" s="21" t="s">
-        <v>410</v>
       </c>
       <c r="E194" s="31"/>
       <c r="F194" s="36"/>
       <c r="G194" s="36"/>
-      <c r="H194" s="47" t="s">
-        <v>321</v>
-      </c>
+      <c r="H194" s="44"/>
       <c r="I194" s="45"/>
     </row>
     <row r="195" spans="2:9" x14ac:dyDescent="0.25">
@@ -5638,8 +5611,8 @@
       <c r="I195" s="45"/>
     </row>
     <row r="196" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B196" s="6" t="s">
-        <v>184</v>
+      <c r="B196" s="8" t="s">
+        <v>183</v>
       </c>
       <c r="E196" s="31"/>
       <c r="F196" s="36"/>
@@ -5648,200 +5621,201 @@
       <c r="I196" s="45"/>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B197" t="s">
+        <v>185</v>
+      </c>
+      <c r="C197" s="22" t="s">
+        <v>187</v>
+      </c>
       <c r="E197" s="31"/>
       <c r="F197" s="36"/>
       <c r="G197" s="36"/>
-      <c r="H197" s="44"/>
+      <c r="H197" s="44" t="s">
+        <v>187</v>
+      </c>
       <c r="I197" s="45"/>
     </row>
     <row r="198" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B198" s="8" t="s">
-        <v>185</v>
+      <c r="B198" t="s">
+        <v>186</v>
+      </c>
+      <c r="C198" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D198" s="22" t="s">
+        <v>243</v>
       </c>
       <c r="E198" s="31"/>
       <c r="F198" s="36"/>
       <c r="G198" s="36"/>
-      <c r="H198" s="44"/>
+      <c r="H198" s="44" t="s">
+        <v>243</v>
+      </c>
       <c r="I198" s="45"/>
     </row>
     <row r="199" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
-        <v>187</v>
-      </c>
-      <c r="C199" s="22" t="s">
-        <v>189</v>
-      </c>
       <c r="E199" s="31"/>
       <c r="F199" s="36"/>
       <c r="G199" s="36"/>
-      <c r="H199" s="44" t="s">
-        <v>189</v>
-      </c>
+      <c r="H199" s="44"/>
       <c r="I199" s="45"/>
     </row>
     <row r="200" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B200" t="s">
-        <v>188</v>
-      </c>
-      <c r="C200" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="D200" s="22" t="s">
-        <v>245</v>
+      <c r="B200" s="8" t="s">
+        <v>184</v>
       </c>
       <c r="E200" s="31"/>
       <c r="F200" s="36"/>
       <c r="G200" s="36"/>
-      <c r="H200" s="44" t="s">
-        <v>245</v>
-      </c>
+      <c r="H200" s="44"/>
       <c r="I200" s="45"/>
     </row>
     <row r="201" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
+        <v>189</v>
+      </c>
+      <c r="C201" s="22" t="s">
+        <v>191</v>
+      </c>
       <c r="E201" s="31"/>
       <c r="F201" s="36"/>
       <c r="G201" s="36"/>
-      <c r="H201" s="44"/>
+      <c r="H201" s="44" t="s">
+        <v>191</v>
+      </c>
       <c r="I201" s="45"/>
     </row>
     <row r="202" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B202" s="8" t="s">
-        <v>186</v>
+      <c r="B202" t="s">
+        <v>190</v>
+      </c>
+      <c r="C202" s="22" t="s">
+        <v>192</v>
       </c>
       <c r="E202" s="31"/>
       <c r="F202" s="36"/>
       <c r="G202" s="36"/>
-      <c r="H202" s="44"/>
+      <c r="H202" s="44" t="s">
+        <v>192</v>
+      </c>
       <c r="I202" s="45"/>
     </row>
     <row r="203" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B203" t="s">
-        <v>191</v>
-      </c>
-      <c r="C203" s="22" t="s">
-        <v>193</v>
-      </c>
       <c r="E203" s="31"/>
       <c r="F203" s="36"/>
       <c r="G203" s="36"/>
-      <c r="H203" s="44" t="s">
+      <c r="H203" s="44"/>
+      <c r="I203" s="45"/>
+    </row>
+    <row r="204" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B204" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="I203" s="45"/>
-    </row>
-    <row r="204" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B204" t="s">
-        <v>192</v>
-      </c>
-      <c r="C204" s="22" t="s">
-        <v>194</v>
       </c>
       <c r="E204" s="31"/>
       <c r="F204" s="36"/>
       <c r="G204" s="36"/>
-      <c r="H204" s="44" t="s">
+      <c r="H204" s="44"/>
+      <c r="I204" s="45"/>
+    </row>
+    <row r="205" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
         <v>194</v>
       </c>
-      <c r="I204" s="45"/>
-    </row>
-    <row r="205" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C205" s="22" t="s">
+        <v>197</v>
+      </c>
       <c r="E205" s="31"/>
       <c r="F205" s="36"/>
       <c r="G205" s="36"/>
-      <c r="H205" s="44"/>
+      <c r="H205" s="44" t="s">
+        <v>197</v>
+      </c>
       <c r="I205" s="45"/>
     </row>
     <row r="206" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B206" s="8" t="s">
+      <c r="B206" t="s">
         <v>195</v>
       </c>
-      <c r="E206" s="31"/>
+      <c r="C206" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="E206" s="31" t="s">
+        <v>295</v>
+      </c>
       <c r="F206" s="36"/>
       <c r="G206" s="36"/>
-      <c r="H206" s="44"/>
+      <c r="H206" s="44" t="s">
+        <v>198</v>
+      </c>
       <c r="I206" s="45"/>
     </row>
-    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
         <v>196</v>
       </c>
-      <c r="C207" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="E207" s="31"/>
-      <c r="F207" s="36"/>
+      <c r="C207" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="D207" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="E207" s="63" t="s">
+        <v>397</v>
+      </c>
+      <c r="F207" s="38" t="s">
+        <v>295</v>
+      </c>
       <c r="G207" s="36"/>
       <c r="H207" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="I207" s="45"/>
+        <v>366</v>
+      </c>
+      <c r="I207" s="45" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="208" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>197</v>
-      </c>
-      <c r="C208" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="E208" s="31" t="s">
-        <v>297</v>
-      </c>
-      <c r="F208" s="36"/>
+        <v>396</v>
+      </c>
+      <c r="C208" s="26" t="s">
+        <v>456</v>
+      </c>
+      <c r="D208" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="E208" s="63" t="s">
+        <v>196</v>
+      </c>
+      <c r="F208" s="38" t="s">
+        <v>295</v>
+      </c>
       <c r="G208" s="36"/>
       <c r="H208" s="44" t="s">
-        <v>200</v>
-      </c>
-      <c r="I208" s="45"/>
-    </row>
-    <row r="209" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B209" t="s">
-        <v>198</v>
-      </c>
-      <c r="C209" s="14" t="s">
-        <v>460</v>
-      </c>
-      <c r="D209" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="E209" s="63" t="s">
-        <v>400</v>
-      </c>
-      <c r="F209" s="38" t="s">
-        <v>297</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="I208" s="45" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="209" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E209" s="31"/>
+      <c r="F209" s="36"/>
       <c r="G209" s="36"/>
-      <c r="H209" s="44" t="s">
-        <v>369</v>
-      </c>
-      <c r="I209" s="45" t="s">
-        <v>297</v>
-      </c>
+      <c r="H209" s="44"/>
+      <c r="I209" s="45"/>
     </row>
     <row r="210" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B210" t="s">
-        <v>399</v>
-      </c>
-      <c r="C210" s="26" t="s">
-        <v>459</v>
-      </c>
-      <c r="D210" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="E210" s="63" t="s">
-        <v>198</v>
-      </c>
-      <c r="F210" s="38" t="s">
-        <v>297</v>
-      </c>
+      <c r="B210" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E210" s="31"/>
+      <c r="F210" s="36"/>
       <c r="G210" s="36"/>
-      <c r="H210" s="44" t="s">
-        <v>369</v>
-      </c>
-      <c r="I210" s="45" t="s">
-        <v>297</v>
-      </c>
+      <c r="H210" s="44"/>
+      <c r="I210" s="45"/>
     </row>
     <row r="211" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B211" s="4"/>
       <c r="E211" s="31"/>
       <c r="F211" s="36"/>
       <c r="G211" s="36"/>
@@ -5849,8 +5823,8 @@
       <c r="I211" s="45"/>
     </row>
     <row r="212" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B212" s="6" t="s">
-        <v>201</v>
+      <c r="B212" s="8" t="s">
+        <v>200</v>
       </c>
       <c r="E212" s="31"/>
       <c r="F212" s="36"/>
@@ -5859,21 +5833,33 @@
       <c r="I212" s="45"/>
     </row>
     <row r="213" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B213" s="4"/>
+      <c r="B213" t="s">
+        <v>202</v>
+      </c>
+      <c r="C213" s="22" t="s">
+        <v>205</v>
+      </c>
       <c r="E213" s="31"/>
       <c r="F213" s="36"/>
       <c r="G213" s="36"/>
-      <c r="H213" s="44"/>
+      <c r="H213" s="44" t="s">
+        <v>205</v>
+      </c>
       <c r="I213" s="45"/>
     </row>
     <row r="214" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B214" s="8" t="s">
-        <v>202</v>
+      <c r="B214" t="s">
+        <v>203</v>
+      </c>
+      <c r="C214" s="28" t="s">
+        <v>317</v>
       </c>
       <c r="E214" s="31"/>
       <c r="F214" s="36"/>
       <c r="G214" s="36"/>
-      <c r="H214" s="44"/>
+      <c r="H214" s="44" t="s">
+        <v>317</v>
+      </c>
       <c r="I214" s="45"/>
     </row>
     <row r="215" spans="2:9" x14ac:dyDescent="0.25">
@@ -5881,57 +5867,49 @@
         <v>204</v>
       </c>
       <c r="C215" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E215" s="31"/>
       <c r="F215" s="36"/>
       <c r="G215" s="36"/>
       <c r="H215" s="44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I215" s="45"/>
     </row>
     <row r="216" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B216" t="s">
-        <v>205</v>
-      </c>
-      <c r="C216" s="28" t="s">
-        <v>320</v>
-      </c>
       <c r="E216" s="31"/>
       <c r="F216" s="36"/>
       <c r="G216" s="36"/>
-      <c r="H216" s="44" t="s">
-        <v>320</v>
-      </c>
+      <c r="H216" s="44"/>
       <c r="I216" s="45"/>
     </row>
     <row r="217" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B217" t="s">
-        <v>206</v>
-      </c>
-      <c r="C217" s="22" t="s">
-        <v>208</v>
+      <c r="B217" s="8" t="s">
+        <v>201</v>
       </c>
       <c r="E217" s="31"/>
       <c r="F217" s="36"/>
       <c r="G217" s="36"/>
-      <c r="H217" s="44" t="s">
-        <v>208</v>
-      </c>
+      <c r="H217" s="44"/>
       <c r="I217" s="45"/>
     </row>
     <row r="218" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>207</v>
+      </c>
+      <c r="C218" s="28" t="s">
+        <v>316</v>
+      </c>
       <c r="E218" s="31"/>
       <c r="F218" s="36"/>
       <c r="G218" s="36"/>
-      <c r="H218" s="44"/>
+      <c r="H218" s="44" t="s">
+        <v>316</v>
+      </c>
       <c r="I218" s="45"/>
     </row>
     <row r="219" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B219" s="8" t="s">
-        <v>203</v>
-      </c>
       <c r="E219" s="31"/>
       <c r="F219" s="36"/>
       <c r="G219" s="36"/>
@@ -5939,31 +5917,31 @@
       <c r="I219" s="45"/>
     </row>
     <row r="220" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B220" t="s">
-        <v>209</v>
-      </c>
-      <c r="C220" s="28" t="s">
-        <v>319</v>
+      <c r="B220" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="E220" s="31"/>
       <c r="F220" s="36"/>
       <c r="G220" s="36"/>
-      <c r="H220" s="44" t="s">
-        <v>319</v>
-      </c>
+      <c r="H220" s="44"/>
       <c r="I220" s="45"/>
     </row>
     <row r="221" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
+        <v>209</v>
+      </c>
+      <c r="C221" s="22" t="s">
+        <v>210</v>
+      </c>
       <c r="E221" s="31"/>
-      <c r="F221" s="36"/>
+      <c r="F221" s="37"/>
       <c r="G221" s="36"/>
-      <c r="H221" s="44"/>
+      <c r="H221" s="44" t="s">
+        <v>210</v>
+      </c>
       <c r="I221" s="45"/>
     </row>
     <row r="222" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B222" s="6" t="s">
-        <v>210</v>
-      </c>
       <c r="E222" s="31"/>
       <c r="F222" s="36"/>
       <c r="G222" s="36"/>
@@ -5971,145 +5949,123 @@
       <c r="I222" s="45"/>
     </row>
     <row r="223" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B223" t="s">
+      <c r="B223" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C223" s="22" t="s">
+      <c r="E223" s="31"/>
+      <c r="F223" s="36"/>
+      <c r="G223" s="36"/>
+      <c r="H223" s="44"/>
+      <c r="I223" s="45"/>
+    </row>
+    <row r="224" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
         <v>212</v>
       </c>
-      <c r="E223" s="31"/>
-      <c r="F223" s="37"/>
-      <c r="G223" s="36"/>
-      <c r="H223" s="44" t="s">
+      <c r="C224" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="E224" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F224" s="37" t="s">
+        <v>429</v>
+      </c>
+      <c r="G224" s="36"/>
+      <c r="H224" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="I224" s="45"/>
+    </row>
+    <row r="225" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="B225" t="s">
+        <v>262</v>
+      </c>
+      <c r="C225" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="D225" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="E225" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="I223" s="45"/>
-    </row>
-    <row r="224" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E224" s="31"/>
-      <c r="F224" s="36"/>
-      <c r="G224" s="36"/>
-      <c r="H224" s="44"/>
-      <c r="I224" s="45"/>
-    </row>
-    <row r="225" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B225" s="6" t="s">
+      <c r="F225" s="39" t="s">
+        <v>434</v>
+      </c>
+      <c r="G225" s="36"/>
+      <c r="H225" s="44" t="s">
+        <v>367</v>
+      </c>
+      <c r="I225" s="49" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="226" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B226" t="s">
         <v>213</v>
       </c>
-      <c r="E225" s="31"/>
-      <c r="F225" s="36"/>
-      <c r="G225" s="36"/>
-      <c r="H225" s="44"/>
-      <c r="I225" s="45"/>
-    </row>
-    <row r="226" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B226" t="s">
-        <v>214</v>
-      </c>
       <c r="C226" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="E226" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="F226" s="37" t="s">
-        <v>432</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E226" s="31"/>
+      <c r="F226" s="36"/>
       <c r="G226" s="36"/>
       <c r="H226" s="44" t="s">
-        <v>219</v>
+        <v>35</v>
       </c>
       <c r="I226" s="45"/>
     </row>
-    <row r="227" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>264</v>
-      </c>
-      <c r="C227" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="D227" s="22" t="s">
-        <v>266</v>
-      </c>
-      <c r="E227" s="63" t="s">
         <v>214</v>
       </c>
-      <c r="F227" s="39" t="s">
-        <v>437</v>
-      </c>
+      <c r="C227" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="E227" s="31"/>
+      <c r="F227" s="36"/>
       <c r="G227" s="36"/>
       <c r="H227" s="44" t="s">
-        <v>370</v>
-      </c>
-      <c r="I227" s="49" t="s">
-        <v>438</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="I227" s="45"/>
     </row>
     <row r="228" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
         <v>215</v>
       </c>
       <c r="C228" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E228" s="31"/>
-      <c r="F228" s="36"/>
+        <v>219</v>
+      </c>
+      <c r="E228" s="63" t="s">
+        <v>265</v>
+      </c>
+      <c r="F228" s="38" t="s">
+        <v>266</v>
+      </c>
       <c r="G228" s="36"/>
       <c r="H228" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="I228" s="45"/>
-    </row>
-    <row r="229" spans="2:9" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+      <c r="I228" s="45" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="229" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B229" t="s">
         <v>216</v>
       </c>
       <c r="C229" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="E229" s="31"/>
-      <c r="F229" s="36"/>
-      <c r="G229" s="36"/>
-      <c r="H229" s="44" t="s">
-        <v>220</v>
-      </c>
-      <c r="I229" s="45"/>
-    </row>
-    <row r="230" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B230" t="s">
-        <v>217</v>
-      </c>
-      <c r="C230" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="E230" s="63" t="s">
-        <v>267</v>
-      </c>
-      <c r="F230" s="38" t="s">
-        <v>268</v>
-      </c>
-      <c r="G230" s="36"/>
-      <c r="H230" s="44" t="s">
-        <v>371</v>
-      </c>
-      <c r="I230" s="45" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="231" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B231" t="s">
-        <v>218</v>
-      </c>
-      <c r="C231" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="E231" s="34"/>
-      <c r="F231" s="41"/>
-      <c r="G231" s="41"/>
-      <c r="H231" s="55" t="s">
-        <v>263</v>
-      </c>
-      <c r="I231" s="56"/>
+        <v>261</v>
+      </c>
+      <c r="E229" s="34"/>
+      <c r="F229" s="41"/>
+      <c r="G229" s="41"/>
+      <c r="H229" s="55" t="s">
+        <v>261</v>
+      </c>
+      <c r="I229" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
INCOMPLETE DEC IMPLEMENTATION IN CODE
INCOMPLETE DEC IMPLEMENTATION IN CODE
</commit_message>
<xml_diff>
--- a/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
+++ b/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\omer\myGitHub\Front-End-Compiler-Project\Mio Language Design\Syntax Analyze Phase\FirstFollowSelectionSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A9AC6A-49DE-439B-9AAC-81153E4C0CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155F0079-4A5D-4612-AA19-7841FE946CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="511">
   <si>
     <t>&lt;Start&gt;</t>
   </si>
@@ -1604,6 +1604,15 @@
   <si>
     <t>pm ? Parent ? Self ? id ?inc_dec( ? typeCast ? not? intConst ? 
 floatConst ? charConst ? boolConst ? strConst ? {  ? }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ID_FN&gt; </t>
+  </si>
+  <si>
+    <t>id?&lt;ASSIGN&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id? dot ? ( ?inc_dec ? = ?cma </t>
   </si>
 </sst>
 </file>
@@ -2416,8 +2425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F139" sqref="F139"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3873,13 +3882,21 @@
       <c r="I88" s="45"/>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B89" s="1"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="19"/>
+      <c r="B89" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="D89" s="19" t="s">
+        <v>510</v>
+      </c>
       <c r="E89" s="31"/>
       <c r="F89" s="36"/>
       <c r="G89" s="36"/>
-      <c r="H89" s="48"/>
+      <c r="H89" s="48" t="s">
+        <v>510</v>
+      </c>
       <c r="I89" s="45"/>
     </row>
     <row r="90" spans="2:9" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TESTCASE IS PARSE THRU GRAMMER
WORKS FINE YAYYY
</commit_message>
<xml_diff>
--- a/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
+++ b/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\omer\myGitHub\Front-End-Compiler-Project\Mio Language Design\Syntax Analyze Phase\FirstFollowSelectionSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05CAE52-5FDA-4AB1-891D-D82D1310F7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E9F430-A5DE-4E61-8065-8801EB0E7546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="508">
   <si>
     <t>&lt;Start&gt;</t>
   </si>
@@ -448,9 +448,6 @@
   </si>
   <si>
     <t>&lt;LIST_C&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">const ? dt ? id </t>
   </si>
   <si>
     <t xml:space="preserve">, ? ; </t>
@@ -704,9 +701,6 @@
     <t>dt ? str</t>
   </si>
   <si>
-    <t>id | dt | str</t>
-  </si>
-  <si>
     <t>&lt;ARR_TYPE&gt;? id? Null</t>
   </si>
   <si>
@@ -738,15 +732,6 @@
   </si>
   <si>
     <t>Static ? &lt;IS_FINAL&gt;</t>
-  </si>
-  <si>
-    <t>def ?  Static ? const ? dt ? id  ? }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def ? Static ? const ? dt ? id </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Static ? const ? dt ? id </t>
   </si>
   <si>
     <t xml:space="preserve">&lt;INC_DEC&gt; </t>
@@ -911,9 +896,6 @@
   </si>
   <si>
     <t>else ? Till ? &lt;SST&gt;</t>
-  </si>
-  <si>
-    <t>F&lt;CLASS_BODY&gt;</t>
   </si>
   <si>
     <t>)</t>
@@ -1449,9 +1431,6 @@
     <t>&lt;OPERANDS&gt;</t>
   </si>
   <si>
-    <t>&lt;DOT_ID_SUBSCRIPT&gt; ? F&lt;ID_TO_EXPR&gt; ? &lt;OPERANDS&gt;</t>
-  </si>
-  <si>
     <t>power ?  mdm ?  pm ? Rop ? 
 And ? Or ? &lt;OPER_TO_EXPR&gt; ? &lt;OPERANDS&gt;</t>
   </si>
@@ -1613,6 +1592,18 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;ACM&gt; </t>
+  </si>
+  <si>
+    <t>const? id ? dt ?str</t>
+  </si>
+  <si>
+    <t>Static ? const ? dt ? id ?str</t>
+  </si>
+  <si>
+    <t>def ? Static ? const ? dt ? id ?str</t>
+  </si>
+  <si>
+    <t>def ?  Static ? const ? dt ? id  ?str? }</t>
   </si>
 </sst>
 </file>
@@ -2425,8 +2416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2450,22 +2441,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="H1" s="42" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
@@ -2485,13 +2476,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
@@ -2499,7 +2490,7 @@
         <v>18</v>
       </c>
       <c r="I3" s="45" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2507,23 +2498,23 @@
         <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="E4" s="63" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="46" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="I4" s="45" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -2531,23 +2522,23 @@
         <v>6</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="E5" s="63" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="G5" s="36"/>
       <c r="H5" s="46" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2555,23 +2546,23 @@
         <v>7</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="E6" s="63" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="G6" s="36"/>
       <c r="H6" s="46" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="I6" s="45" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -2611,22 +2602,22 @@
         <v>8</v>
       </c>
       <c r="C10" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="E10" s="64" t="s">
+        <v>287</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>288</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>433</v>
+      </c>
+      <c r="H10" s="47" t="s">
         <v>422</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>404</v>
-      </c>
-      <c r="E10" s="64" t="s">
-        <v>292</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>293</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>439</v>
-      </c>
-      <c r="H10" s="47" t="s">
-        <v>428</v>
       </c>
       <c r="I10" s="45"/>
     </row>
@@ -2653,20 +2644,20 @@
         <v>9</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="47" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="I13" s="45"/>
     </row>
@@ -2675,23 +2666,23 @@
         <v>10</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="E14" s="63" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="G14" s="36"/>
       <c r="H14" s="47" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="I14" s="45" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -2721,14 +2712,14 @@
         <v>11</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="31"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
       <c r="H17" s="48" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="I17" s="45"/>
     </row>
@@ -2791,30 +2782,30 @@
         <v>17</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="31"/>
       <c r="F22" s="36"/>
       <c r="G22" s="36"/>
       <c r="H22" s="48" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="I22" s="45"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="31"/>
       <c r="F23" s="36"/>
       <c r="G23" s="36"/>
       <c r="H23" s="48" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="I23" s="45"/>
     </row>
@@ -2845,14 +2836,14 @@
         <v>21</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="31"/>
       <c r="F26" s="36"/>
       <c r="G26" s="36"/>
       <c r="H26" s="48" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="I26" s="45"/>
     </row>
@@ -2861,14 +2852,14 @@
         <v>22</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="31"/>
       <c r="F27" s="36"/>
       <c r="G27" s="36"/>
       <c r="H27" s="48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I27" s="45"/>
     </row>
@@ -2881,10 +2872,10 @@
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="63" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="F28" s="36" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="G28" s="36"/>
       <c r="H28" s="48" t="s">
@@ -2897,21 +2888,21 @@
         <v>24</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="64" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="G29" s="36"/>
       <c r="H29" s="48" t="s">
         <v>26</v>
       </c>
       <c r="I29" s="45" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -2919,30 +2910,30 @@
         <v>25</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="31"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
       <c r="H30" s="48" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="I30" s="45"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="31"/>
       <c r="F31" s="36"/>
       <c r="G31" s="36"/>
       <c r="H31" s="48" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="I31" s="45"/>
     </row>
@@ -2958,7 +2949,7 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2977,17 +2968,17 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="63" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="F34" s="57" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="G34" s="36"/>
       <c r="H34" s="48" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="I34" s="45" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -3069,16 +3060,16 @@
         <v>32</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E41" s="31"/>
       <c r="F41" s="36"/>
       <c r="G41" s="36"/>
       <c r="H41" s="48" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="I41" s="45"/>
     </row>
@@ -3100,19 +3091,19 @@
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E43" s="31"/>
       <c r="F43" s="36"/>
       <c r="G43" s="36"/>
       <c r="H43" s="48" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="I43" s="45"/>
     </row>
@@ -3131,16 +3122,16 @@
         <v>36</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="E45" s="31"/>
       <c r="F45" s="36"/>
       <c r="G45" s="36"/>
       <c r="H45" s="48" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="I45" s="45"/>
     </row>
@@ -3149,22 +3140,22 @@
         <v>37</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E46" s="63" t="s">
         <v>36</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="G46" s="38" t="s">
         <v>35</v>
       </c>
       <c r="H46" s="48" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="I46" s="45" t="s">
         <v>35</v>
@@ -3213,52 +3204,52 @@
         <v>41</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E50" s="31"/>
       <c r="F50" s="36"/>
       <c r="G50" s="36"/>
       <c r="H50" s="48" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I50" s="45"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>42</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E51" s="31"/>
       <c r="F51" s="36"/>
       <c r="G51" s="36"/>
       <c r="H51" s="48" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I51" s="45"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E52" s="31"/>
       <c r="F52" s="36"/>
       <c r="G52" s="36"/>
       <c r="H52" s="48" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="I52" s="45"/>
     </row>
@@ -3267,40 +3258,40 @@
         <v>42</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E53" s="31"/>
       <c r="F53" s="36"/>
       <c r="G53" s="36"/>
       <c r="H53" s="48" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I53" s="45"/>
     </row>
     <row r="54" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E54" s="63" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="G54" s="38" t="s">
         <v>35</v>
       </c>
       <c r="H54" s="48" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="I54" s="45" t="s">
         <v>35</v>
@@ -3311,14 +3302,14 @@
         <v>43</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="31"/>
       <c r="F55" s="36"/>
       <c r="G55" s="36"/>
       <c r="H55" s="48" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="I55" s="45"/>
     </row>
@@ -3352,13 +3343,13 @@
         <v>52</v>
       </c>
       <c r="D58" s="19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E58" s="31"/>
       <c r="F58" s="36"/>
       <c r="G58" s="36"/>
       <c r="H58" s="48" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I58" s="45"/>
     </row>
@@ -3367,16 +3358,16 @@
         <v>46</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E59" s="31"/>
       <c r="F59" s="36"/>
       <c r="G59" s="36"/>
       <c r="H59" s="44" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="I59" s="45"/>
     </row>
@@ -3385,14 +3376,14 @@
         <v>47</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="31"/>
       <c r="F60" s="36"/>
       <c r="G60" s="36"/>
       <c r="H60" s="48" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I60" s="45"/>
     </row>
@@ -3405,15 +3396,15 @@
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="32" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F61" s="36"/>
       <c r="G61" s="36"/>
       <c r="H61" s="48" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="I61" s="45" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
@@ -3430,7 +3421,7 @@
       <c r="F62" s="36"/>
       <c r="G62" s="36"/>
       <c r="H62" s="48" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="I62" s="45" t="s">
         <v>35</v>
@@ -3498,13 +3489,13 @@
         <v>59</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>237</v>
+        <v>507</v>
       </c>
       <c r="E67" s="31"/>
       <c r="F67" s="36"/>
       <c r="G67" s="36"/>
       <c r="H67" s="48" t="s">
-        <v>237</v>
+        <v>507</v>
       </c>
       <c r="I67" s="45"/>
     </row>
@@ -3516,17 +3507,11 @@
         <v>60</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>238</v>
-      </c>
-      <c r="E68" s="63" t="s">
-        <v>294</v>
-      </c>
-      <c r="F68" s="36" t="s">
-        <v>237</v>
+        <v>506</v>
       </c>
       <c r="G68" s="36"/>
       <c r="H68" s="48" t="s">
-        <v>238</v>
+        <v>506</v>
       </c>
       <c r="I68" s="45"/>
     </row>
@@ -3534,9 +3519,6 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
-      <c r="E69" s="63" t="s">
-        <v>461</v>
-      </c>
       <c r="F69" s="36"/>
       <c r="G69" s="36"/>
       <c r="H69" s="44"/>
@@ -3544,7 +3526,7 @@
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="9" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3556,7 +3538,7 @@
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="9" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -3571,22 +3553,22 @@
         <v>61</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="D72" s="19" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F72" s="58" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="G72" s="39" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="H72" s="46" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="I72" s="49" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
     </row>
     <row r="73" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3598,13 +3580,13 @@
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="65" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F73" s="59" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="G73" s="37" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="H73" s="48" t="s">
         <v>26</v>
@@ -3613,26 +3595,26 @@
     </row>
     <row r="74" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="D74" s="19" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E74" s="63" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F74" s="18" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="G74" s="36"/>
       <c r="H74" s="46" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="I74" s="49" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
@@ -3659,13 +3641,13 @@
         <v>67</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E76" s="31"/>
       <c r="F76" s="36"/>
       <c r="G76" s="36"/>
       <c r="H76" s="47" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="I76" s="45"/>
     </row>
@@ -3693,37 +3675,37 @@
         <v>68</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E78" s="63" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F78" s="36" t="s">
         <v>38</v>
       </c>
       <c r="G78" s="36"/>
       <c r="H78" s="46" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="I78" s="45"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C79" s="97" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="D79" s="19" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="F79" s="36"/>
       <c r="G79" s="36"/>
       <c r="H79" s="44" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="I79" s="45"/>
     </row>
@@ -3739,7 +3721,7 @@
     </row>
     <row r="81" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B81" s="10" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -3754,25 +3736,25 @@
         <v>69</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="D82" s="23" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E82" s="63" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="G82" s="39" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="H82" s="50" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="I82" s="49" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="83" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3780,51 +3762,51 @@
         <v>70</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="D83" s="23" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="E83" s="63" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="G83" s="39" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="H83" s="51" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="I83" s="49" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="84" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="C84" s="97" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="D84" s="19" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="E84" s="63" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="F84" s="60" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="G84" s="39" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="H84" s="48" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="I84" s="49" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
@@ -3866,16 +3848,16 @@
         <v>73</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="E88" s="31"/>
       <c r="F88" s="37"/>
       <c r="G88" s="36"/>
       <c r="H88" s="48" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="I88" s="45"/>
     </row>
@@ -3887,30 +3869,30 @@
         <v>85</v>
       </c>
       <c r="D89" s="19" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="E89" s="31"/>
       <c r="F89" s="36"/>
       <c r="G89" s="36"/>
       <c r="H89" s="48" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="I89" s="45"/>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="D90" s="19" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="E90" s="31"/>
       <c r="F90" s="36"/>
       <c r="H90" s="48" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="I90" s="45"/>
     </row>
@@ -3919,16 +3901,16 @@
         <v>75</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="E91" s="33"/>
       <c r="F91" s="36"/>
       <c r="G91" s="36"/>
       <c r="H91" s="46" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="I91" s="45"/>
     </row>
@@ -3937,16 +3919,16 @@
         <v>76</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="D92" s="19" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="E92" s="31"/>
       <c r="F92" s="37"/>
       <c r="G92" s="36"/>
       <c r="H92" s="48" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="I92" s="45"/>
     </row>
@@ -3955,16 +3937,16 @@
         <v>77</v>
       </c>
       <c r="C93" s="99" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="E93" s="31"/>
       <c r="F93" s="36"/>
       <c r="G93" s="36"/>
       <c r="H93" s="44" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="I93" s="45"/>
     </row>
@@ -3973,19 +3955,19 @@
         <v>78</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="D94" s="21" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="E94" s="64" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="F94" s="36" t="s">
         <v>88</v>
       </c>
       <c r="H94" s="47" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="I94" s="45"/>
     </row>
@@ -3997,18 +3979,18 @@
         <v>86</v>
       </c>
       <c r="D95" s="19" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E95" s="32" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F95" s="36"/>
       <c r="G95" s="36"/>
       <c r="H95" s="48" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="I95" s="45" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="96" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -4016,19 +3998,19 @@
         <v>80</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D96" s="24" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="E96" s="31" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F96" s="36" t="s">
         <v>88</v>
       </c>
       <c r="H96" s="52" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="I96" s="45"/>
     </row>
@@ -4037,22 +4019,22 @@
         <v>81</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="D97" s="20" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="E97" s="63" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G97" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H97" s="98" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="I97" s="45" t="s">
         <v>88</v>
@@ -4063,22 +4045,22 @@
         <v>82</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="E98" s="63" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G98" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H98" s="98" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="I98" s="45" t="s">
         <v>88</v>
@@ -4086,25 +4068,25 @@
     </row>
     <row r="99" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C99" s="11" t="s">
         <v>87</v>
       </c>
       <c r="D99" s="20" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="E99" s="64" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="G99" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H99" s="98" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="I99" s="45" t="s">
         <v>88</v>
@@ -4181,88 +4163,88 @@
         <v>92</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="E105" s="31"/>
       <c r="F105" s="36"/>
       <c r="G105" s="36"/>
       <c r="H105" s="48" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="I105" s="45"/>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="D106" s="19" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="E106" s="31"/>
       <c r="F106" s="36"/>
       <c r="G106" s="36"/>
       <c r="H106" s="48" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="I106" s="45"/>
     </row>
     <row r="107" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="D107" s="19" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="E107" s="31"/>
       <c r="F107" s="36"/>
       <c r="G107" s="36"/>
       <c r="H107" s="48" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="I107" s="45"/>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D108" s="19" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="E108" s="31"/>
       <c r="F108" s="36"/>
       <c r="G108" s="36"/>
       <c r="H108" s="48" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="I108" s="45"/>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="C109" s="97" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="E109" s="31"/>
       <c r="F109" s="36"/>
       <c r="G109" s="36"/>
       <c r="H109" s="48" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="I109" s="45"/>
     </row>
@@ -4274,13 +4256,13 @@
         <v>94</v>
       </c>
       <c r="D110" s="23" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E110" s="31"/>
       <c r="F110" s="36"/>
       <c r="G110" s="36"/>
       <c r="H110" s="51" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="I110" s="45"/>
     </row>
@@ -4315,10 +4297,10 @@
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="31" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="F113" s="37" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="G113" s="36"/>
       <c r="H113" s="48" t="s">
@@ -4331,7 +4313,7 @@
         <v>97</v>
       </c>
       <c r="C114" s="70" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="E114" s="31" t="s">
         <v>96</v>
@@ -4339,19 +4321,19 @@
       <c r="F114" s="37"/>
       <c r="G114" s="36"/>
       <c r="H114" s="48" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="I114" s="45"/>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="C115" s="11" t="s">
         <v>99</v>
       </c>
       <c r="D115" s="19" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="E115" s="31" t="s">
         <v>97</v>
@@ -4359,7 +4341,7 @@
       <c r="F115" s="37"/>
       <c r="G115" s="36"/>
       <c r="H115" s="48" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="I115" s="45"/>
     </row>
@@ -4461,13 +4443,13 @@
         <v>118</v>
       </c>
       <c r="D122" s="78" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E122" s="73"/>
       <c r="F122" s="74"/>
       <c r="G122" s="80"/>
       <c r="H122" s="92" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="I122" s="75"/>
     </row>
@@ -4476,14 +4458,14 @@
         <v>106</v>
       </c>
       <c r="C123" s="79" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D123" s="79"/>
       <c r="E123" s="73"/>
       <c r="F123" s="80"/>
       <c r="G123" s="80"/>
       <c r="H123" s="93" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="I123" s="75"/>
     </row>
@@ -4495,13 +4477,13 @@
         <v>118</v>
       </c>
       <c r="D124" s="82" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E124" s="73"/>
       <c r="F124" s="80"/>
       <c r="G124" s="80"/>
       <c r="H124" s="94" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="I124" s="75"/>
     </row>
@@ -4510,16 +4492,16 @@
         <v>108</v>
       </c>
       <c r="C125" s="83" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="D125" s="79" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="E125" s="73"/>
       <c r="F125" s="87"/>
       <c r="G125" s="87"/>
       <c r="H125" s="94" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="I125" s="85"/>
     </row>
@@ -4528,7 +4510,7 @@
         <v>109</v>
       </c>
       <c r="C126" s="79" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D126" s="79"/>
       <c r="E126" s="73"/>
@@ -4539,19 +4521,19 @@
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" s="79" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C127" s="81" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="D127" s="79" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="E127" s="73"/>
       <c r="F127" s="80"/>
       <c r="G127" s="88"/>
       <c r="H127" s="93" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="I127" s="75"/>
     </row>
@@ -4560,16 +4542,16 @@
         <v>110</v>
       </c>
       <c r="C128" s="81" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D128" s="79" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="E128" s="73"/>
       <c r="F128" s="87"/>
       <c r="G128" s="80"/>
       <c r="H128" s="93" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="I128" s="75"/>
     </row>
@@ -4578,22 +4560,22 @@
         <v>111</v>
       </c>
       <c r="C129" s="86" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="D129" s="87" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="E129" s="73"/>
       <c r="F129" s="88"/>
       <c r="G129" s="80"/>
       <c r="H129" s="95" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="I129" s="75"/>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" s="79" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C130" s="84" t="s">
         <v>88</v>
@@ -4615,17 +4597,17 @@
         <v>119</v>
       </c>
       <c r="D131" s="21" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="E131" s="31" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="F131" s="36" t="s">
         <v>97</v>
       </c>
       <c r="G131" s="37"/>
       <c r="H131" s="47" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="I131" s="45"/>
     </row>
@@ -4641,20 +4623,20 @@
         <v>125</v>
       </c>
       <c r="C133" s="89" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="E133" s="31" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="F133" s="96" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="G133" s="36"/>
       <c r="H133" s="44" t="s">
         <v>26</v>
       </c>
       <c r="I133" s="45" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="134" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4665,7 +4647,7 @@
         <v>128</v>
       </c>
       <c r="D134" s="21" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="E134" s="31" t="s">
         <v>125</v>
@@ -4673,7 +4655,7 @@
       <c r="F134" s="36"/>
       <c r="G134" s="36"/>
       <c r="H134" s="47" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="I134" s="45"/>
     </row>
@@ -4685,13 +4667,13 @@
         <v>120</v>
       </c>
       <c r="D135" s="22" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="E135" s="31"/>
       <c r="F135" s="36"/>
       <c r="G135" s="36"/>
       <c r="H135" s="44" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="I135" s="45"/>
     </row>
@@ -4700,20 +4682,20 @@
         <v>124</v>
       </c>
       <c r="C136" s="89" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="E136" s="31" t="s">
         <v>126</v>
       </c>
       <c r="F136" s="96" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="G136" s="36"/>
       <c r="H136" s="44" t="s">
         <v>26</v>
       </c>
       <c r="I136" s="45" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.25">
@@ -4753,13 +4735,13 @@
         <v>122</v>
       </c>
       <c r="D140" s="20" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="E140" s="31"/>
       <c r="F140" s="36"/>
       <c r="G140" s="36"/>
       <c r="H140" s="46" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="I140" s="45"/>
     </row>
@@ -4804,13 +4786,13 @@
         <v>21</v>
       </c>
       <c r="D144" s="22" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E144" s="31"/>
       <c r="F144" s="37"/>
       <c r="G144" s="36"/>
       <c r="H144" s="44" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="I144" s="45"/>
     </row>
@@ -4819,34 +4801,34 @@
         <v>131</v>
       </c>
       <c r="C145" s="13" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="D145" s="19" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="E145" s="31"/>
       <c r="F145" s="37"/>
       <c r="G145" s="36"/>
       <c r="H145" s="48" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="I145" s="45"/>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C146" s="13" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D146" s="19" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E146" s="31"/>
       <c r="F146" s="37"/>
       <c r="G146" s="36"/>
       <c r="H146" s="48" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="I146" s="45"/>
     </row>
@@ -4855,16 +4837,16 @@
         <v>132</v>
       </c>
       <c r="C147" s="69" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="D147" s="25" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="E147" s="31"/>
       <c r="F147" s="36"/>
       <c r="G147" s="36"/>
       <c r="H147" s="53" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="I147" s="45"/>
     </row>
@@ -4905,16 +4887,16 @@
         <v>136</v>
       </c>
       <c r="C151" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D151" s="22" t="s">
-        <v>239</v>
+        <v>505</v>
       </c>
       <c r="E151" s="31"/>
       <c r="F151" s="36"/>
       <c r="G151" s="36"/>
       <c r="H151" s="54" t="s">
-        <v>239</v>
+        <v>505</v>
       </c>
       <c r="I151" s="45"/>
     </row>
@@ -4923,34 +4905,34 @@
         <v>137</v>
       </c>
       <c r="C152" s="26" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="D152" s="22" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="E152" s="31"/>
       <c r="F152" s="36"/>
       <c r="G152" s="36"/>
       <c r="H152" s="44" t="s">
-        <v>141</v>
+        <v>504</v>
       </c>
       <c r="I152" s="45"/>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="C153" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D153" s="22" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E153" s="31"/>
       <c r="F153" s="36"/>
       <c r="G153" s="36"/>
       <c r="H153" s="44" t="s">
-        <v>225</v>
+        <v>312</v>
       </c>
       <c r="I153" s="45"/>
     </row>
@@ -4959,33 +4941,35 @@
         <v>138</v>
       </c>
       <c r="C154" s="13" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="D154" s="28" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E154" s="31"/>
       <c r="F154" s="36"/>
       <c r="G154" s="36"/>
       <c r="H154" s="44" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="I154" s="45"/>
     </row>
     <row r="155" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="C155" s="13" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="D155" s="28" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="E155" s="31"/>
       <c r="F155" s="36"/>
       <c r="G155" s="36"/>
-      <c r="H155" s="44"/>
+      <c r="H155" s="44" t="s">
+        <v>382</v>
+      </c>
       <c r="I155" s="45"/>
     </row>
     <row r="156" spans="2:9" x14ac:dyDescent="0.25">
@@ -4993,16 +4977,16 @@
         <v>139</v>
       </c>
       <c r="C156" s="69" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="D156" s="25" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="E156" s="31"/>
       <c r="F156" s="36"/>
       <c r="G156" s="36"/>
       <c r="H156" s="53" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="I156" s="45"/>
     </row>
@@ -5011,13 +4995,13 @@
         <v>140</v>
       </c>
       <c r="C157" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E157" s="31"/>
       <c r="F157" s="36"/>
       <c r="G157" s="36"/>
       <c r="H157" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I157" s="45"/>
     </row>
@@ -5030,7 +5014,7 @@
     </row>
     <row r="159" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B159" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E159" s="31"/>
       <c r="F159" s="36"/>
@@ -5040,246 +5024,246 @@
     </row>
     <row r="160" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C160" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D160" s="20" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="E160" s="63" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F160" s="36" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="G160" s="36"/>
       <c r="H160" s="46" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="I160" s="45"/>
     </row>
     <row r="161" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C161" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E161" s="63" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F161" s="39" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="G161" s="36"/>
       <c r="H161" s="44" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="I161" s="45" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="162" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C162" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D162" s="20" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="E162" s="63" t="s">
+        <v>275</v>
+      </c>
+      <c r="F162" s="36" t="s">
         <v>280</v>
-      </c>
-      <c r="F162" s="36" t="s">
-        <v>285</v>
       </c>
       <c r="G162" s="36"/>
       <c r="H162" s="46" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="I162" s="45"/>
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C163" s="28" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="E163" s="66" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="F163" s="58" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="G163" s="38" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="H163" s="44" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="I163" s="45" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="164" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C164" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D164" s="20" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="E164" s="67" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="F164" s="36" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="G164" s="36"/>
       <c r="H164" s="46" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="I164" s="45"/>
     </row>
     <row r="165" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C165" s="22" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E165" s="66" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="F165" s="58" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="G165" s="38" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="H165" s="44" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I165" s="45" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="166" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C166" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D166" s="20" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="E166" s="63" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F166" s="36" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="G166" s="36"/>
       <c r="H166" s="46" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="I166" s="45"/>
     </row>
     <row r="167" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C167" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E167" s="65" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="F167" s="58" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="G167" s="38" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="H167" s="44" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="I167" s="45" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="168" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C168" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D168" s="20" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="E168" s="63" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="F168" s="36" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="G168" s="36"/>
       <c r="H168" s="46" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="I168" s="45"/>
     </row>
     <row r="169" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C169" s="22" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E169" s="65" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="F169" s="58" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="G169" s="39" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="H169" s="47" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="I169" s="49" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="170" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
+        <v>153</v>
+      </c>
+      <c r="C170" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="C170" s="13" t="s">
-        <v>155</v>
-      </c>
       <c r="D170" s="20" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="E170" s="63" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="F170" s="36" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="G170" s="36"/>
       <c r="H170" s="46" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="I170" s="45"/>
     </row>
@@ -5288,65 +5272,65 @@
         <v>87</v>
       </c>
       <c r="C171" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E171" s="65" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="F171" s="58" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="G171" s="39" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="H171" s="44" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="I171" s="49" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="172" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
+        <v>154</v>
+      </c>
+      <c r="C172" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="C172" s="13" t="s">
-        <v>156</v>
-      </c>
       <c r="D172" s="20" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="E172" s="63" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F172" s="36" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="G172" s="36"/>
       <c r="H172" s="46" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="I172" s="45"/>
     </row>
     <row r="173" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="E173" s="68" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F173" s="36" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="G173" s="36"/>
       <c r="H173" s="46" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="I173" s="45"/>
     </row>
@@ -5359,7 +5343,7 @@
     </row>
     <row r="175" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B175" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E175" s="31"/>
       <c r="F175" s="36"/>
@@ -5369,55 +5353,55 @@
     </row>
     <row r="176" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B176" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C176" s="14" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="D176" s="20" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="E176" s="63" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="F176" s="61" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="G176" s="37" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="H176" s="46" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="I176" s="45"/>
     </row>
     <row r="177" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C177" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E177" s="31"/>
       <c r="F177" s="36"/>
       <c r="G177" s="36"/>
       <c r="H177" s="44" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I177" s="45"/>
     </row>
     <row r="178" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C178" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E178" s="31"/>
       <c r="F178" s="36"/>
       <c r="G178" s="36"/>
       <c r="H178" s="44" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I178" s="45"/>
     </row>
@@ -5430,7 +5414,7 @@
     </row>
     <row r="180" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B180" s="6" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E180" s="31"/>
       <c r="F180" s="36"/>
@@ -5440,31 +5424,31 @@
     </row>
     <row r="181" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B181" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C181" s="21" t="s">
         <v>167</v>
-      </c>
-      <c r="C181" s="21" t="s">
-        <v>168</v>
       </c>
       <c r="E181" s="31"/>
       <c r="F181" s="36"/>
       <c r="G181" s="36"/>
       <c r="H181" s="47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I181" s="45"/>
     </row>
     <row r="182" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B182" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C182" s="24" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E182" s="31"/>
       <c r="F182" s="36"/>
       <c r="G182" s="36"/>
       <c r="H182" s="52" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="I182" s="45"/>
     </row>
@@ -5477,7 +5461,7 @@
     </row>
     <row r="184" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B184" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E184" s="31"/>
       <c r="F184" s="36"/>
@@ -5487,7 +5471,7 @@
     </row>
     <row r="185" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B185" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E185" s="31"/>
       <c r="F185" s="36"/>
@@ -5497,42 +5481,42 @@
     </row>
     <row r="186" spans="2:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C186" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E186" s="63" t="s">
         <v>9</v>
       </c>
       <c r="F186" s="37" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="G186" s="36"/>
       <c r="H186" s="44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I186" s="45"/>
     </row>
     <row r="187" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C187" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E187" s="63" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F187" s="39" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="G187" s="36"/>
       <c r="H187" s="44" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="I187" s="49" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
     </row>
     <row r="188" spans="2:9" x14ac:dyDescent="0.25">
@@ -5544,7 +5528,7 @@
     </row>
     <row r="189" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B189" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E189" s="31"/>
       <c r="F189" s="36"/>
@@ -5554,67 +5538,67 @@
     </row>
     <row r="190" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C190" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E190" s="31"/>
       <c r="F190" s="36"/>
       <c r="G190" s="36"/>
       <c r="H190" s="44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I190" s="45"/>
     </row>
     <row r="191" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C191" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D191" s="22" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E191" s="31"/>
       <c r="F191" s="36"/>
       <c r="G191" s="36"/>
       <c r="H191" s="44" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="I191" s="45"/>
     </row>
     <row r="192" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C192" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E192" s="31"/>
       <c r="F192" s="36"/>
       <c r="G192" s="36"/>
       <c r="H192" s="44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I192" s="45"/>
     </row>
     <row r="193" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C193" s="13" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="D193" s="21" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E193" s="31"/>
       <c r="F193" s="36"/>
       <c r="G193" s="36"/>
       <c r="H193" s="47" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="I193" s="45"/>
     </row>
@@ -5627,7 +5611,7 @@
     </row>
     <row r="195" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B195" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E195" s="31"/>
       <c r="F195" s="36"/>
@@ -5644,7 +5628,7 @@
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B197" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E197" s="31"/>
       <c r="F197" s="36"/>
@@ -5654,34 +5638,34 @@
     </row>
     <row r="198" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C198" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E198" s="31"/>
       <c r="F198" s="36"/>
       <c r="G198" s="36"/>
       <c r="H198" s="44" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I198" s="45"/>
     </row>
     <row r="199" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C199" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D199" s="22" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E199" s="31"/>
       <c r="F199" s="36"/>
       <c r="G199" s="36"/>
       <c r="H199" s="44" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="I199" s="45"/>
     </row>
@@ -5694,7 +5678,7 @@
     </row>
     <row r="201" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B201" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E201" s="31"/>
       <c r="F201" s="36"/>
@@ -5704,31 +5688,31 @@
     </row>
     <row r="202" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C202" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E202" s="31"/>
       <c r="F202" s="36"/>
       <c r="G202" s="36"/>
       <c r="H202" s="44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I202" s="45"/>
     </row>
     <row r="203" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C203" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E203" s="31"/>
       <c r="F203" s="36"/>
       <c r="G203" s="36"/>
       <c r="H203" s="44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I203" s="45"/>
     </row>
@@ -5741,7 +5725,7 @@
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B205" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E205" s="31"/>
       <c r="F205" s="36"/>
@@ -5751,82 +5735,82 @@
     </row>
     <row r="206" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C206" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E206" s="31"/>
       <c r="F206" s="36"/>
       <c r="G206" s="36"/>
       <c r="H206" s="44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I206" s="45"/>
     </row>
     <row r="207" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C207" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E207" s="31" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="F207" s="36"/>
       <c r="G207" s="36"/>
       <c r="H207" s="44" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I207" s="45"/>
     </row>
     <row r="208" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C208" s="14" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="D208" s="22" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E208" s="63" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="F208" s="38" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="G208" s="36"/>
       <c r="H208" s="44" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="I208" s="45" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="209" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="C209" s="26" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D209" s="22" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E209" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F209" s="38" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="G209" s="36"/>
       <c r="H209" s="44" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="I209" s="45" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="210" spans="2:9" x14ac:dyDescent="0.25">
@@ -5838,7 +5822,7 @@
     </row>
     <row r="211" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B211" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E211" s="31"/>
       <c r="F211" s="36"/>
@@ -5856,7 +5840,7 @@
     </row>
     <row r="213" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B213" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E213" s="31"/>
       <c r="F213" s="36"/>
@@ -5866,46 +5850,46 @@
     </row>
     <row r="214" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C214" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E214" s="31"/>
       <c r="F214" s="36"/>
       <c r="G214" s="36"/>
       <c r="H214" s="44" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I214" s="45"/>
     </row>
     <row r="215" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C215" s="28" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E215" s="31"/>
       <c r="F215" s="36"/>
       <c r="G215" s="36"/>
       <c r="H215" s="44" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="I215" s="45"/>
     </row>
     <row r="216" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C216" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E216" s="31"/>
       <c r="F216" s="36"/>
       <c r="G216" s="36"/>
       <c r="H216" s="44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I216" s="45"/>
     </row>
@@ -5918,7 +5902,7 @@
     </row>
     <row r="218" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B218" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E218" s="31"/>
       <c r="F218" s="36"/>
@@ -5928,16 +5912,16 @@
     </row>
     <row r="219" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C219" s="28" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E219" s="31"/>
       <c r="F219" s="36"/>
       <c r="G219" s="36"/>
       <c r="H219" s="44" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="I219" s="45"/>
     </row>
@@ -5950,7 +5934,7 @@
     </row>
     <row r="221" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B221" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E221" s="31"/>
       <c r="F221" s="36"/>
@@ -5960,16 +5944,16 @@
     </row>
     <row r="222" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
+        <v>208</v>
+      </c>
+      <c r="C222" s="22" t="s">
         <v>209</v>
-      </c>
-      <c r="C222" s="22" t="s">
-        <v>210</v>
       </c>
       <c r="E222" s="31"/>
       <c r="F222" s="37"/>
       <c r="G222" s="36"/>
       <c r="H222" s="44" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I222" s="45"/>
     </row>
@@ -5982,7 +5966,7 @@
     </row>
     <row r="224" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B224" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E224" s="31"/>
       <c r="F224" s="36"/>
@@ -5992,50 +5976,50 @@
     </row>
     <row r="225" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C225" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E225" s="63" t="s">
         <v>9</v>
       </c>
       <c r="F225" s="37" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="G225" s="36"/>
       <c r="H225" s="44" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I225" s="45"/>
     </row>
     <row r="226" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C226" s="16" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D226" s="22" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E226" s="63" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F226" s="39" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="G226" s="36"/>
       <c r="H226" s="44" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="I226" s="49" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C227" s="22" t="s">
         <v>35</v>
@@ -6050,52 +6034,52 @@
     </row>
     <row r="228" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C228" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E228" s="31"/>
       <c r="F228" s="36"/>
       <c r="G228" s="36"/>
       <c r="H228" s="44" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I228" s="45"/>
     </row>
     <row r="229" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C229" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E229" s="63" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F229" s="38" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="G229" s="36"/>
       <c r="H229" s="44" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="I229" s="45" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="230" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B230" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C230" s="22" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E230" s="34"/>
       <c r="F230" s="41"/>
       <c r="G230" s="41"/>
       <c r="H230" s="55" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I230" s="56"/>
     </row>

</xml_diff>

<commit_message>
ERROR THROWS IS FIXED
ID.ID errors
and multiple error thorws comma separated added
</commit_message>
<xml_diff>
--- a/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
+++ b/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\omer\myGitHub\Front-End-Compiler-Project\Mio Language Design\Syntax Analyze Phase\FirstFollowSelectionSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94F0CDC-6A5E-4609-8E01-6FC5FC7DD9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1816D862-F877-457A-865F-A0704C0D22EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="490">
   <si>
     <t>&lt;Start&gt;</t>
   </si>
@@ -722,6 +722,9 @@
   </si>
   <si>
     <t>Access Modifier</t>
+  </si>
+  <si>
+    <t>dot</t>
   </si>
   <si>
     <t xml:space="preserve">inc_dec ? = ? cma </t>
@@ -1519,6 +1522,33 @@
   </si>
   <si>
     <t>def ?  Static ? const ? dt ? id  ?str? }</t>
+  </si>
+  <si>
+    <t>&lt;ID_ERR&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ERR_DOT_ID&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ERR_LIST&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ERR_DOT_ID&gt;?&lt;ERR_LIST&gt;</t>
+  </si>
+  <si>
+    <t>dot?,?null</t>
+  </si>
+  <si>
+    <t>dot?,</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>dot?null</t>
+  </si>
+  <si>
+    <t>&lt;ID_ERR&gt;?&lt;ERR_LIST&gt;</t>
   </si>
 </sst>
 </file>
@@ -1811,7 +1841,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1984,6 +2014,8 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="40% - Accent1" xfId="6" builtinId="31"/>
@@ -2270,10 +2302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I217"/>
+  <dimension ref="B1:I220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D221" sqref="D221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,19 +2332,19 @@
         <v>205</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H1" s="42" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
@@ -2332,13 +2364,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
@@ -2346,7 +2378,7 @@
         <v>18</v>
       </c>
       <c r="I3" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2354,23 +2386,23 @@
         <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E4" s="63" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="46" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="I4" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -2381,20 +2413,20 @@
         <v>207</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E5" s="63" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G5" s="36"/>
       <c r="H5" s="46" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2405,20 +2437,20 @@
         <v>226</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E6" s="63" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G6" s="36"/>
       <c r="H6" s="46" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="I6" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -2458,22 +2490,22 @@
         <v>8</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E10" s="64" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H10" s="47" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="I10" s="45"/>
     </row>
@@ -2500,20 +2532,20 @@
         <v>9</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="47" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="I13" s="45"/>
     </row>
@@ -2522,23 +2554,23 @@
         <v>10</v>
       </c>
       <c r="C14" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="D14" s="27" t="s">
         <v>391</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>390</v>
-      </c>
       <c r="E14" s="63" t="s">
+        <v>247</v>
+      </c>
+      <c r="F14" s="38" t="s">
         <v>246</v>
-      </c>
-      <c r="F14" s="38" t="s">
-        <v>245</v>
       </c>
       <c r="G14" s="36"/>
       <c r="H14" s="47" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="I14" s="45" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -2568,14 +2600,14 @@
         <v>11</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="31"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
       <c r="H17" s="48" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="I17" s="45"/>
     </row>
@@ -2651,7 +2683,7 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>227</v>
@@ -2692,14 +2724,14 @@
         <v>21</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="31"/>
       <c r="F26" s="36"/>
       <c r="G26" s="36"/>
       <c r="H26" s="48" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="I26" s="45"/>
     </row>
@@ -2728,10 +2760,10 @@
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="63" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F28" s="36" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G28" s="36"/>
       <c r="H28" s="48" t="s">
@@ -2748,17 +2780,17 @@
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="64" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G29" s="36"/>
       <c r="H29" s="48" t="s">
         <v>26</v>
       </c>
       <c r="I29" s="45" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -2766,30 +2798,30 @@
         <v>25</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="31"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
       <c r="H30" s="48" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="I30" s="45"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="31"/>
       <c r="F31" s="36"/>
       <c r="G31" s="36"/>
       <c r="H31" s="48" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="I31" s="45"/>
     </row>
@@ -2824,17 +2856,17 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="63" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F34" s="57" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G34" s="36"/>
       <c r="H34" s="48" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I34" s="45" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -2916,16 +2948,16 @@
         <v>32</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E41" s="31"/>
       <c r="F41" s="36"/>
       <c r="G41" s="36"/>
       <c r="H41" s="48" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="I41" s="45"/>
     </row>
@@ -2947,19 +2979,19 @@
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E43" s="31"/>
       <c r="F43" s="36"/>
       <c r="G43" s="36"/>
       <c r="H43" s="48" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I43" s="45"/>
     </row>
@@ -2978,16 +3010,16 @@
         <v>36</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E45" s="31"/>
       <c r="F45" s="36"/>
       <c r="G45" s="36"/>
       <c r="H45" s="48" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="I45" s="45"/>
     </row>
@@ -2999,19 +3031,19 @@
         <v>210</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E46" s="63" t="s">
         <v>36</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G46" s="38" t="s">
         <v>35</v>
       </c>
       <c r="H46" s="48" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="I46" s="45" t="s">
         <v>35</v>
@@ -3081,13 +3113,13 @@
         <v>42</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E51" s="31"/>
       <c r="F51" s="36"/>
       <c r="G51" s="36"/>
       <c r="H51" s="48" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I51" s="45"/>
     </row>
@@ -3099,13 +3131,13 @@
         <v>218</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E52" s="31"/>
       <c r="F52" s="36"/>
       <c r="G52" s="36"/>
       <c r="H52" s="48" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I52" s="45"/>
     </row>
@@ -3114,16 +3146,16 @@
         <v>42</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E53" s="31"/>
       <c r="F53" s="36"/>
       <c r="G53" s="36"/>
       <c r="H53" s="48" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I53" s="45"/>
     </row>
@@ -3132,22 +3164,22 @@
         <v>219</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E54" s="63" t="s">
+        <v>250</v>
+      </c>
+      <c r="F54" s="17" t="s">
         <v>249</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>248</v>
       </c>
       <c r="G54" s="38" t="s">
         <v>35</v>
       </c>
       <c r="H54" s="48" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="I54" s="45" t="s">
         <v>35</v>
@@ -3158,14 +3190,14 @@
         <v>43</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="31"/>
       <c r="F55" s="36"/>
       <c r="G55" s="36"/>
       <c r="H55" s="48" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="I55" s="45"/>
     </row>
@@ -3214,16 +3246,16 @@
         <v>46</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E59" s="31"/>
       <c r="F59" s="36"/>
       <c r="G59" s="36"/>
       <c r="H59" s="44" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="I59" s="45"/>
     </row>
@@ -3252,15 +3284,15 @@
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="32" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F61" s="36"/>
       <c r="G61" s="36"/>
       <c r="H61" s="48" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="I61" s="45" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
@@ -3277,7 +3309,7 @@
       <c r="F62" s="36"/>
       <c r="G62" s="36"/>
       <c r="H62" s="48" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="I62" s="45" t="s">
         <v>35</v>
@@ -3345,13 +3377,13 @@
         <v>59</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E67" s="31"/>
       <c r="F67" s="36"/>
       <c r="G67" s="36"/>
       <c r="H67" s="48" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="I67" s="45"/>
     </row>
@@ -3363,11 +3395,11 @@
         <v>60</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="G68" s="36"/>
       <c r="H68" s="48" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="I68" s="45"/>
     </row>
@@ -3382,7 +3414,7 @@
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3394,7 +3426,7 @@
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -3409,22 +3441,22 @@
         <v>61</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D72" s="19" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F72" s="58" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="G72" s="39" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="H72" s="46" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="I72" s="49" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="73" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3436,13 +3468,13 @@
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="65" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F73" s="59" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="G73" s="37" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="H73" s="48" t="s">
         <v>26</v>
@@ -3454,23 +3486,23 @@
         <v>212</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D74" s="19" t="s">
         <v>213</v>
       </c>
       <c r="E74" s="63" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F74" s="18" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="G74" s="36"/>
       <c r="H74" s="46" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I74" s="49" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
@@ -3497,13 +3529,13 @@
         <v>67</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E76" s="31"/>
       <c r="F76" s="36"/>
       <c r="G76" s="36"/>
       <c r="H76" s="47" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="I76" s="45"/>
     </row>
@@ -3531,37 +3563,37 @@
         <v>68</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E78" s="63" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F78" s="36" t="s">
         <v>38</v>
       </c>
       <c r="G78" s="36"/>
       <c r="H78" s="46" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I78" s="45"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C79" s="73" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D79" s="19" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F79" s="36"/>
       <c r="G79" s="36"/>
       <c r="H79" s="44" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="I79" s="45"/>
     </row>
@@ -3577,7 +3609,7 @@
     </row>
     <row r="81" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B81" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -3592,25 +3624,25 @@
         <v>69</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D82" s="23" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E82" s="63" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G82" s="39" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H82" s="50" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="I82" s="49" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="83" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3618,51 +3650,51 @@
         <v>70</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D83" s="23" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E83" s="63" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G83" s="39" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H83" s="51" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="I83" s="49" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="84" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C84" s="73" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D84" s="19" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E84" s="63" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="F84" s="60" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G84" s="39" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H84" s="48" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="I84" s="49" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
@@ -3704,16 +3736,16 @@
         <v>73</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E88" s="31"/>
       <c r="F88" s="37"/>
       <c r="G88" s="36"/>
       <c r="H88" s="48" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="I88" s="45"/>
     </row>
@@ -3725,30 +3757,30 @@
         <v>85</v>
       </c>
       <c r="D89" s="19" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="E89" s="31"/>
       <c r="F89" s="36"/>
       <c r="G89" s="36"/>
       <c r="H89" s="48" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="I89" s="45"/>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D90" s="19" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="E90" s="31"/>
       <c r="F90" s="36"/>
       <c r="H90" s="48" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="I90" s="45"/>
     </row>
@@ -3757,16 +3789,16 @@
         <v>75</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="E91" s="33"/>
       <c r="F91" s="36"/>
       <c r="G91" s="36"/>
       <c r="H91" s="46" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="I91" s="45"/>
     </row>
@@ -3775,16 +3807,16 @@
         <v>76</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D92" s="19" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E92" s="31"/>
       <c r="F92" s="37"/>
       <c r="G92" s="36"/>
       <c r="H92" s="48" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I92" s="45"/>
     </row>
@@ -3793,16 +3825,16 @@
         <v>77</v>
       </c>
       <c r="C93" s="75" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="E93" s="31"/>
       <c r="F93" s="36"/>
       <c r="G93" s="36"/>
       <c r="H93" s="44" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="I93" s="45"/>
     </row>
@@ -3811,19 +3843,19 @@
         <v>78</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D94" s="21" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="E94" s="64" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F94" s="36" t="s">
         <v>88</v>
       </c>
       <c r="H94" s="47" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="I94" s="45"/>
     </row>
@@ -3835,18 +3867,18 @@
         <v>86</v>
       </c>
       <c r="D95" s="19" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E95" s="32" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F95" s="36"/>
       <c r="G95" s="36"/>
       <c r="H95" s="48" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="I95" s="45" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="96" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3857,16 +3889,16 @@
         <v>229</v>
       </c>
       <c r="D96" s="24" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="E96" s="31" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F96" s="36" t="s">
         <v>88</v>
       </c>
       <c r="H96" s="52" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="I96" s="45"/>
     </row>
@@ -3875,22 +3907,22 @@
         <v>81</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D97" s="20" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E97" s="63" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G97" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H97" s="74" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="I97" s="45" t="s">
         <v>88</v>
@@ -3901,22 +3933,22 @@
         <v>82</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E98" s="63" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G98" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H98" s="74" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="I98" s="45" t="s">
         <v>88</v>
@@ -3924,25 +3956,25 @@
     </row>
     <row r="99" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C99" s="11" t="s">
         <v>87</v>
       </c>
       <c r="D99" s="20" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E99" s="64" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="G99" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H99" s="74" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="I99" s="45" t="s">
         <v>88</v>
@@ -4019,88 +4051,88 @@
         <v>92</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E105" s="31"/>
       <c r="F105" s="36"/>
       <c r="G105" s="36"/>
       <c r="H105" s="48" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="I105" s="45"/>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D106" s="19" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E106" s="31"/>
       <c r="F106" s="36"/>
       <c r="G106" s="36"/>
       <c r="H106" s="48" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="I106" s="45"/>
     </row>
     <row r="107" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D107" s="19" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="E107" s="31"/>
       <c r="F107" s="36"/>
       <c r="G107" s="36"/>
       <c r="H107" s="48" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="I107" s="45"/>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D108" s="19" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E108" s="31"/>
       <c r="F108" s="36"/>
       <c r="G108" s="36"/>
       <c r="H108" s="48" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="I108" s="45"/>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C109" s="73" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E109" s="31"/>
       <c r="F109" s="36"/>
       <c r="G109" s="36"/>
       <c r="H109" s="48" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="I109" s="45"/>
     </row>
@@ -4112,13 +4144,13 @@
         <v>94</v>
       </c>
       <c r="D110" s="23" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E110" s="31"/>
       <c r="F110" s="36"/>
       <c r="G110" s="36"/>
       <c r="H110" s="51" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I110" s="45"/>
     </row>
@@ -4153,10 +4185,10 @@
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="31" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F113" s="37" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G113" s="36"/>
       <c r="H113" s="48" t="s">
@@ -4169,7 +4201,7 @@
         <v>97</v>
       </c>
       <c r="C114" s="70" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E114" s="31" t="s">
         <v>96</v>
@@ -4177,19 +4209,19 @@
       <c r="F114" s="37"/>
       <c r="G114" s="36"/>
       <c r="H114" s="48" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="I114" s="45"/>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C115" s="11" t="s">
         <v>99</v>
       </c>
       <c r="D115" s="19" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E115" s="31" t="s">
         <v>97</v>
@@ -4197,7 +4229,7 @@
       <c r="F115" s="37"/>
       <c r="G115" s="36"/>
       <c r="H115" s="48" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="I115" s="45"/>
     </row>
@@ -4231,17 +4263,17 @@
         <v>105</v>
       </c>
       <c r="D118" s="21" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E118" s="31" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F118" s="36" t="s">
         <v>97</v>
       </c>
       <c r="G118" s="37"/>
       <c r="H118" s="47" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="I118" s="45"/>
     </row>
@@ -4257,20 +4289,20 @@
         <v>111</v>
       </c>
       <c r="C120" s="71" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E120" s="31" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F120" s="72" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="G120" s="36"/>
       <c r="H120" s="44" t="s">
         <v>26</v>
       </c>
       <c r="I120" s="45" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="121" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4281,7 +4313,7 @@
         <v>114</v>
       </c>
       <c r="D121" s="21" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E121" s="31" t="s">
         <v>111</v>
@@ -4289,7 +4321,7 @@
       <c r="F121" s="36"/>
       <c r="G121" s="36"/>
       <c r="H121" s="47" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="I121" s="45"/>
     </row>
@@ -4316,20 +4348,20 @@
         <v>110</v>
       </c>
       <c r="C123" s="71" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E123" s="31" t="s">
         <v>112</v>
       </c>
       <c r="F123" s="72" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="G123" s="36"/>
       <c r="H123" s="44" t="s">
         <v>26</v>
       </c>
       <c r="I123" s="45" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
@@ -4369,13 +4401,13 @@
         <v>108</v>
       </c>
       <c r="D127" s="20" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E127" s="31"/>
       <c r="F127" s="36"/>
       <c r="G127" s="36"/>
       <c r="H127" s="46" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="I127" s="45"/>
     </row>
@@ -4420,13 +4452,13 @@
         <v>21</v>
       </c>
       <c r="D131" s="22" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E131" s="31"/>
       <c r="F131" s="37"/>
       <c r="G131" s="36"/>
       <c r="H131" s="44" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="I131" s="45"/>
     </row>
@@ -4435,34 +4467,34 @@
         <v>117</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D132" s="19" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E132" s="31"/>
       <c r="F132" s="37"/>
       <c r="G132" s="36"/>
       <c r="H132" s="48" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="I132" s="45"/>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D133" s="19" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E133" s="31"/>
       <c r="F133" s="37"/>
       <c r="G133" s="36"/>
       <c r="H133" s="48" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="I133" s="45"/>
     </row>
@@ -4471,16 +4503,16 @@
         <v>118</v>
       </c>
       <c r="C134" s="69" t="s">
+        <v>398</v>
+      </c>
+      <c r="D134" s="25" t="s">
         <v>397</v>
-      </c>
-      <c r="D134" s="25" t="s">
-        <v>396</v>
       </c>
       <c r="E134" s="31"/>
       <c r="F134" s="36"/>
       <c r="G134" s="36"/>
       <c r="H134" s="53" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="I134" s="45"/>
     </row>
@@ -4524,13 +4556,13 @@
         <v>220</v>
       </c>
       <c r="D138" s="22" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E138" s="31"/>
       <c r="F138" s="36"/>
       <c r="G138" s="36"/>
       <c r="H138" s="54" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="I138" s="45"/>
     </row>
@@ -4539,34 +4571,34 @@
         <v>123</v>
       </c>
       <c r="C139" s="26" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D139" s="22" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E139" s="31"/>
       <c r="F139" s="36"/>
       <c r="G139" s="36"/>
       <c r="H139" s="44" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="I139" s="45"/>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C140" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D140" s="22" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E140" s="31"/>
       <c r="F140" s="36"/>
       <c r="G140" s="36"/>
       <c r="H140" s="44" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="I140" s="45"/>
     </row>
@@ -4575,34 +4607,34 @@
         <v>124</v>
       </c>
       <c r="C141" s="13" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D141" s="28" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E141" s="31"/>
       <c r="F141" s="36"/>
       <c r="G141" s="36"/>
       <c r="H141" s="44" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I141" s="45"/>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C142" s="13" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D142" s="28" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E142" s="31"/>
       <c r="F142" s="36"/>
       <c r="G142" s="36"/>
       <c r="H142" s="44" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="I142" s="45"/>
     </row>
@@ -4611,16 +4643,16 @@
         <v>125</v>
       </c>
       <c r="C143" s="69" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D143" s="25" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E143" s="31"/>
       <c r="F143" s="36"/>
       <c r="G143" s="36"/>
       <c r="H143" s="53" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="I143" s="45"/>
     </row>
@@ -4664,17 +4696,17 @@
         <v>131</v>
       </c>
       <c r="D147" s="20" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E147" s="63" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F147" s="36" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G147" s="36"/>
       <c r="H147" s="46" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I147" s="45"/>
     </row>
@@ -4686,17 +4718,17 @@
         <v>142</v>
       </c>
       <c r="E148" s="63" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F148" s="39" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G148" s="36"/>
       <c r="H148" s="44" t="s">
+        <v>333</v>
+      </c>
+      <c r="I148" s="45" t="s">
         <v>332</v>
-      </c>
-      <c r="I148" s="45" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="149" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4707,17 +4739,17 @@
         <v>133</v>
       </c>
       <c r="D149" s="20" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E149" s="63" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F149" s="36" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G149" s="36"/>
       <c r="H149" s="46" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I149" s="45"/>
     </row>
@@ -4726,22 +4758,22 @@
         <v>132</v>
       </c>
       <c r="C150" s="28" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E150" s="66" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F150" s="58" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G150" s="38" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H150" s="44" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="I150" s="45" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="151" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4752,17 +4784,17 @@
         <v>135</v>
       </c>
       <c r="D151" s="20" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E151" s="67" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F151" s="36" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G151" s="36"/>
       <c r="H151" s="46" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I151" s="45"/>
     </row>
@@ -4771,22 +4803,22 @@
         <v>134</v>
       </c>
       <c r="C152" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="E152" s="66" t="s">
+        <v>460</v>
+      </c>
+      <c r="F152" s="58" t="s">
+        <v>309</v>
+      </c>
+      <c r="G152" s="38" t="s">
         <v>310</v>
       </c>
-      <c r="E152" s="66" t="s">
-        <v>459</v>
-      </c>
-      <c r="F152" s="58" t="s">
-        <v>308</v>
-      </c>
-      <c r="G152" s="38" t="s">
-        <v>309</v>
-      </c>
       <c r="H152" s="44" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="I152" s="45" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="153" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4797,17 +4829,17 @@
         <v>137</v>
       </c>
       <c r="D153" s="20" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E153" s="63" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F153" s="36" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="G153" s="36"/>
       <c r="H153" s="46" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I153" s="45"/>
     </row>
@@ -4819,19 +4851,19 @@
         <v>143</v>
       </c>
       <c r="E154" s="65" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="F154" s="58" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="G154" s="38" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H154" s="44" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="I154" s="45" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="155" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4842,17 +4874,17 @@
         <v>144</v>
       </c>
       <c r="D155" s="20" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E155" s="63" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F155" s="36" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G155" s="36"/>
       <c r="H155" s="46" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I155" s="45"/>
     </row>
@@ -4861,22 +4893,22 @@
         <v>138</v>
       </c>
       <c r="C156" s="22" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E156" s="65" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F156" s="58" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G156" s="39" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H156" s="47" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="I156" s="49" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="157" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4887,17 +4919,17 @@
         <v>140</v>
       </c>
       <c r="D157" s="20" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E157" s="63" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F157" s="36" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G157" s="36"/>
       <c r="H157" s="46" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I157" s="45"/>
     </row>
@@ -4909,19 +4941,19 @@
         <v>145</v>
       </c>
       <c r="E158" s="65" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F158" s="58" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G158" s="39" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H158" s="44" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I158" s="49" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="159" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4932,17 +4964,17 @@
         <v>141</v>
       </c>
       <c r="D159" s="20" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E159" s="63" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F159" s="36" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G159" s="36"/>
       <c r="H159" s="46" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I159" s="45"/>
     </row>
@@ -4954,17 +4986,17 @@
         <v>146</v>
       </c>
       <c r="D160" s="20" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E160" s="68" t="s">
         <v>140</v>
       </c>
       <c r="F160" s="36" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G160" s="36"/>
       <c r="H160" s="46" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I160" s="45"/>
     </row>
@@ -4987,25 +5019,25 @@
     </row>
     <row r="163" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B163" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="C163" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="D163" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="E163" s="63" t="s">
+        <v>425</v>
+      </c>
+      <c r="F163" s="61" t="s">
         <v>426</v>
       </c>
-      <c r="C163" s="14" t="s">
-        <v>402</v>
-      </c>
-      <c r="D163" s="20" t="s">
-        <v>439</v>
-      </c>
-      <c r="E163" s="63" t="s">
-        <v>424</v>
-      </c>
-      <c r="F163" s="61" t="s">
-        <v>425</v>
-      </c>
       <c r="G163" s="37" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H163" s="46" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I163" s="45"/>
     </row>
@@ -5076,13 +5108,13 @@
         <v>221</v>
       </c>
       <c r="C169" s="24" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E169" s="31"/>
       <c r="F169" s="36"/>
       <c r="G169" s="36"/>
       <c r="H169" s="52" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I169" s="45"/>
     </row>
@@ -5124,7 +5156,7 @@
         <v>9</v>
       </c>
       <c r="F173" s="37" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G173" s="36"/>
       <c r="H173" s="44" t="s">
@@ -5143,14 +5175,14 @@
         <v>155</v>
       </c>
       <c r="F174" s="39" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G174" s="36"/>
       <c r="H174" s="44" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="I174" s="49" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="175" spans="2:9" x14ac:dyDescent="0.25">
@@ -5220,19 +5252,19 @@
     </row>
     <row r="180" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C180" s="13" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D180" s="21" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E180" s="31"/>
       <c r="F180" s="36"/>
       <c r="G180" s="36"/>
       <c r="H180" s="47" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="I180" s="45"/>
     </row>
@@ -5390,7 +5422,7 @@
         <v>183</v>
       </c>
       <c r="E194" s="31" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F194" s="36"/>
       <c r="G194" s="36"/>
@@ -5404,47 +5436,47 @@
         <v>181</v>
       </c>
       <c r="C195" s="14" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D195" s="22" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E195" s="63" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F195" s="38" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G195" s="36"/>
       <c r="H195" s="44" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="I195" s="45" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="196" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C196" s="26" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D196" s="22" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E196" s="63" t="s">
         <v>181</v>
       </c>
       <c r="F196" s="38" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G196" s="36"/>
       <c r="H196" s="44" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="I196" s="45" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.25">
@@ -5502,13 +5534,13 @@
         <v>188</v>
       </c>
       <c r="C202" s="28" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E202" s="31"/>
       <c r="F202" s="36"/>
       <c r="G202" s="36"/>
       <c r="H202" s="44" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="I202" s="45"/>
     </row>
@@ -5549,13 +5581,13 @@
         <v>192</v>
       </c>
       <c r="C206" s="28" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E206" s="31"/>
       <c r="F206" s="36"/>
       <c r="G206" s="36"/>
       <c r="H206" s="44" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="I206" s="45"/>
     </row>
@@ -5619,7 +5651,7 @@
         <v>9</v>
       </c>
       <c r="F212" s="37" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G212" s="36"/>
       <c r="H212" s="44" t="s">
@@ -5629,26 +5661,26 @@
     </row>
     <row r="213" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C213" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D213" s="22" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E213" s="63" t="s">
         <v>197</v>
       </c>
       <c r="F213" s="39" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G213" s="36"/>
       <c r="H213" s="44" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="I213" s="49" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="214" spans="2:9" x14ac:dyDescent="0.25">
@@ -5689,33 +5721,96 @@
         <v>204</v>
       </c>
       <c r="E216" s="63" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F216" s="38" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G216" s="36"/>
       <c r="H216" s="44" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="I216" s="45" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="217" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="217" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
+        <v>481</v>
+      </c>
+      <c r="C217" s="26" t="s">
+        <v>484</v>
+      </c>
+      <c r="D217" s="22" t="s">
+        <v>485</v>
+      </c>
+      <c r="E217" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="F217" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="G217" s="36"/>
+      <c r="H217" s="44" t="s">
+        <v>486</v>
+      </c>
+      <c r="I217" s="45" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="218" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>482</v>
+      </c>
+      <c r="C218" s="76" t="s">
+        <v>488</v>
+      </c>
+      <c r="E218" s="67" t="s">
+        <v>489</v>
+      </c>
+      <c r="F218" s="77" t="s">
+        <v>245</v>
+      </c>
+      <c r="G218" s="36"/>
+      <c r="H218" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="I218" s="45" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="219" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
+        <v>483</v>
+      </c>
+      <c r="C219" s="76" t="s">
+        <v>487</v>
+      </c>
+      <c r="E219" s="13" t="s">
+        <v>481</v>
+      </c>
+      <c r="F219" t="s">
+        <v>245</v>
+      </c>
+      <c r="G219" s="36"/>
+      <c r="H219" s="44" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="220" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B220" t="s">
         <v>201</v>
       </c>
-      <c r="C217" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="E217" s="34"/>
-      <c r="F217" s="41"/>
-      <c r="G217" s="41"/>
-      <c r="H217" s="55" t="s">
-        <v>239</v>
-      </c>
-      <c r="I217" s="56"/>
+      <c r="C220" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="E220" s="34"/>
+      <c r="F220" s="41"/>
+      <c r="G220" s="41"/>
+      <c r="H220" s="55" t="s">
+        <v>240</v>
+      </c>
+      <c r="I220" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UPDATE STATIC CONST ABSTRACT FUNCTION FIX
</commit_message>
<xml_diff>
--- a/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
+++ b/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\omer\myGitHub\Front-End-Compiler-Project\Mio Language Design\Syntax Analyze Phase\FirstFollowSelectionSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AFA404-1D9C-4B7C-A4F5-2FD20040A4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592E2F74-66C1-48E5-B419-EA61B70E0C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="494">
   <si>
     <t>&lt;Start&gt;</t>
   </si>
@@ -671,19 +671,7 @@
     <t>[ ? Null</t>
   </si>
   <si>
-    <t>Abstract ?  const ? &lt;WITH_STATIC&gt;</t>
-  </si>
-  <si>
-    <t>Abstract ? const ? Static</t>
-  </si>
-  <si>
     <t>&lt;RET_TO_THROW&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;WITH_STATIC&gt; </t>
-  </si>
-  <si>
-    <t>Static? &lt;RET_TO_THROW&gt;</t>
   </si>
   <si>
     <t>&lt;RET_OBJ_C&gt;</t>
@@ -937,9 +925,6 @@
   </si>
   <si>
     <t>dt ? str ? id ? private ? protected</t>
-  </si>
-  <si>
-    <t>Static ?dt ? str ? id ? private ? protected</t>
   </si>
   <si>
     <t xml:space="preserve">[ ? private ? protected ? id ? null </t>
@@ -1559,6 +1544,26 @@
   <si>
     <t>def ?  Static ? const ? dt 
 ? id  ?str? }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;WITH_FINAL&gt; </t>
+  </si>
+  <si>
+    <t>const? &lt;RET_TO_THROW&gt;</t>
+  </si>
+  <si>
+    <t>const?dt ? str ? id ? private ? protected</t>
+  </si>
+  <si>
+    <t>Abstract ?  Static ? &lt;WITH_FINAL&gt;?
+&lt;RET_TO_THROW&gt;</t>
+  </si>
+  <si>
+    <t>Abstract ?  Static?const?dt ? str ? id ?
+ private ?protected</t>
+  </si>
+  <si>
+    <t>const?dt ? str ? id ? private ?protected</t>
   </si>
 </sst>
 </file>
@@ -2314,8 +2319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I142" sqref="I142"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,19 +2347,19 @@
         <v>205</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H1" s="42" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
@@ -2374,13 +2379,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
@@ -2388,7 +2393,7 @@
         <v>18</v>
       </c>
       <c r="I3" s="45" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2396,23 +2401,23 @@
         <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E4" s="63" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="46" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="I4" s="45" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -2423,20 +2428,20 @@
         <v>207</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="E5" s="63" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G5" s="36"/>
       <c r="H5" s="46" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -2444,23 +2449,23 @@
         <v>7</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E6" s="63" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G6" s="36"/>
       <c r="H6" s="46" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="I6" s="45" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -2500,22 +2505,22 @@
         <v>8</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="E10" s="64" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="H10" s="47" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="I10" s="45"/>
     </row>
@@ -2542,20 +2547,20 @@
         <v>9</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="47" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="I13" s="45"/>
     </row>
@@ -2564,23 +2569,23 @@
         <v>10</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E14" s="63" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="G14" s="36"/>
       <c r="H14" s="47" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="I14" s="45" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -2610,14 +2615,14 @@
         <v>11</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="31"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
       <c r="H17" s="48" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="I17" s="45"/>
     </row>
@@ -2680,30 +2685,30 @@
         <v>17</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="31"/>
       <c r="F22" s="36"/>
       <c r="G22" s="36"/>
       <c r="H22" s="48" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I22" s="45"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="31"/>
       <c r="F23" s="36"/>
       <c r="G23" s="36"/>
       <c r="H23" s="48" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I23" s="45"/>
     </row>
@@ -2734,14 +2739,14 @@
         <v>21</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="31"/>
       <c r="F26" s="36"/>
       <c r="G26" s="36"/>
       <c r="H26" s="48" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="I26" s="45"/>
     </row>
@@ -2770,10 +2775,10 @@
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="63" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F28" s="36" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G28" s="36"/>
       <c r="H28" s="48" t="s">
@@ -2790,17 +2795,17 @@
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="64" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G29" s="36"/>
       <c r="H29" s="48" t="s">
         <v>26</v>
       </c>
       <c r="I29" s="45" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -2808,30 +2813,30 @@
         <v>25</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="31"/>
       <c r="F30" s="36"/>
       <c r="G30" s="36"/>
       <c r="H30" s="48" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="I30" s="45"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="31"/>
       <c r="F31" s="36"/>
       <c r="G31" s="36"/>
       <c r="H31" s="48" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="I31" s="45"/>
     </row>
@@ -2847,7 +2852,7 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2866,17 +2871,17 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="63" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F34" s="57" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G34" s="36"/>
       <c r="H34" s="48" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="I34" s="45" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -2958,16 +2963,16 @@
         <v>32</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E41" s="31"/>
       <c r="F41" s="36"/>
       <c r="G41" s="36"/>
       <c r="H41" s="48" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="I41" s="45"/>
     </row>
@@ -2989,19 +2994,19 @@
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E43" s="31"/>
       <c r="F43" s="36"/>
       <c r="G43" s="36"/>
       <c r="H43" s="48" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="I43" s="45"/>
     </row>
@@ -3020,16 +3025,16 @@
         <v>36</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E45" s="31"/>
       <c r="F45" s="36"/>
       <c r="G45" s="36"/>
       <c r="H45" s="48" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="I45" s="45"/>
     </row>
@@ -3041,19 +3046,19 @@
         <v>210</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E46" s="63" t="s">
         <v>36</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G46" s="38" t="s">
         <v>35</v>
       </c>
       <c r="H46" s="48" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="I46" s="45" t="s">
         <v>35</v>
@@ -3097,57 +3102,57 @@
       </c>
       <c r="I49" s="45"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>215</v>
+      <c r="C50" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>492</v>
       </c>
       <c r="E50" s="31"/>
       <c r="F50" s="36"/>
       <c r="G50" s="36"/>
-      <c r="H50" s="48" t="s">
-        <v>215</v>
+      <c r="H50" s="46" t="s">
+        <v>492</v>
       </c>
       <c r="I50" s="45"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>42</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E51" s="31"/>
       <c r="F51" s="36"/>
       <c r="G51" s="36"/>
       <c r="H51" s="48" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="I51" s="45"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>217</v>
+        <v>488</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>218</v>
+        <v>489</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>301</v>
+        <v>490</v>
       </c>
       <c r="E52" s="31"/>
       <c r="F52" s="36"/>
       <c r="G52" s="36"/>
       <c r="H52" s="48" t="s">
-        <v>301</v>
+        <v>493</v>
       </c>
       <c r="I52" s="45"/>
     </row>
@@ -3156,40 +3161,40 @@
         <v>42</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E53" s="31"/>
       <c r="F53" s="36"/>
       <c r="G53" s="36"/>
       <c r="H53" s="48" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="I53" s="45"/>
     </row>
     <row r="54" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E54" s="63" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G54" s="38" t="s">
         <v>35</v>
       </c>
       <c r="H54" s="48" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="I54" s="45" t="s">
         <v>35</v>
@@ -3200,14 +3205,14 @@
         <v>43</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="31"/>
       <c r="F55" s="36"/>
       <c r="G55" s="36"/>
       <c r="H55" s="48" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="I55" s="45"/>
     </row>
@@ -3256,16 +3261,16 @@
         <v>46</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E59" s="31"/>
       <c r="F59" s="36"/>
       <c r="G59" s="36"/>
       <c r="H59" s="44" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I59" s="45"/>
     </row>
@@ -3294,15 +3299,15 @@
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="32" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F61" s="36"/>
       <c r="G61" s="36"/>
       <c r="H61" s="48" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I61" s="45" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
@@ -3319,7 +3324,7 @@
       <c r="F62" s="36"/>
       <c r="G62" s="36"/>
       <c r="H62" s="48" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="I62" s="45" t="s">
         <v>35</v>
@@ -3387,13 +3392,13 @@
         <v>59</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="E67" s="31"/>
       <c r="F67" s="36"/>
       <c r="G67" s="36"/>
       <c r="H67" s="48" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="I67" s="45"/>
     </row>
@@ -3405,11 +3410,11 @@
         <v>60</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="G68" s="36"/>
       <c r="H68" s="48" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="I68" s="45"/>
     </row>
@@ -3424,7 +3429,7 @@
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="9" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3436,7 +3441,7 @@
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -3451,22 +3456,22 @@
         <v>61</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D72" s="19" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F72" s="58" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="G72" s="39" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="H72" s="46" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="I72" s="49" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="73" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3478,13 +3483,13 @@
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="65" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F73" s="59" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="G73" s="37" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="H73" s="48" t="s">
         <v>26</v>
@@ -3496,23 +3501,23 @@
         <v>212</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D74" s="19" t="s">
         <v>213</v>
       </c>
       <c r="E74" s="63" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F74" s="18" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="G74" s="36"/>
       <c r="H74" s="46" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="I74" s="49" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
@@ -3539,13 +3544,13 @@
         <v>67</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="E76" s="31"/>
       <c r="F76" s="36"/>
       <c r="G76" s="36"/>
       <c r="H76" s="47" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I76" s="45"/>
     </row>
@@ -3573,37 +3578,37 @@
         <v>68</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E78" s="63" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F78" s="36" t="s">
         <v>38</v>
       </c>
       <c r="G78" s="36"/>
       <c r="H78" s="46" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="I78" s="45"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C79" s="73" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="D79" s="19" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="F79" s="36"/>
       <c r="G79" s="36"/>
       <c r="H79" s="44" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I79" s="45"/>
     </row>
@@ -3619,7 +3624,7 @@
     </row>
     <row r="81" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B81" s="10" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -3634,25 +3639,25 @@
         <v>69</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D82" s="23" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E82" s="63" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="G82" s="39" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H82" s="50" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="I82" s="49" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="83" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3660,51 +3665,51 @@
         <v>70</v>
       </c>
       <c r="C83" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="D83" s="23" t="s">
         <v>411</v>
       </c>
-      <c r="D83" s="23" t="s">
-        <v>416</v>
-      </c>
       <c r="E83" s="63" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G83" s="39" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H83" s="51" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="I83" s="49" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="84" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C84" s="73" t="s">
+        <v>409</v>
+      </c>
+      <c r="D84" s="19" t="s">
         <v>410</v>
       </c>
-      <c r="C84" s="73" t="s">
-        <v>414</v>
-      </c>
-      <c r="D84" s="19" t="s">
-        <v>415</v>
-      </c>
       <c r="E84" s="63" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F84" s="60" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G84" s="39" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H84" s="48" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="I84" s="49" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
@@ -3746,16 +3751,16 @@
         <v>73</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E88" s="31"/>
       <c r="F88" s="37"/>
       <c r="G88" s="36"/>
       <c r="H88" s="48" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="I88" s="45"/>
     </row>
@@ -3767,30 +3772,30 @@
         <v>85</v>
       </c>
       <c r="D89" s="19" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="E89" s="31"/>
       <c r="F89" s="36"/>
       <c r="G89" s="36"/>
       <c r="H89" s="48" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="I89" s="45"/>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D90" s="19" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="E90" s="31"/>
       <c r="F90" s="36"/>
       <c r="H90" s="48" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="I90" s="45"/>
     </row>
@@ -3799,16 +3804,16 @@
         <v>75</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E91" s="33"/>
       <c r="F91" s="36"/>
       <c r="G91" s="36"/>
       <c r="H91" s="46" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="I91" s="45"/>
     </row>
@@ -3817,16 +3822,16 @@
         <v>76</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="D92" s="19" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E92" s="31"/>
       <c r="F92" s="37"/>
       <c r="G92" s="36"/>
       <c r="H92" s="48" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="I92" s="45"/>
     </row>
@@ -3835,16 +3840,16 @@
         <v>77</v>
       </c>
       <c r="C93" s="75" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="E93" s="31"/>
       <c r="F93" s="36"/>
       <c r="G93" s="36"/>
       <c r="H93" s="44" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="I93" s="45"/>
     </row>
@@ -3853,19 +3858,19 @@
         <v>78</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="D94" s="21" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="E94" s="64" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="F94" s="36" t="s">
         <v>88</v>
       </c>
       <c r="H94" s="47" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="I94" s="45"/>
     </row>
@@ -3877,18 +3882,18 @@
         <v>86</v>
       </c>
       <c r="D95" s="19" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E95" s="32" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F95" s="36"/>
       <c r="G95" s="36"/>
       <c r="H95" s="48" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="I95" s="45" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="96" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3896,19 +3901,19 @@
         <v>80</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D96" s="24" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E96" s="31" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F96" s="36" t="s">
         <v>88</v>
       </c>
       <c r="H96" s="52" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="I96" s="45"/>
     </row>
@@ -3917,22 +3922,22 @@
         <v>81</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="D97" s="20" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="E97" s="63" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G97" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H97" s="74" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="I97" s="45" t="s">
         <v>88</v>
@@ -3943,22 +3948,22 @@
         <v>82</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="E98" s="63" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G98" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H98" s="74" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="I98" s="45" t="s">
         <v>88</v>
@@ -3966,25 +3971,25 @@
     </row>
     <row r="99" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C99" s="11" t="s">
         <v>87</v>
       </c>
       <c r="D99" s="20" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E99" s="64" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="G99" s="38" t="s">
         <v>88</v>
       </c>
       <c r="H99" s="74" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="I99" s="45" t="s">
         <v>88</v>
@@ -4061,88 +4066,88 @@
         <v>92</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="E105" s="31"/>
       <c r="F105" s="36"/>
       <c r="G105" s="36"/>
       <c r="H105" s="48" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="I105" s="45"/>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="D106" s="19" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="E106" s="31"/>
       <c r="F106" s="36"/>
       <c r="G106" s="36"/>
       <c r="H106" s="48" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="I106" s="45"/>
     </row>
     <row r="107" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D107" s="19" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="E107" s="31"/>
       <c r="F107" s="36"/>
       <c r="G107" s="36"/>
       <c r="H107" s="48" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I107" s="45"/>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="D108" s="19" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="E108" s="31"/>
       <c r="F108" s="36"/>
       <c r="G108" s="36"/>
       <c r="H108" s="48" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="I108" s="45"/>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C109" s="73" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E109" s="31"/>
       <c r="F109" s="36"/>
       <c r="G109" s="36"/>
       <c r="H109" s="48" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="I109" s="45"/>
     </row>
@@ -4154,13 +4159,13 @@
         <v>94</v>
       </c>
       <c r="D110" s="23" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E110" s="31"/>
       <c r="F110" s="36"/>
       <c r="G110" s="36"/>
       <c r="H110" s="51" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="I110" s="45"/>
     </row>
@@ -4195,10 +4200,10 @@
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="31" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F113" s="37" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G113" s="36"/>
       <c r="H113" s="48" t="s">
@@ -4211,7 +4216,7 @@
         <v>97</v>
       </c>
       <c r="C114" s="70" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E114" s="31" t="s">
         <v>96</v>
@@ -4219,19 +4224,19 @@
       <c r="F114" s="37"/>
       <c r="G114" s="36"/>
       <c r="H114" s="48" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="I114" s="45"/>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C115" s="11" t="s">
         <v>99</v>
       </c>
       <c r="D115" s="19" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="E115" s="31" t="s">
         <v>97</v>
@@ -4239,7 +4244,7 @@
       <c r="F115" s="37"/>
       <c r="G115" s="36"/>
       <c r="H115" s="48" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="I115" s="45"/>
     </row>
@@ -4273,17 +4278,17 @@
         <v>105</v>
       </c>
       <c r="D118" s="21" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E118" s="31" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="F118" s="36" t="s">
         <v>97</v>
       </c>
       <c r="G118" s="37"/>
       <c r="H118" s="47" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="I118" s="45"/>
     </row>
@@ -4299,20 +4304,20 @@
         <v>111</v>
       </c>
       <c r="C120" s="71" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="E120" s="31" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="F120" s="72" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="G120" s="36"/>
       <c r="H120" s="44" t="s">
         <v>26</v>
       </c>
       <c r="I120" s="45" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="121" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4323,7 +4328,7 @@
         <v>114</v>
       </c>
       <c r="D121" s="21" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E121" s="31" t="s">
         <v>111</v>
@@ -4331,7 +4336,7 @@
       <c r="F121" s="36"/>
       <c r="G121" s="36"/>
       <c r="H121" s="47" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="I121" s="45"/>
     </row>
@@ -4343,13 +4348,13 @@
         <v>106</v>
       </c>
       <c r="D122" s="22" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E122" s="31"/>
       <c r="F122" s="36"/>
       <c r="G122" s="36"/>
       <c r="H122" s="44" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="I122" s="45"/>
     </row>
@@ -4358,20 +4363,20 @@
         <v>110</v>
       </c>
       <c r="C123" s="71" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="E123" s="31" t="s">
         <v>112</v>
       </c>
       <c r="F123" s="72" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="G123" s="36"/>
       <c r="H123" s="44" t="s">
         <v>26</v>
       </c>
       <c r="I123" s="45" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
@@ -4411,13 +4416,13 @@
         <v>108</v>
       </c>
       <c r="D127" s="20" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E127" s="31"/>
       <c r="F127" s="36"/>
       <c r="G127" s="36"/>
       <c r="H127" s="46" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="I127" s="45"/>
     </row>
@@ -4462,13 +4467,13 @@
         <v>21</v>
       </c>
       <c r="D131" s="22" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E131" s="31"/>
       <c r="F131" s="37"/>
       <c r="G131" s="36"/>
       <c r="H131" s="44" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="I131" s="45"/>
     </row>
@@ -4477,34 +4482,34 @@
         <v>117</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D132" s="19" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="E132" s="31"/>
       <c r="F132" s="37"/>
       <c r="G132" s="36"/>
       <c r="H132" s="48" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="I132" s="45"/>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D133" s="19" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E133" s="31"/>
       <c r="F133" s="37"/>
       <c r="G133" s="36"/>
       <c r="H133" s="48" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I133" s="45"/>
     </row>
@@ -4513,16 +4518,16 @@
         <v>118</v>
       </c>
       <c r="C134" s="69" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D134" s="25" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="E134" s="31"/>
       <c r="F134" s="36"/>
       <c r="G134" s="36"/>
       <c r="H134" s="53" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I134" s="45"/>
     </row>
@@ -4563,16 +4568,16 @@
         <v>122</v>
       </c>
       <c r="C138" s="13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D138" s="22" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="E138" s="31"/>
       <c r="F138" s="36"/>
       <c r="G138" s="36"/>
       <c r="H138" s="54" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="I138" s="45"/>
     </row>
@@ -4581,34 +4586,34 @@
         <v>123</v>
       </c>
       <c r="C139" s="26" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D139" s="22" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="E139" s="31"/>
       <c r="F139" s="36"/>
       <c r="G139" s="36"/>
       <c r="H139" s="44" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="I139" s="45"/>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C140" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D140" s="22" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E140" s="31"/>
       <c r="F140" s="36"/>
       <c r="G140" s="36"/>
       <c r="H140" s="44" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="I140" s="45"/>
     </row>
@@ -4617,41 +4622,41 @@
         <v>124</v>
       </c>
       <c r="C141" s="13" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D141" s="28" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E141" s="31"/>
       <c r="F141" s="36"/>
       <c r="G141" s="36"/>
       <c r="H141" s="44" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="I141" s="45"/>
     </row>
     <row r="142" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C142" s="13" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="D142" s="28" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="E142" s="13" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="F142" s="38" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="G142" s="36"/>
       <c r="H142" s="44" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="I142" s="49" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.25">
@@ -4659,16 +4664,16 @@
         <v>125</v>
       </c>
       <c r="C143" s="69" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D143" s="25" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="E143" s="31"/>
       <c r="F143" s="36"/>
       <c r="G143" s="36"/>
       <c r="H143" s="53" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I143" s="45"/>
     </row>
@@ -4712,17 +4717,17 @@
         <v>131</v>
       </c>
       <c r="D147" s="20" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E147" s="63" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F147" s="36" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G147" s="36"/>
       <c r="H147" s="46" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I147" s="45"/>
     </row>
@@ -4734,17 +4739,17 @@
         <v>142</v>
       </c>
       <c r="E148" s="63" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="F148" s="39" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G148" s="36"/>
       <c r="H148" s="44" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="I148" s="45" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="149" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4755,17 +4760,17 @@
         <v>133</v>
       </c>
       <c r="D149" s="20" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E149" s="63" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F149" s="36" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G149" s="36"/>
       <c r="H149" s="46" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I149" s="45"/>
     </row>
@@ -4774,22 +4779,22 @@
         <v>132</v>
       </c>
       <c r="C150" s="28" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E150" s="66" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="F150" s="58" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G150" s="38" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H150" s="44" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="I150" s="45" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="151" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4800,17 +4805,17 @@
         <v>135</v>
       </c>
       <c r="D151" s="20" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E151" s="67" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F151" s="36" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G151" s="36"/>
       <c r="H151" s="46" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I151" s="45"/>
     </row>
@@ -4819,22 +4824,22 @@
         <v>134</v>
       </c>
       <c r="C152" s="22" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E152" s="66" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="F152" s="58" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G152" s="38" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="H152" s="44" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="I152" s="45" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="153" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4845,17 +4850,17 @@
         <v>137</v>
       </c>
       <c r="D153" s="20" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E153" s="63" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F153" s="36" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="G153" s="36"/>
       <c r="H153" s="46" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I153" s="45"/>
     </row>
@@ -4867,19 +4872,19 @@
         <v>143</v>
       </c>
       <c r="E154" s="65" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="F154" s="58" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G154" s="38" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="H154" s="44" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I154" s="45" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="155" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4890,17 +4895,17 @@
         <v>144</v>
       </c>
       <c r="D155" s="20" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E155" s="63" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F155" s="36" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="G155" s="36"/>
       <c r="H155" s="46" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I155" s="45"/>
     </row>
@@ -4909,22 +4914,22 @@
         <v>138</v>
       </c>
       <c r="C156" s="22" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E156" s="65" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="F156" s="58" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G156" s="39" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="H156" s="47" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="I156" s="49" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="157" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4935,17 +4940,17 @@
         <v>140</v>
       </c>
       <c r="D157" s="20" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E157" s="63" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F157" s="36" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="G157" s="36"/>
       <c r="H157" s="46" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I157" s="45"/>
     </row>
@@ -4957,19 +4962,19 @@
         <v>145</v>
       </c>
       <c r="E158" s="65" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="F158" s="58" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G158" s="39" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="H158" s="44" t="s">
+        <v>336</v>
+      </c>
+      <c r="I158" s="49" t="s">
         <v>341</v>
-      </c>
-      <c r="I158" s="49" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="159" spans="2:9" ht="60" x14ac:dyDescent="0.25">
@@ -4980,17 +4985,17 @@
         <v>141</v>
       </c>
       <c r="D159" s="20" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E159" s="63" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F159" s="36" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G159" s="36"/>
       <c r="H159" s="46" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I159" s="45"/>
     </row>
@@ -5002,17 +5007,17 @@
         <v>146</v>
       </c>
       <c r="D160" s="20" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E160" s="68" t="s">
         <v>140</v>
       </c>
       <c r="F160" s="36" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G160" s="36"/>
       <c r="H160" s="46" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I160" s="45"/>
     </row>
@@ -5035,25 +5040,25 @@
     </row>
     <row r="163" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B163" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="C163" s="14" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D163" s="20" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="E163" s="63" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F163" s="61" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G163" s="37" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H163" s="46" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I163" s="45"/>
     </row>
@@ -5096,7 +5101,7 @@
     </row>
     <row r="167" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B167" s="6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E167" s="31"/>
       <c r="F167" s="36"/>
@@ -5121,16 +5126,16 @@
     </row>
     <row r="169" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B169" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C169" s="24" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E169" s="31"/>
       <c r="F169" s="36"/>
       <c r="G169" s="36"/>
       <c r="H169" s="52" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="I169" s="45"/>
     </row>
@@ -5172,7 +5177,7 @@
         <v>9</v>
       </c>
       <c r="F173" s="37" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G173" s="36"/>
       <c r="H173" s="44" t="s">
@@ -5191,14 +5196,14 @@
         <v>155</v>
       </c>
       <c r="F174" s="39" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G174" s="36"/>
       <c r="H174" s="44" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I174" s="49" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="175" spans="2:9" x14ac:dyDescent="0.25">
@@ -5241,13 +5246,13 @@
         <v>166</v>
       </c>
       <c r="D178" s="22" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E178" s="31"/>
       <c r="F178" s="36"/>
       <c r="G178" s="36"/>
       <c r="H178" s="44" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="I178" s="45"/>
     </row>
@@ -5268,19 +5273,19 @@
     </row>
     <row r="180" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C180" s="13" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D180" s="21" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="E180" s="31"/>
       <c r="F180" s="36"/>
       <c r="G180" s="36"/>
       <c r="H180" s="47" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="I180" s="45"/>
     </row>
@@ -5341,13 +5346,13 @@
         <v>173</v>
       </c>
       <c r="D186" s="22" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E186" s="31"/>
       <c r="F186" s="36"/>
       <c r="G186" s="36"/>
       <c r="H186" s="44" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I186" s="45"/>
     </row>
@@ -5438,7 +5443,7 @@
         <v>183</v>
       </c>
       <c r="E194" s="31" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F194" s="36"/>
       <c r="G194" s="36"/>
@@ -5452,47 +5457,47 @@
         <v>181</v>
       </c>
       <c r="C195" s="14" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D195" s="22" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E195" s="63" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="F195" s="38" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G195" s="36"/>
       <c r="H195" s="44" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="I195" s="45" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="196" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C196" s="26" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D196" s="22" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E196" s="63" t="s">
         <v>181</v>
       </c>
       <c r="F196" s="38" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G196" s="36"/>
       <c r="H196" s="44" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="I196" s="45" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.25">
@@ -5550,13 +5555,13 @@
         <v>188</v>
       </c>
       <c r="C202" s="28" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E202" s="31"/>
       <c r="F202" s="36"/>
       <c r="G202" s="36"/>
       <c r="H202" s="44" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="I202" s="45"/>
     </row>
@@ -5597,13 +5602,13 @@
         <v>192</v>
       </c>
       <c r="C206" s="28" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E206" s="31"/>
       <c r="F206" s="36"/>
       <c r="G206" s="36"/>
       <c r="H206" s="44" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="I206" s="45"/>
     </row>
@@ -5667,7 +5672,7 @@
         <v>9</v>
       </c>
       <c r="F212" s="37" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G212" s="36"/>
       <c r="H212" s="44" t="s">
@@ -5677,26 +5682,26 @@
     </row>
     <row r="213" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C213" s="16" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D213" s="22" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E213" s="63" t="s">
         <v>197</v>
       </c>
       <c r="F213" s="39" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="G213" s="36"/>
       <c r="H213" s="44" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I213" s="49" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="214" spans="2:9" x14ac:dyDescent="0.25">
@@ -5737,80 +5742,80 @@
         <v>204</v>
       </c>
       <c r="E216" s="63" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="F216" s="38" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G216" s="36"/>
       <c r="H216" s="44" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="I216" s="45" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="217" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="C217" s="26" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D217" s="22" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="E217" s="67" t="s">
         <v>200</v>
       </c>
       <c r="F217" s="38" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G217" s="36"/>
       <c r="H217" s="44" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="I217" s="45" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="218" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="C218" s="76" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E218" s="67" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="F218" s="77" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G218" s="36"/>
       <c r="H218" s="44" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="I218" s="45" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="219" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="C219" s="76" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="E219" s="13" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="F219" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G219" s="36"/>
       <c r="H219" s="44" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="220" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5818,13 +5823,13 @@
         <v>201</v>
       </c>
       <c r="C220" s="22" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E220" s="34"/>
       <c r="F220" s="41"/>
       <c r="G220" s="41"/>
       <c r="H220" s="55" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I220" s="56"/>
     </row>

</xml_diff>

<commit_message>
class function fix, default body cfg,scope add
scope added in body
switch case
try catch
</commit_message>
<xml_diff>
--- a/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
+++ b/Mio Language Design/Syntax Analyze Phase/FirstFollowSelectionSet/firstFollowSelectionSet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\omer\myGitHub\Front-End-Compiler-Project\Mio Language Design\Syntax Analyze Phase\FirstFollowSelectionSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592E2F74-66C1-48E5-B419-EA61B70E0C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28298AA-3796-45A0-B353-B2E55C15F664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="498">
   <si>
     <t>&lt;Start&gt;</t>
   </si>
@@ -1564,6 +1564,18 @@
   </si>
   <si>
     <t>const?dt ? str ? id ? private ?protected</t>
+  </si>
+  <si>
+    <t>&lt;DEFAULT_BODY&gt;</t>
+  </si>
+  <si>
+    <t>{ ?if ? shift ? const ? dt ?str?id ?Parent ? Self ?  test ?  loop ? do ? stop ?ret ?cont ? raise ?;? Null</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>{ ?if ? shift ? const ? dt ?str?id ?Parent ? Self ?  test ?  loop ? do ? stop ?ret ?cont ? raise ?;</t>
   </si>
 </sst>
 </file>
@@ -2317,10 +2329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I220"/>
+  <dimension ref="B1:I221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G181" sqref="G181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5289,17 +5301,29 @@
       </c>
       <c r="I180" s="45"/>
     </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E181" s="31"/>
+    <row r="181" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B181" t="s">
+        <v>494</v>
+      </c>
+      <c r="C181" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="D181" s="21" t="s">
+        <v>495</v>
+      </c>
+      <c r="E181" s="31" t="s">
+        <v>496</v>
+      </c>
       <c r="F181" s="36"/>
       <c r="G181" s="36"/>
-      <c r="H181" s="44"/>
-      <c r="I181" s="45"/>
+      <c r="H181" s="47" t="s">
+        <v>497</v>
+      </c>
+      <c r="I181" s="49" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="182" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B182" s="6" t="s">
-        <v>167</v>
-      </c>
       <c r="E182" s="31"/>
       <c r="F182" s="36"/>
       <c r="G182" s="36"/>
@@ -5307,6 +5331,9 @@
       <c r="I182" s="45"/>
     </row>
     <row r="183" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B183" s="6" t="s">
+        <v>167</v>
+      </c>
       <c r="E183" s="31"/>
       <c r="F183" s="36"/>
       <c r="G183" s="36"/>
@@ -5314,9 +5341,6 @@
       <c r="I183" s="45"/>
     </row>
     <row r="184" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B184" s="8" t="s">
-        <v>168</v>
-      </c>
       <c r="E184" s="31"/>
       <c r="F184" s="36"/>
       <c r="G184" s="36"/>
@@ -5324,49 +5348,49 @@
       <c r="I184" s="45"/>
     </row>
     <row r="185" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B185" t="s">
-        <v>170</v>
-      </c>
-      <c r="C185" s="22" t="s">
-        <v>172</v>
+      <c r="B185" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="E185" s="31"/>
       <c r="F185" s="36"/>
       <c r="G185" s="36"/>
-      <c r="H185" s="44" t="s">
-        <v>172</v>
-      </c>
+      <c r="H185" s="44"/>
       <c r="I185" s="45"/>
     </row>
     <row r="186" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>171</v>
-      </c>
-      <c r="C186" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="D186" s="22" t="s">
-        <v>220</v>
+        <v>170</v>
+      </c>
+      <c r="C186" s="22" t="s">
+        <v>172</v>
       </c>
       <c r="E186" s="31"/>
       <c r="F186" s="36"/>
       <c r="G186" s="36"/>
       <c r="H186" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="I186" s="45"/>
+    </row>
+    <row r="187" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B187" t="s">
+        <v>171</v>
+      </c>
+      <c r="C187" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="D187" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="I186" s="45"/>
-    </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E187" s="31"/>
       <c r="F187" s="36"/>
       <c r="G187" s="36"/>
-      <c r="H187" s="44"/>
+      <c r="H187" s="44" t="s">
+        <v>220</v>
+      </c>
       <c r="I187" s="45"/>
     </row>
     <row r="188" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B188" s="8" t="s">
-        <v>169</v>
-      </c>
       <c r="E188" s="31"/>
       <c r="F188" s="36"/>
       <c r="G188" s="36"/>
@@ -5374,46 +5398,46 @@
       <c r="I188" s="45"/>
     </row>
     <row r="189" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B189" t="s">
-        <v>174</v>
-      </c>
-      <c r="C189" s="22" t="s">
-        <v>176</v>
+      <c r="B189" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="E189" s="31"/>
       <c r="F189" s="36"/>
       <c r="G189" s="36"/>
-      <c r="H189" s="44" t="s">
-        <v>176</v>
-      </c>
+      <c r="H189" s="44"/>
       <c r="I189" s="45"/>
     </row>
     <row r="190" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C190" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E190" s="31"/>
       <c r="F190" s="36"/>
       <c r="G190" s="36"/>
       <c r="H190" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="I190" s="45"/>
+    </row>
+    <row r="191" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
+        <v>175</v>
+      </c>
+      <c r="C191" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="I190" s="45"/>
-    </row>
-    <row r="191" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E191" s="31"/>
       <c r="F191" s="36"/>
       <c r="G191" s="36"/>
-      <c r="H191" s="44"/>
+      <c r="H191" s="44" t="s">
+        <v>177</v>
+      </c>
       <c r="I191" s="45"/>
     </row>
     <row r="192" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B192" s="8" t="s">
-        <v>178</v>
-      </c>
       <c r="E192" s="31"/>
       <c r="F192" s="36"/>
       <c r="G192" s="36"/>
@@ -5421,73 +5445,59 @@
       <c r="I192" s="45"/>
     </row>
     <row r="193" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
-        <v>179</v>
-      </c>
-      <c r="C193" s="22" t="s">
-        <v>182</v>
+      <c r="B193" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="E193" s="31"/>
       <c r="F193" s="36"/>
       <c r="G193" s="36"/>
-      <c r="H193" s="44" t="s">
-        <v>182</v>
-      </c>
+      <c r="H193" s="44"/>
       <c r="I193" s="45"/>
     </row>
     <row r="194" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C194" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="E194" s="31" t="s">
-        <v>269</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="E194" s="31"/>
       <c r="F194" s="36"/>
       <c r="G194" s="36"/>
       <c r="H194" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="I194" s="45"/>
+    </row>
+    <row r="195" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>180</v>
+      </c>
+      <c r="C195" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="I194" s="45"/>
-    </row>
-    <row r="195" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B195" t="s">
-        <v>181</v>
-      </c>
-      <c r="C195" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="D195" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="E195" s="63" t="s">
-        <v>358</v>
-      </c>
-      <c r="F195" s="38" t="s">
+      <c r="E195" s="31" t="s">
         <v>269</v>
       </c>
+      <c r="F195" s="36"/>
       <c r="G195" s="36"/>
       <c r="H195" s="44" t="s">
-        <v>338</v>
-      </c>
-      <c r="I195" s="45" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="196" spans="2:9" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="I195" s="45"/>
+    </row>
+    <row r="196" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>357</v>
-      </c>
-      <c r="C196" s="26" t="s">
-        <v>416</v>
+        <v>181</v>
+      </c>
+      <c r="C196" s="14" t="s">
+        <v>417</v>
       </c>
       <c r="D196" s="22" t="s">
         <v>263</v>
       </c>
       <c r="E196" s="63" t="s">
-        <v>181</v>
+        <v>358</v>
       </c>
       <c r="F196" s="38" t="s">
         <v>269</v>
@@ -5501,16 +5511,30 @@
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E197" s="31"/>
-      <c r="F197" s="36"/>
+      <c r="B197" t="s">
+        <v>357</v>
+      </c>
+      <c r="C197" s="26" t="s">
+        <v>416</v>
+      </c>
+      <c r="D197" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="E197" s="63" t="s">
+        <v>181</v>
+      </c>
+      <c r="F197" s="38" t="s">
+        <v>269</v>
+      </c>
       <c r="G197" s="36"/>
-      <c r="H197" s="44"/>
-      <c r="I197" s="45"/>
+      <c r="H197" s="44" t="s">
+        <v>338</v>
+      </c>
+      <c r="I197" s="45" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="198" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B198" s="6" t="s">
-        <v>184</v>
-      </c>
       <c r="E198" s="31"/>
       <c r="F198" s="36"/>
       <c r="G198" s="36"/>
@@ -5518,7 +5542,9 @@
       <c r="I198" s="45"/>
     </row>
     <row r="199" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B199" s="4"/>
+      <c r="B199" s="6" t="s">
+        <v>184</v>
+      </c>
       <c r="E199" s="31"/>
       <c r="F199" s="36"/>
       <c r="G199" s="36"/>
@@ -5526,9 +5552,7 @@
       <c r="I199" s="45"/>
     </row>
     <row r="200" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B200" s="8" t="s">
-        <v>185</v>
-      </c>
+      <c r="B200" s="4"/>
       <c r="E200" s="31"/>
       <c r="F200" s="36"/>
       <c r="G200" s="36"/>
@@ -5536,61 +5560,61 @@
       <c r="I200" s="45"/>
     </row>
     <row r="201" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B201" t="s">
-        <v>187</v>
-      </c>
-      <c r="C201" s="22" t="s">
-        <v>190</v>
+      <c r="B201" s="8" t="s">
+        <v>185</v>
       </c>
       <c r="E201" s="31"/>
       <c r="F201" s="36"/>
       <c r="G201" s="36"/>
-      <c r="H201" s="44" t="s">
-        <v>190</v>
-      </c>
+      <c r="H201" s="44"/>
       <c r="I201" s="45"/>
     </row>
     <row r="202" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>188</v>
-      </c>
-      <c r="C202" s="28" t="s">
-        <v>290</v>
+        <v>187</v>
+      </c>
+      <c r="C202" s="22" t="s">
+        <v>190</v>
       </c>
       <c r="E202" s="31"/>
       <c r="F202" s="36"/>
       <c r="G202" s="36"/>
       <c r="H202" s="44" t="s">
-        <v>290</v>
+        <v>190</v>
       </c>
       <c r="I202" s="45"/>
     </row>
     <row r="203" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>189</v>
-      </c>
-      <c r="C203" s="22" t="s">
-        <v>191</v>
+        <v>188</v>
+      </c>
+      <c r="C203" s="28" t="s">
+        <v>290</v>
       </c>
       <c r="E203" s="31"/>
       <c r="F203" s="36"/>
       <c r="G203" s="36"/>
       <c r="H203" s="44" t="s">
+        <v>290</v>
+      </c>
+      <c r="I203" s="45"/>
+    </row>
+    <row r="204" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
+        <v>189</v>
+      </c>
+      <c r="C204" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="I203" s="45"/>
-    </row>
-    <row r="204" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E204" s="31"/>
       <c r="F204" s="36"/>
       <c r="G204" s="36"/>
-      <c r="H204" s="44"/>
+      <c r="H204" s="44" t="s">
+        <v>191</v>
+      </c>
       <c r="I204" s="45"/>
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B205" s="8" t="s">
-        <v>186</v>
-      </c>
       <c r="E205" s="31"/>
       <c r="F205" s="36"/>
       <c r="G205" s="36"/>
@@ -5598,31 +5622,31 @@
       <c r="I205" s="45"/>
     </row>
     <row r="206" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B206" t="s">
-        <v>192</v>
-      </c>
-      <c r="C206" s="28" t="s">
-        <v>289</v>
+      <c r="B206" s="8" t="s">
+        <v>186</v>
       </c>
       <c r="E206" s="31"/>
       <c r="F206" s="36"/>
       <c r="G206" s="36"/>
-      <c r="H206" s="44" t="s">
+      <c r="H206" s="44"/>
+      <c r="I206" s="45"/>
+    </row>
+    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B207" t="s">
+        <v>192</v>
+      </c>
+      <c r="C207" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="I206" s="45"/>
-    </row>
-    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E207" s="31"/>
       <c r="F207" s="36"/>
       <c r="G207" s="36"/>
-      <c r="H207" s="44"/>
+      <c r="H207" s="44" t="s">
+        <v>289</v>
+      </c>
       <c r="I207" s="45"/>
     </row>
     <row r="208" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B208" s="6" t="s">
-        <v>193</v>
-      </c>
       <c r="E208" s="31"/>
       <c r="F208" s="36"/>
       <c r="G208" s="36"/>
@@ -5630,150 +5654,136 @@
       <c r="I208" s="45"/>
     </row>
     <row r="209" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B209" t="s">
+      <c r="B209" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E209" s="31"/>
+      <c r="F209" s="36"/>
+      <c r="G209" s="36"/>
+      <c r="H209" s="44"/>
+      <c r="I209" s="45"/>
+    </row>
+    <row r="210" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
         <v>194</v>
       </c>
-      <c r="C209" s="22" t="s">
+      <c r="C210" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="E209" s="31"/>
-      <c r="F209" s="37"/>
-      <c r="G209" s="36"/>
-      <c r="H209" s="44" t="s">
+      <c r="E210" s="31"/>
+      <c r="F210" s="37"/>
+      <c r="G210" s="36"/>
+      <c r="H210" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="I209" s="45"/>
-    </row>
-    <row r="210" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E210" s="31"/>
-      <c r="F210" s="36"/>
-      <c r="G210" s="36"/>
-      <c r="H210" s="44"/>
       <c r="I210" s="45"/>
     </row>
     <row r="211" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B211" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="E211" s="31"/>
       <c r="F211" s="36"/>
       <c r="G211" s="36"/>
       <c r="H211" s="44"/>
       <c r="I211" s="45"/>
     </row>
-    <row r="212" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B212" t="s">
+    <row r="212" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B212" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E212" s="31"/>
+      <c r="F212" s="36"/>
+      <c r="G212" s="36"/>
+      <c r="H212" s="44"/>
+      <c r="I212" s="45"/>
+    </row>
+    <row r="213" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
         <v>197</v>
       </c>
-      <c r="C212" s="22" t="s">
+      <c r="C213" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="E212" s="63" t="s">
+      <c r="E213" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="F212" s="37" t="s">
+      <c r="F213" s="37" t="s">
         <v>389</v>
-      </c>
-      <c r="G212" s="36"/>
-      <c r="H212" s="44" t="s">
-        <v>202</v>
-      </c>
-      <c r="I212" s="45"/>
-    </row>
-    <row r="213" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B213" t="s">
-        <v>237</v>
-      </c>
-      <c r="C213" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="D213" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="E213" s="63" t="s">
-        <v>197</v>
-      </c>
-      <c r="F213" s="39" t="s">
-        <v>394</v>
       </c>
       <c r="G213" s="36"/>
       <c r="H213" s="44" t="s">
-        <v>339</v>
-      </c>
-      <c r="I213" s="49" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="214" spans="2:9" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="I213" s="45"/>
+    </row>
+    <row r="214" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>198</v>
-      </c>
-      <c r="C214" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E214" s="31"/>
-      <c r="F214" s="36"/>
+        <v>237</v>
+      </c>
+      <c r="C214" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="D214" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="E214" s="63" t="s">
+        <v>197</v>
+      </c>
+      <c r="F214" s="39" t="s">
+        <v>394</v>
+      </c>
       <c r="G214" s="36"/>
       <c r="H214" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="I214" s="45"/>
+        <v>339</v>
+      </c>
+      <c r="I214" s="49" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="215" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C215" s="22" t="s">
-        <v>203</v>
+        <v>35</v>
       </c>
       <c r="E215" s="31"/>
       <c r="F215" s="36"/>
       <c r="G215" s="36"/>
       <c r="H215" s="44" t="s">
-        <v>203</v>
+        <v>35</v>
       </c>
       <c r="I215" s="45"/>
     </row>
     <row r="216" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C216" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="E216" s="63" t="s">
-        <v>240</v>
-      </c>
-      <c r="F216" s="38" t="s">
-        <v>241</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="E216" s="31"/>
+      <c r="F216" s="36"/>
       <c r="G216" s="36"/>
       <c r="H216" s="44" t="s">
-        <v>340</v>
-      </c>
-      <c r="I216" s="45" t="s">
-        <v>241</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="I216" s="45"/>
     </row>
     <row r="217" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>476</v>
-      </c>
-      <c r="C217" s="26" t="s">
-        <v>479</v>
-      </c>
-      <c r="D217" s="22" t="s">
-        <v>480</v>
-      </c>
-      <c r="E217" s="67" t="s">
         <v>200</v>
+      </c>
+      <c r="C217" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="E217" s="63" t="s">
+        <v>240</v>
       </c>
       <c r="F217" s="38" t="s">
         <v>241</v>
       </c>
       <c r="G217" s="36"/>
       <c r="H217" s="44" t="s">
-        <v>481</v>
+        <v>340</v>
       </c>
       <c r="I217" s="45" t="s">
         <v>241</v>
@@ -5781,20 +5791,23 @@
     </row>
     <row r="218" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>477</v>
-      </c>
-      <c r="C218" s="76" t="s">
-        <v>483</v>
+        <v>476</v>
+      </c>
+      <c r="C218" s="26" t="s">
+        <v>479</v>
+      </c>
+      <c r="D218" s="22" t="s">
+        <v>480</v>
       </c>
       <c r="E218" s="67" t="s">
-        <v>484</v>
-      </c>
-      <c r="F218" s="77" t="s">
+        <v>200</v>
+      </c>
+      <c r="F218" s="38" t="s">
         <v>241</v>
       </c>
       <c r="G218" s="36"/>
       <c r="H218" s="44" t="s">
-        <v>227</v>
+        <v>481</v>
       </c>
       <c r="I218" s="45" t="s">
         <v>241</v>
@@ -5802,36 +5815,57 @@
     </row>
     <row r="219" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C219" s="76" t="s">
-        <v>482</v>
-      </c>
-      <c r="E219" s="13" t="s">
-        <v>476</v>
-      </c>
-      <c r="F219" t="s">
+        <v>483</v>
+      </c>
+      <c r="E219" s="67" t="s">
+        <v>484</v>
+      </c>
+      <c r="F219" s="77" t="s">
         <v>241</v>
       </c>
       <c r="G219" s="36"/>
       <c r="H219" s="44" t="s">
+        <v>227</v>
+      </c>
+      <c r="I219" s="45" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="220" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
+        <v>478</v>
+      </c>
+      <c r="C220" s="76" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="220" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B220" t="s">
+      <c r="E220" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="F220" t="s">
+        <v>241</v>
+      </c>
+      <c r="G220" s="36"/>
+      <c r="H220" s="44" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="221" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B221" t="s">
         <v>201</v>
       </c>
-      <c r="C220" s="22" t="s">
+      <c r="C221" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="E220" s="34"/>
-      <c r="F220" s="41"/>
-      <c r="G220" s="41"/>
-      <c r="H220" s="55" t="s">
+      <c r="E221" s="34"/>
+      <c r="F221" s="41"/>
+      <c r="G221" s="41"/>
+      <c r="H221" s="55" t="s">
         <v>236</v>
       </c>
-      <c r="I220" s="56"/>
+      <c r="I221" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>